<commit_message>
Update excel after 1.1.3 and masvs 1.2 release: Making mstg version 1.1.3 and updating V1 related links
</commit_message>
<xml_diff>
--- a/Checklists/Mobile_App_Security_Checklist-English_1.1.2.xlsx
+++ b/Checklists/Mobile_App_Security_Checklist-English_1.1.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abderrahmane.LAPTOP-NBPOQCF6\Personal\R&amp;D\OWASP\MSTG\owasp-mstg\Checklists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2CF0B19-9DD4-4086-A824-A5DCF03BDF21}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386A3027-FFCA-462E-B6E6-315C07307B68}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="6" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="366">
   <si>
     <t>ID</t>
   </si>
@@ -1290,6 +1290,9 @@
     <t>Updates:
 - Adding the MSTG-IDs
 - Covering the V1 MSTG links</t>
+  </si>
+  <si>
+    <t>1.1.3</t>
   </si>
 </sst>
 </file>
@@ -2469,13 +2472,34 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2510,12 +2534,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -2533,21 +2551,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="14" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3937,48 +3940,48 @@
   <sheetData>
     <row r="1" spans="2:4" ht="8" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B2" s="150" t="s">
+      <c r="B2" s="157" t="s">
         <v>219</v>
       </c>
-      <c r="C2" s="151"/>
-      <c r="D2" s="152"/>
+      <c r="C2" s="158"/>
+      <c r="D2" s="159"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B3" s="153"/>
-      <c r="C3" s="154"/>
-      <c r="D3" s="155"/>
+      <c r="B3" s="160"/>
+      <c r="C3" s="161"/>
+      <c r="D3" s="162"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B4" s="153"/>
-      <c r="C4" s="154"/>
-      <c r="D4" s="155"/>
+      <c r="B4" s="160"/>
+      <c r="C4" s="161"/>
+      <c r="D4" s="162"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B5" s="153"/>
-      <c r="C5" s="154"/>
-      <c r="D5" s="155"/>
+      <c r="B5" s="160"/>
+      <c r="C5" s="161"/>
+      <c r="D5" s="162"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B6" s="153"/>
-      <c r="C6" s="154"/>
-      <c r="D6" s="155"/>
+      <c r="B6" s="160"/>
+      <c r="C6" s="161"/>
+      <c r="D6" s="162"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B7" s="153"/>
-      <c r="C7" s="154"/>
-      <c r="D7" s="155"/>
+      <c r="B7" s="160"/>
+      <c r="C7" s="161"/>
+      <c r="D7" s="162"/>
     </row>
     <row r="8" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="156"/>
-      <c r="C8" s="157"/>
-      <c r="D8" s="158"/>
+      <c r="B8" s="163"/>
+      <c r="C8" s="164"/>
+      <c r="D8" s="165"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B9" s="159" t="s">
+      <c r="B9" s="166" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="160"/>
-      <c r="D9" s="161"/>
+      <c r="C9" s="153"/>
+      <c r="D9" s="154"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" s="126" t="s">
@@ -3988,19 +3991,19 @@
       <c r="D10" s="128"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B11" s="167" t="s">
+      <c r="B11" s="172" t="s">
         <v>278</v>
       </c>
-      <c r="C11" s="167"/>
+      <c r="C11" s="172"/>
       <c r="D11" s="129" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B12" s="148" t="s">
+      <c r="B12" s="146" t="s">
         <v>280</v>
       </c>
-      <c r="C12" s="149"/>
+      <c r="C12" s="156"/>
       <c r="D12" s="130" t="str">
         <f>HYPERLINK(CONCATENATE(
 "https://github.com/OWASP/owasp-masvs/blob/",
@@ -4010,91 +4013,91 @@
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B13" s="162" t="s">
+      <c r="B13" s="167" t="s">
         <v>277</v>
       </c>
-      <c r="C13" s="163"/>
+      <c r="C13" s="168"/>
       <c r="D13" s="12" t="s">
-        <v>273</v>
+        <v>365</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B14" s="148" t="s">
+      <c r="B14" s="146" t="s">
         <v>221</v>
       </c>
-      <c r="C14" s="149"/>
+      <c r="C14" s="156"/>
       <c r="D14" s="124" t="str">
         <f>HYPERLINK(CONCATENATE(
 "https://github.com/OWASP/owasp-mstg/blob/",
 MSTG_VERSION,
 "/Document/"))</f>
-        <v>https://github.com/OWASP/owasp-mstg/blob/1.1.2/Document/</v>
+        <v>https://github.com/OWASP/owasp-mstg/blob/1.1.3/Document/</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="164" t="s">
+      <c r="B15" s="169" t="s">
         <v>263</v>
       </c>
-      <c r="C15" s="165"/>
-      <c r="D15" s="166"/>
+      <c r="C15" s="170"/>
+      <c r="D15" s="171"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B16" s="146" t="s">
+      <c r="B16" s="151" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="147"/>
+      <c r="C16" s="152"/>
       <c r="D16" s="12"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B17" s="148" t="s">
+      <c r="B17" s="146" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="149"/>
+      <c r="C17" s="156"/>
       <c r="D17" s="12"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B18" s="146" t="s">
+      <c r="B18" s="151" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="147"/>
+      <c r="C18" s="152"/>
       <c r="D18" s="12"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B19" s="146" t="s">
+      <c r="B19" s="151" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="147"/>
+      <c r="C19" s="152"/>
       <c r="D19" s="12"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B20" s="146" t="s">
+      <c r="B20" s="151" t="s">
         <v>135</v>
       </c>
-      <c r="C20" s="147"/>
+      <c r="C20" s="152"/>
       <c r="D20" s="12"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B21" s="146" t="s">
+      <c r="B21" s="151" t="s">
         <v>104</v>
       </c>
-      <c r="C21" s="147"/>
+      <c r="C21" s="152"/>
       <c r="D21" s="12" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="146" t="s">
+      <c r="B22" s="151" t="s">
         <v>106</v>
       </c>
-      <c r="C22" s="147"/>
+      <c r="C22" s="152"/>
       <c r="D22" s="12" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B23" s="160"/>
-      <c r="C23" s="160"/>
-      <c r="D23" s="161"/>
+      <c r="B23" s="153"/>
+      <c r="C23" s="153"/>
+      <c r="D23" s="154"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B24" s="1" t="s">
@@ -4111,37 +4114,37 @@
       <c r="D25" s="12"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B26" s="146" t="s">
+      <c r="B26" s="151" t="s">
         <v>98</v>
       </c>
-      <c r="C26" s="147"/>
+      <c r="C26" s="152"/>
       <c r="D26" s="12"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B27" s="146" t="s">
+      <c r="B27" s="151" t="s">
         <v>99</v>
       </c>
-      <c r="C27" s="147"/>
+      <c r="C27" s="152"/>
       <c r="D27" s="12"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B28" s="146" t="s">
+      <c r="B28" s="151" t="s">
         <v>100</v>
       </c>
-      <c r="C28" s="147"/>
+      <c r="C28" s="152"/>
       <c r="D28" s="12"/>
     </row>
     <row r="29" spans="2:4" ht="66" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="172" t="s">
+      <c r="B29" s="155" t="s">
         <v>257</v>
       </c>
-      <c r="C29" s="147"/>
+      <c r="C29" s="152"/>
       <c r="D29" s="12"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B30" s="160"/>
-      <c r="C30" s="160"/>
-      <c r="D30" s="161"/>
+      <c r="B30" s="153"/>
+      <c r="C30" s="153"/>
+      <c r="D30" s="154"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B31" s="1" t="s">
@@ -4158,37 +4161,37 @@
       <c r="D32" s="12"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B33" s="146" t="s">
+      <c r="B33" s="151" t="s">
         <v>89</v>
       </c>
-      <c r="C33" s="147"/>
+      <c r="C33" s="152"/>
       <c r="D33" s="12"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B34" s="146" t="s">
+      <c r="B34" s="151" t="s">
         <v>99</v>
       </c>
-      <c r="C34" s="147"/>
+      <c r="C34" s="152"/>
       <c r="D34" s="12"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B35" s="146" t="s">
+      <c r="B35" s="151" t="s">
         <v>100</v>
       </c>
-      <c r="C35" s="147"/>
+      <c r="C35" s="152"/>
       <c r="D35" s="12"/>
     </row>
     <row r="36" spans="2:4" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="172" t="s">
+      <c r="B36" s="155" t="s">
         <v>258</v>
       </c>
-      <c r="C36" s="147"/>
+      <c r="C36" s="152"/>
       <c r="D36" s="12"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B37" s="160"/>
-      <c r="C37" s="160"/>
-      <c r="D37" s="161"/>
+      <c r="B37" s="153"/>
+      <c r="C37" s="153"/>
+      <c r="D37" s="154"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B38" s="1" t="s">
@@ -4198,97 +4201,100 @@
       <c r="D38" s="3"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B39" s="168"/>
-      <c r="C39" s="169"/>
-      <c r="D39" s="170"/>
+      <c r="B39" s="148"/>
+      <c r="C39" s="149"/>
+      <c r="D39" s="150"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B40" s="148" t="s">
+      <c r="B40" s="146" t="s">
         <v>91</v>
       </c>
-      <c r="C40" s="171"/>
+      <c r="C40" s="147"/>
       <c r="D40" s="39"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B41" s="148" t="s">
+      <c r="B41" s="146" t="s">
         <v>92</v>
       </c>
-      <c r="C41" s="171"/>
+      <c r="C41" s="147"/>
       <c r="D41" s="39"/>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B42" s="148" t="s">
+      <c r="B42" s="146" t="s">
         <v>93</v>
       </c>
-      <c r="C42" s="171"/>
+      <c r="C42" s="147"/>
       <c r="D42" s="39"/>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B43" s="148" t="s">
+      <c r="B43" s="146" t="s">
         <v>94</v>
       </c>
-      <c r="C43" s="171"/>
+      <c r="C43" s="147"/>
       <c r="D43" s="40"/>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B44" s="148" t="s">
+      <c r="B44" s="146" t="s">
         <v>95</v>
       </c>
-      <c r="C44" s="171"/>
+      <c r="C44" s="147"/>
       <c r="D44" s="39"/>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B45" s="168"/>
-      <c r="C45" s="169"/>
-      <c r="D45" s="170"/>
+      <c r="B45" s="148"/>
+      <c r="C45" s="149"/>
+      <c r="D45" s="150"/>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B46" s="148" t="s">
+      <c r="B46" s="146" t="s">
         <v>91</v>
       </c>
-      <c r="C46" s="171"/>
+      <c r="C46" s="147"/>
       <c r="D46" s="39"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B47" s="148" t="s">
+      <c r="B47" s="146" t="s">
         <v>92</v>
       </c>
-      <c r="C47" s="171"/>
+      <c r="C47" s="147"/>
       <c r="D47" s="39"/>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B48" s="148" t="s">
+      <c r="B48" s="146" t="s">
         <v>93</v>
       </c>
-      <c r="C48" s="171"/>
+      <c r="C48" s="147"/>
       <c r="D48" s="39"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B49" s="148" t="s">
+      <c r="B49" s="146" t="s">
         <v>94</v>
       </c>
-      <c r="C49" s="171"/>
+      <c r="C49" s="147"/>
       <c r="D49" s="40"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B50" s="148" t="s">
+      <c r="B50" s="146" t="s">
         <v>95</v>
       </c>
-      <c r="C50" s="171"/>
+      <c r="C50" s="147"/>
       <c r="D50" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B2:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B39:D39"/>
@@ -4303,19 +4309,16 @@
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B2:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B46:C46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -4929,8 +4932,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:L85"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScale="62" zoomScaleNormal="62" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="62" zoomScaleNormal="62" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -5062,16 +5065,16 @@
       <c r="H6" s="98" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
-"0x04h-Testing-Code-Quality.md#injection-flaws"),
-"Injection Flaws")</f>
-        <v>Injection Flaws</v>
+"0x04h-Testing-Code-Quality.md#injection-flaws-mstg-arch-2-and-mstg-platform-2"),
+"Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)")</f>
+        <v>Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)</v>
       </c>
       <c r="I6" s="98" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
-"0x04h-Testing-Code-Quality.md#cross-site-scripting-flaws"),
-"Cross-Site Scripting Flaws")</f>
-        <v>Cross-Site Scripting Flaws</v>
+"0x04h-Testing-Code-Quality.md#cross-site-scripting-flaws-mstg-arch-2-and-mstg-platform-2"),
+"Cross-Site Scripting Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)")</f>
+        <v>Cross-Site Scripting Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)</v>
       </c>
       <c r="J6" s="115"/>
     </row>
@@ -5263,9 +5266,9 @@
       <c r="H13" s="98" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
-"0x05h-Testing-Platform-Interaction.md#testing-enforced-updating"),
-"Testing enforced updating")</f>
-        <v>Testing enforced updating</v>
+"0x05h-Testing-Platform-Interaction.md#testing-enforced-updating-mstg-arch-9"),
+"Testing enforced updating (MSTG-ARCH-9)")</f>
+        <v>Testing enforced updating (MSTG-ARCH-9)</v>
       </c>
       <c r="I13" s="95"/>
       <c r="J13" s="115"/>
@@ -7486,7 +7489,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B1:L85"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" zoomScale="74" zoomScaleNormal="74" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="74" zoomScaleNormal="74" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -7617,16 +7620,16 @@
       <c r="H6" s="98" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
-"0x04h-Testing-Code-Quality.md#injection-flaws"),
-"Injection Flaws")</f>
-        <v>Injection Flaws</v>
+"0x04h-Testing-Code-Quality.md#injection-flaws-mstg-arch-2-and-mstg-platform-2"),
+"Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)")</f>
+        <v>Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)</v>
       </c>
       <c r="I6" s="98" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
-"0x04h-Testing-Code-Quality.md#cross-site-scripting-flaws"),
-"Cross-Site Scripting Flaws")</f>
-        <v>Cross-Site Scripting Flaws</v>
+"0x04h-Testing-Code-Quality.md#cross-site-scripting-flaws-mstg-arch-2-and-mstg-platform-2"),
+"Cross-Site Scripting Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)")</f>
+        <v>Cross-Site Scripting Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)</v>
       </c>
       <c r="J6" s="115"/>
     </row>
@@ -7818,9 +7821,9 @@
       <c r="H13" s="98" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
-"0x06h-Testing-Platform-Interaction.md#testing-enforced-updating"),
-"Testing enforced updating")</f>
-        <v>Testing enforced updating</v>
+"0x06h-Testing-Platform-Interaction.md#testing-enforced-updating-mstg-arch-9"),
+"Testing enforced updating (MSTG-ARCH-9)")</f>
+        <v>Testing enforced updating (MSTG-ARCH-9)</v>
       </c>
       <c r="I13" s="110"/>
       <c r="J13" s="115"/>
@@ -10095,8 +10098,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -10493,7 +10496,7 @@
         <v>279</v>
       </c>
       <c r="D25" s="144">
-        <v>43683</v>
+        <v>43684</v>
       </c>
       <c r="E25" s="145" t="s">
         <v>364</v>

</xml_diff>

<commit_message>
updating the Arch-2 link based on #1406
</commit_message>
<xml_diff>
--- a/Checklists/Mobile_App_Security_Checklist-English_1.1.2.xlsx
+++ b/Checklists/Mobile_App_Security_Checklist-English_1.1.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abderrahmane.LAPTOP-NBPOQCF6\Personal\R&amp;D\OWASP\MSTG\owasp-mstg\Checklists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A1D778-61F6-4581-8E67-07F2FE4EB4A2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3788FDF-1673-4488-8C43-1D76F6C726B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="6" r:id="rId1"/>
@@ -2501,148 +2501,6 @@
     <xf numFmtId="0" fontId="18" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="21" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="20" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="22" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="9" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2716,6 +2574,148 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="21" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="20" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="22" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="63">
@@ -2783,7 +2783,14 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3" xfId="62" xr:uid="{34BD3A51-AA52-F643-9E6A-B40E3FA0D56F}"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -4051,48 +4058,48 @@
   <sheetData>
     <row r="1" spans="2:4" ht="8" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B2" s="145" t="s">
+      <c r="B2" s="180" t="s">
         <v>218</v>
       </c>
-      <c r="C2" s="146"/>
-      <c r="D2" s="147"/>
+      <c r="C2" s="181"/>
+      <c r="D2" s="182"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B3" s="148"/>
-      <c r="C3" s="149"/>
-      <c r="D3" s="150"/>
+      <c r="B3" s="183"/>
+      <c r="C3" s="184"/>
+      <c r="D3" s="185"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B4" s="148"/>
-      <c r="C4" s="149"/>
-      <c r="D4" s="150"/>
+      <c r="B4" s="183"/>
+      <c r="C4" s="184"/>
+      <c r="D4" s="185"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B5" s="148"/>
-      <c r="C5" s="149"/>
-      <c r="D5" s="150"/>
+      <c r="B5" s="183"/>
+      <c r="C5" s="184"/>
+      <c r="D5" s="185"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B6" s="148"/>
-      <c r="C6" s="149"/>
-      <c r="D6" s="150"/>
+      <c r="B6" s="183"/>
+      <c r="C6" s="184"/>
+      <c r="D6" s="185"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B7" s="148"/>
-      <c r="C7" s="149"/>
-      <c r="D7" s="150"/>
+      <c r="B7" s="183"/>
+      <c r="C7" s="184"/>
+      <c r="D7" s="185"/>
     </row>
     <row r="8" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="151"/>
-      <c r="C8" s="152"/>
-      <c r="D8" s="153"/>
+      <c r="B8" s="186"/>
+      <c r="C8" s="187"/>
+      <c r="D8" s="188"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B9" s="154" t="s">
+      <c r="B9" s="189" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="155"/>
-      <c r="D9" s="156"/>
+      <c r="C9" s="176"/>
+      <c r="D9" s="177"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" s="120" t="s">
@@ -4102,19 +4109,19 @@
       <c r="D10" s="122"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B11" s="162" t="s">
+      <c r="B11" s="195" t="s">
         <v>277</v>
       </c>
-      <c r="C11" s="162"/>
+      <c r="C11" s="195"/>
       <c r="D11" s="123" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B12" s="143" t="s">
+      <c r="B12" s="169" t="s">
         <v>279</v>
       </c>
-      <c r="C12" s="144"/>
+      <c r="C12" s="179"/>
       <c r="D12" s="124" t="str">
         <f>HYPERLINK(CONCATENATE(
 "https://github.com/OWASP/owasp-masvs/blob/",
@@ -4124,19 +4131,19 @@
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B13" s="157" t="s">
+      <c r="B13" s="190" t="s">
         <v>276</v>
       </c>
-      <c r="C13" s="158"/>
+      <c r="C13" s="191"/>
       <c r="D13" s="12" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B14" s="143" t="s">
+      <c r="B14" s="169" t="s">
         <v>220</v>
       </c>
-      <c r="C14" s="144"/>
+      <c r="C14" s="179"/>
       <c r="D14" s="119" t="str">
         <f>HYPERLINK(CONCATENATE(
 "https://github.com/OWASP/owasp-mstg/blob/",
@@ -4146,69 +4153,69 @@
       </c>
     </row>
     <row r="15" spans="2:4" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="159" t="s">
+      <c r="B15" s="192" t="s">
         <v>262</v>
       </c>
-      <c r="C15" s="160"/>
-      <c r="D15" s="161"/>
+      <c r="C15" s="193"/>
+      <c r="D15" s="194"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B16" s="141" t="s">
+      <c r="B16" s="174" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="142"/>
+      <c r="C16" s="175"/>
       <c r="D16" s="12"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B17" s="143" t="s">
+      <c r="B17" s="169" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="144"/>
+      <c r="C17" s="179"/>
       <c r="D17" s="12"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B18" s="141" t="s">
+      <c r="B18" s="174" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="142"/>
+      <c r="C18" s="175"/>
       <c r="D18" s="12"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B19" s="141" t="s">
+      <c r="B19" s="174" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="142"/>
+      <c r="C19" s="175"/>
       <c r="D19" s="12"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B20" s="141" t="s">
+      <c r="B20" s="174" t="s">
         <v>134</v>
       </c>
-      <c r="C20" s="142"/>
+      <c r="C20" s="175"/>
       <c r="D20" s="12"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B21" s="141" t="s">
+      <c r="B21" s="174" t="s">
         <v>104</v>
       </c>
-      <c r="C21" s="142"/>
+      <c r="C21" s="175"/>
       <c r="D21" s="12" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="141" t="s">
+      <c r="B22" s="174" t="s">
         <v>106</v>
       </c>
-      <c r="C22" s="142"/>
+      <c r="C22" s="175"/>
       <c r="D22" s="12" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B23" s="155"/>
-      <c r="C23" s="155"/>
-      <c r="D23" s="156"/>
+      <c r="B23" s="176"/>
+      <c r="C23" s="176"/>
+      <c r="D23" s="177"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B24" s="1" t="s">
@@ -4225,37 +4232,37 @@
       <c r="D25" s="12"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B26" s="141" t="s">
+      <c r="B26" s="174" t="s">
         <v>98</v>
       </c>
-      <c r="C26" s="142"/>
+      <c r="C26" s="175"/>
       <c r="D26" s="12"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B27" s="141" t="s">
+      <c r="B27" s="174" t="s">
         <v>99</v>
       </c>
-      <c r="C27" s="142"/>
+      <c r="C27" s="175"/>
       <c r="D27" s="12"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B28" s="141" t="s">
+      <c r="B28" s="174" t="s">
         <v>100</v>
       </c>
-      <c r="C28" s="142"/>
+      <c r="C28" s="175"/>
       <c r="D28" s="12"/>
     </row>
     <row r="29" spans="2:4" ht="66" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="167" t="s">
+      <c r="B29" s="178" t="s">
         <v>256</v>
       </c>
-      <c r="C29" s="142"/>
+      <c r="C29" s="175"/>
       <c r="D29" s="12"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B30" s="155"/>
-      <c r="C30" s="155"/>
-      <c r="D30" s="156"/>
+      <c r="B30" s="176"/>
+      <c r="C30" s="176"/>
+      <c r="D30" s="177"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B31" s="1" t="s">
@@ -4272,37 +4279,37 @@
       <c r="D32" s="12"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B33" s="141" t="s">
+      <c r="B33" s="174" t="s">
         <v>89</v>
       </c>
-      <c r="C33" s="142"/>
+      <c r="C33" s="175"/>
       <c r="D33" s="12"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B34" s="141" t="s">
+      <c r="B34" s="174" t="s">
         <v>99</v>
       </c>
-      <c r="C34" s="142"/>
+      <c r="C34" s="175"/>
       <c r="D34" s="12"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B35" s="141" t="s">
+      <c r="B35" s="174" t="s">
         <v>100</v>
       </c>
-      <c r="C35" s="142"/>
+      <c r="C35" s="175"/>
       <c r="D35" s="12"/>
     </row>
     <row r="36" spans="2:4" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="167" t="s">
+      <c r="B36" s="178" t="s">
         <v>257</v>
       </c>
-      <c r="C36" s="142"/>
+      <c r="C36" s="175"/>
       <c r="D36" s="12"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B37" s="155"/>
-      <c r="C37" s="155"/>
-      <c r="D37" s="156"/>
+      <c r="B37" s="176"/>
+      <c r="C37" s="176"/>
+      <c r="D37" s="177"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B38" s="1" t="s">
@@ -4312,97 +4319,100 @@
       <c r="D38" s="3"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B39" s="163"/>
-      <c r="C39" s="164"/>
-      <c r="D39" s="165"/>
+      <c r="B39" s="171"/>
+      <c r="C39" s="172"/>
+      <c r="D39" s="173"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B40" s="143" t="s">
+      <c r="B40" s="169" t="s">
         <v>91</v>
       </c>
-      <c r="C40" s="166"/>
+      <c r="C40" s="170"/>
       <c r="D40" s="39"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B41" s="143" t="s">
+      <c r="B41" s="169" t="s">
         <v>92</v>
       </c>
-      <c r="C41" s="166"/>
+      <c r="C41" s="170"/>
       <c r="D41" s="39"/>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B42" s="143" t="s">
+      <c r="B42" s="169" t="s">
         <v>93</v>
       </c>
-      <c r="C42" s="166"/>
+      <c r="C42" s="170"/>
       <c r="D42" s="39"/>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B43" s="143" t="s">
+      <c r="B43" s="169" t="s">
         <v>94</v>
       </c>
-      <c r="C43" s="166"/>
+      <c r="C43" s="170"/>
       <c r="D43" s="40"/>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B44" s="143" t="s">
+      <c r="B44" s="169" t="s">
         <v>95</v>
       </c>
-      <c r="C44" s="166"/>
+      <c r="C44" s="170"/>
       <c r="D44" s="39"/>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B45" s="163"/>
-      <c r="C45" s="164"/>
-      <c r="D45" s="165"/>
+      <c r="B45" s="171"/>
+      <c r="C45" s="172"/>
+      <c r="D45" s="173"/>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B46" s="143" t="s">
+      <c r="B46" s="169" t="s">
         <v>91</v>
       </c>
-      <c r="C46" s="166"/>
+      <c r="C46" s="170"/>
       <c r="D46" s="39"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B47" s="143" t="s">
+      <c r="B47" s="169" t="s">
         <v>92</v>
       </c>
-      <c r="C47" s="166"/>
+      <c r="C47" s="170"/>
       <c r="D47" s="39"/>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B48" s="143" t="s">
+      <c r="B48" s="169" t="s">
         <v>93</v>
       </c>
-      <c r="C48" s="166"/>
+      <c r="C48" s="170"/>
       <c r="D48" s="39"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B49" s="143" t="s">
+      <c r="B49" s="169" t="s">
         <v>94</v>
       </c>
-      <c r="C49" s="166"/>
+      <c r="C49" s="170"/>
       <c r="D49" s="40"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B50" s="143" t="s">
+      <c r="B50" s="169" t="s">
         <v>95</v>
       </c>
-      <c r="C50" s="166"/>
+      <c r="C50" s="170"/>
       <c r="D50" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B2:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B39:D39"/>
@@ -4417,19 +4427,16 @@
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B2:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B46:C46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -4476,11 +4483,11 @@
       <c r="F3" s="8"/>
     </row>
     <row r="4" spans="2:24" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="172"/>
-      <c r="C4" s="172"/>
-      <c r="D4" s="172"/>
-      <c r="E4" s="172"/>
-      <c r="F4" s="172"/>
+      <c r="B4" s="212"/>
+      <c r="C4" s="212"/>
+      <c r="D4" s="212"/>
+      <c r="E4" s="212"/>
+      <c r="F4" s="212"/>
     </row>
     <row r="5" spans="2:24" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="20"/>
@@ -4495,16 +4502,16 @@
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
       <c r="F6" s="21"/>
-      <c r="G6" s="182" t="s">
+      <c r="G6" s="196" t="s">
         <v>117</v>
       </c>
-      <c r="H6" s="183"/>
-      <c r="I6" s="184"/>
-      <c r="V6" s="182" t="s">
+      <c r="H6" s="197"/>
+      <c r="I6" s="198"/>
+      <c r="V6" s="196" t="s">
         <v>117</v>
       </c>
-      <c r="W6" s="183"/>
-      <c r="X6" s="184"/>
+      <c r="W6" s="197"/>
+      <c r="X6" s="198"/>
     </row>
     <row r="7" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="13"/>
@@ -4519,18 +4526,18 @@
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
-      <c r="G8" s="173">
+      <c r="G8" s="199">
         <f>AVERAGE(G43:G50)*5</f>
         <v>0</v>
       </c>
-      <c r="H8" s="174"/>
-      <c r="I8" s="175"/>
-      <c r="V8" s="173">
+      <c r="H8" s="200"/>
+      <c r="I8" s="201"/>
+      <c r="V8" s="199">
         <f>AVERAGE(K43:K50)*5</f>
         <v>0</v>
       </c>
-      <c r="W8" s="174"/>
-      <c r="X8" s="175"/>
+      <c r="W8" s="200"/>
+      <c r="X8" s="201"/>
     </row>
     <row r="9" spans="2:24" ht="91" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="21"/>
@@ -4538,12 +4545,12 @@
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
-      <c r="G9" s="176"/>
-      <c r="H9" s="177"/>
-      <c r="I9" s="178"/>
-      <c r="V9" s="176"/>
-      <c r="W9" s="177"/>
-      <c r="X9" s="178"/>
+      <c r="G9" s="202"/>
+      <c r="H9" s="203"/>
+      <c r="I9" s="204"/>
+      <c r="V9" s="202"/>
+      <c r="W9" s="203"/>
+      <c r="X9" s="204"/>
     </row>
     <row r="10" spans="2:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="13"/>
@@ -4551,12 +4558,12 @@
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="176"/>
-      <c r="H10" s="177"/>
-      <c r="I10" s="178"/>
-      <c r="V10" s="176"/>
-      <c r="W10" s="177"/>
-      <c r="X10" s="178"/>
+      <c r="G10" s="202"/>
+      <c r="H10" s="203"/>
+      <c r="I10" s="204"/>
+      <c r="V10" s="202"/>
+      <c r="W10" s="203"/>
+      <c r="X10" s="204"/>
     </row>
     <row r="11" spans="2:24" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="13"/>
@@ -4564,19 +4571,19 @@
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="179"/>
-      <c r="H11" s="180"/>
-      <c r="I11" s="181"/>
-      <c r="V11" s="179"/>
-      <c r="W11" s="180"/>
-      <c r="X11" s="181"/>
+      <c r="G11" s="205"/>
+      <c r="H11" s="206"/>
+      <c r="I11" s="207"/>
+      <c r="V11" s="205"/>
+      <c r="W11" s="206"/>
+      <c r="X11" s="207"/>
     </row>
     <row r="12" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="168"/>
-      <c r="C12" s="168"/>
-      <c r="D12" s="168"/>
-      <c r="E12" s="168"/>
-      <c r="F12" s="168"/>
+      <c r="B12" s="208"/>
+      <c r="C12" s="208"/>
+      <c r="D12" s="208"/>
+      <c r="E12" s="208"/>
+      <c r="F12" s="208"/>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B13" s="14"/>
@@ -4600,11 +4607,11 @@
       <c r="F15" s="13"/>
     </row>
     <row r="16" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="168"/>
-      <c r="C16" s="168"/>
-      <c r="D16" s="168"/>
-      <c r="E16" s="168"/>
-      <c r="F16" s="168"/>
+      <c r="B16" s="208"/>
+      <c r="C16" s="208"/>
+      <c r="D16" s="208"/>
+      <c r="E16" s="208"/>
+      <c r="F16" s="208"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="14"/>
@@ -4657,18 +4664,18 @@
     </row>
     <row r="35" spans="3:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="3:11" ht="14.5" x14ac:dyDescent="0.3">
-      <c r="D41" s="169" t="s">
+      <c r="D41" s="209" t="s">
         <v>115</v>
       </c>
-      <c r="E41" s="170"/>
-      <c r="F41" s="170"/>
-      <c r="G41" s="171"/>
-      <c r="H41" s="169" t="s">
+      <c r="E41" s="210"/>
+      <c r="F41" s="210"/>
+      <c r="G41" s="211"/>
+      <c r="H41" s="209" t="s">
         <v>116</v>
       </c>
-      <c r="I41" s="170"/>
-      <c r="J41" s="170"/>
-      <c r="K41" s="171"/>
+      <c r="I41" s="210"/>
+      <c r="J41" s="210"/>
+      <c r="K41" s="211"/>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.3">
       <c r="D42" s="17" t="s">
@@ -4994,15 +5001,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="G8:I11"/>
+    <mergeCell ref="G6:I6"/>
     <mergeCell ref="V6:X6"/>
     <mergeCell ref="V8:X11"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="D41:G41"/>
     <mergeCell ref="H41:K41"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="G8:I11"/>
-    <mergeCell ref="G6:I6"/>
   </mergeCells>
   <conditionalFormatting sqref="F14">
     <cfRule type="iconSet" priority="3">
@@ -5014,7 +5021,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14">
-    <cfRule type="expression" dxfId="12" priority="4">
+    <cfRule type="expression" dxfId="13" priority="4">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5028,7 +5035,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="12" priority="2">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5043,7 +5050,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:M85"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="62" zoomScaleNormal="62" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="62" zoomScaleNormal="62" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -5065,18 +5072,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B1" s="185" t="s">
+      <c r="B1" s="213" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="185"/>
-      <c r="D1" s="185"/>
-      <c r="E1" s="185"/>
-      <c r="F1" s="185"/>
-      <c r="G1" s="185"/>
-      <c r="H1" s="185"/>
-      <c r="I1" s="185"/>
-      <c r="J1" s="185"/>
-      <c r="K1" s="185"/>
+      <c r="C1" s="213"/>
+      <c r="D1" s="213"/>
+      <c r="E1" s="213"/>
+      <c r="F1" s="213"/>
+      <c r="G1" s="213"/>
+      <c r="H1" s="213"/>
+      <c r="I1" s="213"/>
+      <c r="J1" s="213"/>
+      <c r="K1" s="213"/>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B2" s="73"/>
@@ -5085,9 +5092,9 @@
       <c r="E2" s="74"/>
       <c r="F2" s="74"/>
       <c r="G2" s="74"/>
-      <c r="H2" s="189"/>
-      <c r="I2" s="189"/>
-      <c r="J2" s="189"/>
+      <c r="H2" s="141"/>
+      <c r="I2" s="141"/>
+      <c r="J2" s="141"/>
       <c r="K2" s="101"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.35">
@@ -5109,10 +5116,10 @@
       <c r="G3" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="H3" s="186" t="s">
+      <c r="H3" s="214" t="s">
         <v>270</v>
       </c>
-      <c r="I3" s="186"/>
+      <c r="I3" s="214"/>
       <c r="J3" s="140"/>
       <c r="K3" s="109" t="s">
         <v>108</v>
@@ -5151,24 +5158,24 @@
         <v>7</v>
       </c>
       <c r="G5" s="29"/>
-      <c r="H5" s="190" t="str">
+      <c r="H5" s="142" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#architectural-information"),
 "Architectural Information")</f>
         <v>Architectural Information</v>
       </c>
-      <c r="I5" s="190" t="str">
+      <c r="I5" s="142" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05h-Testing-Platform-Interaction.md#testing-for-insecure-configuration-of-instant-apps-mstg-arch-1-mstg-arch-7"),
 "Testing for insecure Configuration of Instant Apps (MSTG-ARCH-1, MSTG-ARCH-7)")</f>
         <v>Testing for insecure Configuration of Instant Apps (MSTG-ARCH-1, MSTG-ARCH-7)</v>
       </c>
-      <c r="J5" s="202"/>
+      <c r="J5" s="154"/>
       <c r="K5" s="111"/>
     </row>
-    <row r="6" spans="2:11" ht="31" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B6" s="70" t="s">
         <v>232</v>
       </c>
@@ -5185,24 +5192,18 @@
         <v>7</v>
       </c>
       <c r="G6" s="29"/>
-      <c r="H6" s="191" t="str">
+      <c r="H6" s="143" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04h-Testing-Code-Quality.md#injection-flaws-mstg-arch-2-and-mstg-platform-2"),
 "Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)")</f>
         <v>Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)</v>
       </c>
-      <c r="I6" s="201" t="str">
-        <f>HYPERLINK(CONCATENATE(
-BASE_URL,
-"0x04h-Testing-Code-Quality.md#cross-site-scripting-flaws-mstg-arch-2-and-mstg-platform-2"),
-"Cross-Site Scripting Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)")</f>
-        <v>Cross-Site Scripting Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)</v>
-      </c>
-      <c r="J6" s="201" t="str">
+      <c r="I6" s="153" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#verifying-that-appropriate-authentication-is-in-place-mstg-arch-2-and-mstg-auth-1"),"Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)")</f>
         <v>Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)</v>
       </c>
+      <c r="J6" s="153"/>
       <c r="K6" s="111"/>
     </row>
     <row r="7" spans="2:11" ht="29" x14ac:dyDescent="0.35">
@@ -5222,15 +5223,15 @@
         <v>7</v>
       </c>
       <c r="G7" s="29"/>
-      <c r="H7" s="190" t="str">
+      <c r="H7" s="142" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#architectural-information"),
 "Architectural Information")</f>
         <v>Architectural Information</v>
       </c>
-      <c r="I7" s="202"/>
-      <c r="J7" s="202"/>
+      <c r="I7" s="154"/>
+      <c r="J7" s="154"/>
       <c r="K7" s="111"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.35">
@@ -5250,15 +5251,15 @@
         <v>7</v>
       </c>
       <c r="G8" s="29"/>
-      <c r="H8" s="190" t="str">
+      <c r="H8" s="142" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#identifying-sensitive-data"),
 "Identifying Sensitive Data")</f>
         <v>Identifying Sensitive Data</v>
       </c>
-      <c r="I8" s="202"/>
-      <c r="J8" s="202"/>
+      <c r="I8" s="154"/>
+      <c r="J8" s="154"/>
       <c r="K8" s="111"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.35">
@@ -5278,15 +5279,15 @@
       <c r="G9" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H9" s="190" t="str">
+      <c r="H9" s="142" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#environmental-information"),
 "Environmental Information")</f>
         <v>Environmental Information</v>
       </c>
-      <c r="I9" s="202"/>
-      <c r="J9" s="202"/>
+      <c r="I9" s="154"/>
+      <c r="J9" s="154"/>
       <c r="K9" s="111"/>
     </row>
     <row r="10" spans="2:11" ht="29" x14ac:dyDescent="0.35">
@@ -5306,15 +5307,15 @@
       <c r="G10" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H10" s="190" t="str">
+      <c r="H10" s="142" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#mapping-the-application"),
 "Mapping the Application")</f>
         <v>Mapping the Application</v>
       </c>
-      <c r="I10" s="202"/>
-      <c r="J10" s="202"/>
+      <c r="I10" s="154"/>
+      <c r="J10" s="154"/>
       <c r="K10" s="111"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.35">
@@ -5334,18 +5335,18 @@
       <c r="G11" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H11" s="190" t="str">
+      <c r="H11" s="142" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#testing-for-insecure-configuration-of-instant-apps-mstg-arch-1-mstg-arch-7"),"Testing for insecure Configuration of Instant Apps (MSTG-ARCH-1, MSTG-ARCH-7)")</f>
         <v>Testing for insecure Configuration of Instant Apps (MSTG-ARCH-1, MSTG-ARCH-7)</v>
       </c>
-      <c r="I11" s="201" t="str">
+      <c r="I11" s="153" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#principles-of-testing"),
 "Principles of Testing")</f>
         <v>Principles of Testing</v>
       </c>
-      <c r="J11" s="190" t="str">
+      <c r="J11" s="142" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#penetration-testing-aka-pentesting"),
@@ -5371,15 +5372,15 @@
       <c r="G12" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H12" s="190" t="str">
+      <c r="H12" s="142" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04g-Testing-Cryptography.md#cryptographic-policy"),
 "Cryptographic policy")</f>
         <v>Cryptographic policy</v>
       </c>
-      <c r="I12" s="202"/>
-      <c r="J12" s="202"/>
+      <c r="I12" s="154"/>
+      <c r="J12" s="154"/>
       <c r="K12" s="111"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.35">
@@ -5399,15 +5400,15 @@
       <c r="G13" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H13" s="190" t="str">
+      <c r="H13" s="142" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05h-Testing-Platform-Interaction.md#testing-enforced-updating-mstg-arch-9"),
 "Testing enforced updating (MSTG-ARCH-9)")</f>
         <v>Testing enforced updating (MSTG-ARCH-9)</v>
       </c>
-      <c r="I13" s="202"/>
-      <c r="J13" s="202"/>
+      <c r="I13" s="154"/>
+      <c r="J13" s="154"/>
       <c r="K13" s="111"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.35">
@@ -5427,15 +5428,15 @@
       <c r="G14" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H14" s="190" t="str">
+      <c r="H14" s="142" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#security-testing-and-the-sdlc"),
 "Security Testing and the SDLC")</f>
         <v>Security Testing and the SDLC</v>
       </c>
-      <c r="I14" s="202"/>
-      <c r="J14" s="202"/>
+      <c r="I14" s="154"/>
+      <c r="J14" s="154"/>
       <c r="K14" s="111"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.35">
@@ -5449,9 +5450,9 @@
       <c r="E15" s="30"/>
       <c r="F15" s="36"/>
       <c r="G15" s="30"/>
-      <c r="H15" s="192"/>
-      <c r="I15" s="203"/>
-      <c r="J15" s="203"/>
+      <c r="H15" s="144"/>
+      <c r="I15" s="155"/>
+      <c r="J15" s="155"/>
       <c r="K15" s="110"/>
     </row>
     <row r="16" spans="2:11" ht="29" x14ac:dyDescent="0.35">
@@ -5471,15 +5472,15 @@
         <v>7</v>
       </c>
       <c r="G16" s="29"/>
-      <c r="H16" s="193" t="str">
+      <c r="H16" s="145" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#testing-local-storage-for-sensitive-data-mstg-storage-1-and-mstg-storage-2"),"Testing Local Storage for Sensitive Data (MSTG-STORAGE-1 and MSTG-STORAGE-2)")</f>
         <v>Testing Local Storage for Sensitive Data (MSTG-STORAGE-1 and MSTG-STORAGE-2)</v>
       </c>
-      <c r="I16" s="195" t="str">
+      <c r="I16" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05e-Testing-Cryptography.md#testing-key-management-mstg-storage-1-mstg-crypto-1-and-mstg-crypto-5"),"Testing Key Management (MSTG-STORAGE-1, MSTG-CRYPTO-1 and MSTG-CRYPTO-5)")</f>
         <v>Testing Key Management (MSTG-STORAGE-1, MSTG-CRYPTO-1 and MSTG-CRYPTO-5)</v>
       </c>
-      <c r="J16" s="202"/>
+      <c r="J16" s="154"/>
       <c r="K16" s="111"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.35">
@@ -5495,12 +5496,12 @@
       <c r="E17" s="25"/>
       <c r="F17" s="34"/>
       <c r="G17" s="29"/>
-      <c r="H17" s="194" t="str">
+      <c r="H17" s="146" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#testing-local-storage-for-sensitive-data-mstg-storage-1-and-mstg-storage-2"),"Testing Local Storage for Sensitive Data (MSTG-STORAGE-1 and MSTG-STORAGE-2)")</f>
         <v>Testing Local Storage for Sensitive Data (MSTG-STORAGE-1 and MSTG-STORAGE-2)</v>
       </c>
-      <c r="I17" s="202"/>
-      <c r="J17" s="202"/>
+      <c r="I17" s="154"/>
+      <c r="J17" s="154"/>
       <c r="K17" s="115"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.35">
@@ -5520,12 +5521,12 @@
         <v>7</v>
       </c>
       <c r="G18" s="29"/>
-      <c r="H18" s="195" t="str">
+      <c r="H18" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#testing-logs-for-sensitive-data-mstg-storage-3"),"Testing Logs for Sensitive Data (MSTG-STORAGE-3)")</f>
         <v>Testing Logs for Sensitive Data (MSTG-STORAGE-3)</v>
       </c>
-      <c r="I18" s="202"/>
-      <c r="J18" s="202"/>
+      <c r="I18" s="154"/>
+      <c r="J18" s="154"/>
       <c r="K18" s="111"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.35">
@@ -5545,12 +5546,12 @@
         <v>7</v>
       </c>
       <c r="G19" s="29"/>
-      <c r="H19" s="194" t="str">
+      <c r="H19" s="146" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#determining-whether-sensitive-data-is-sent-to-third-parties-mstg-storage-4"),"Determining Whether Sensitive Data is Sent to Third Parties (MSTG-STORAGE-4)")</f>
         <v>Determining Whether Sensitive Data is Sent to Third Parties (MSTG-STORAGE-4)</v>
       </c>
-      <c r="I19" s="202"/>
-      <c r="J19" s="202"/>
+      <c r="I19" s="154"/>
+      <c r="J19" s="154"/>
       <c r="K19" s="111"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.35">
@@ -5570,12 +5571,12 @@
         <v>7</v>
       </c>
       <c r="G20" s="29"/>
-      <c r="H20" s="194" t="str">
+      <c r="H20" s="146" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#determining-whether-the-keyboard-cache-is-disabled-for-text-input-fields-mstg-storage-5"),"Determining Whether the Keyboard Cache Is Disabled for Text Input Fields (MSTG-STORAGE-5)")</f>
         <v>Determining Whether the Keyboard Cache Is Disabled for Text Input Fields (MSTG-STORAGE-5)</v>
       </c>
-      <c r="I20" s="202"/>
-      <c r="J20" s="202"/>
+      <c r="I20" s="154"/>
+      <c r="J20" s="154"/>
       <c r="K20" s="111"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.35">
@@ -5595,12 +5596,12 @@
         <v>7</v>
       </c>
       <c r="G21" s="29"/>
-      <c r="H21" s="194" t="str">
+      <c r="H21" s="146" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#determining-whether-sensitive-stored-data-has-been-exposed-via-ipc-mechanisms-mstg-storage-6"),"Determining Whether Sensitive Stored Data Has Been Exposed via IPC Mechanisms (MSTG-STORAGE-6)")</f>
         <v>Determining Whether Sensitive Stored Data Has Been Exposed via IPC Mechanisms (MSTG-STORAGE-6)</v>
       </c>
-      <c r="I21" s="202"/>
-      <c r="J21" s="202"/>
+      <c r="I21" s="154"/>
+      <c r="J21" s="154"/>
       <c r="K21" s="111"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.35">
@@ -5620,12 +5621,12 @@
         <v>7</v>
       </c>
       <c r="G22" s="29"/>
-      <c r="H22" s="195" t="str">
+      <c r="H22" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#checking-for-sensitive-data-disclosure-through-the-user-interface-mstg-storage-7"),"Checking for Sensitive Data Disclosure Through the User Interface (MSTG-STORAGE-7)")</f>
         <v>Checking for Sensitive Data Disclosure Through the User Interface (MSTG-STORAGE-7)</v>
       </c>
-      <c r="I22" s="202"/>
-      <c r="J22" s="202"/>
+      <c r="I22" s="154"/>
+      <c r="J22" s="154"/>
       <c r="K22" s="111"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.35">
@@ -5645,12 +5646,12 @@
       <c r="G23" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H23" s="195" t="str">
+      <c r="H23" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#testing-backups-for-sensitive-data-mstg-storage-8"),"Testing Backups for Sensitive Data (MSTG-STORAGE-8)")</f>
         <v>Testing Backups for Sensitive Data (MSTG-STORAGE-8)</v>
       </c>
-      <c r="I23" s="202"/>
-      <c r="J23" s="202"/>
+      <c r="I23" s="154"/>
+      <c r="J23" s="154"/>
       <c r="K23" s="111"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.35">
@@ -5670,12 +5671,12 @@
       <c r="G24" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H24" s="195" t="str">
+      <c r="H24" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#finding-sensitive-information-in-auto-generated-screenshots-mstg-storage-9"),"Finding Sensitive Information in Auto-Generated Screenshots (MSTG-STORAGE-9)")</f>
         <v>Finding Sensitive Information in Auto-Generated Screenshots (MSTG-STORAGE-9)</v>
       </c>
-      <c r="I24" s="202"/>
-      <c r="J24" s="202"/>
+      <c r="I24" s="154"/>
+      <c r="J24" s="154"/>
       <c r="K24" s="111"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.35">
@@ -5695,12 +5696,12 @@
       <c r="G25" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H25" s="195" t="str">
+      <c r="H25" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#checking-memory-for-sensitive-data-mstg-storage-10"),"Checking Memory for Sensitive Data (MSTG-STORAGE-10)")</f>
         <v>Checking Memory for Sensitive Data (MSTG-STORAGE-10)</v>
       </c>
-      <c r="I25" s="202"/>
-      <c r="J25" s="202"/>
+      <c r="I25" s="154"/>
+      <c r="J25" s="154"/>
       <c r="K25" s="111"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.35">
@@ -5720,15 +5721,15 @@
       <c r="G26" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H26" s="195" t="str">
+      <c r="H26" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#testing-the-device-access-security-policy-mstg-storage-11"),"Testing the Device-Access-Security Policy (MSTG-STORAGE-11)")</f>
         <v>Testing the Device-Access-Security Policy (MSTG-STORAGE-11)</v>
       </c>
-      <c r="I26" s="201" t="str">
+      <c r="I26" s="153" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05f-Testing-Local-Authentication.md#testing-confirm-credentials-mstg-auth-1-and-mstg-storage-11"),"Testing Confirm Credentials (MSTG-AUTH-1 and MSTG-STORAGE-11)")</f>
         <v>Testing Confirm Credentials (MSTG-AUTH-1 and MSTG-STORAGE-11)</v>
       </c>
-      <c r="J26" s="202"/>
+      <c r="J26" s="154"/>
       <c r="K26" s="111"/>
     </row>
     <row r="27" spans="2:11" ht="29" x14ac:dyDescent="0.35">
@@ -5748,12 +5749,12 @@
       <c r="G27" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H27" s="196" t="str">
+      <c r="H27" s="148" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04i-Testing-user-interaction.md#testing-user-education-mstg-storage-12"),"Testing User Education (MSTG-STORAGE-12)")</f>
         <v>Testing User Education (MSTG-STORAGE-12)</v>
       </c>
-      <c r="I27" s="202"/>
-      <c r="J27" s="202"/>
+      <c r="I27" s="154"/>
+      <c r="J27" s="154"/>
       <c r="K27" s="111"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.35">
@@ -5767,9 +5768,9 @@
       <c r="E28" s="30"/>
       <c r="F28" s="36"/>
       <c r="G28" s="30"/>
-      <c r="H28" s="192"/>
-      <c r="I28" s="203"/>
-      <c r="J28" s="203"/>
+      <c r="H28" s="144"/>
+      <c r="I28" s="155"/>
+      <c r="J28" s="155"/>
       <c r="K28" s="110"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.35">
@@ -5789,15 +5790,15 @@
         <v>7</v>
       </c>
       <c r="G29" s="29"/>
-      <c r="H29" s="195" t="str">
+      <c r="H29" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05e-Testing-Cryptography.md#testing-key-management-mstg-storage-1-mstg-crypto-1-and-mstg-crypto-5"),"Testing Key Management (MSTG-STORAGE-1, MSTG-CRYPTO-1 and MSTG-CRYPTO-5)")</f>
         <v>Testing Key Management (MSTG-STORAGE-1, MSTG-CRYPTO-1 and MSTG-CRYPTO-5)</v>
       </c>
-      <c r="I29" s="195" t="str">
+      <c r="I29" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04g-Testing-Cryptography.md#common-configuration-issues-mstg-crypto-1-mstg-crypto-2-and-mstg-crypto-3"),"Common Configuration Issues (MSTG-CRYPTO-1, MSTG-CRYPTO-2 and MSTG-CRYPTO-3)")</f>
         <v>Common Configuration Issues (MSTG-CRYPTO-1, MSTG-CRYPTO-2 and MSTG-CRYPTO-3)</v>
       </c>
-      <c r="J29" s="202"/>
+      <c r="J29" s="154"/>
       <c r="K29" s="111"/>
     </row>
     <row r="30" spans="2:11" ht="31" x14ac:dyDescent="0.35">
@@ -5817,15 +5818,15 @@
         <v>7</v>
       </c>
       <c r="G30" s="29"/>
-      <c r="H30" s="195" t="str">
+      <c r="H30" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04g-Testing-Cryptography.md#common-configuration-issues-mstg-crypto-1-mstg-crypto-2-and-mstg-crypto-3"),"Common Configuration Issues (MSTG-CRYPTO-1, MSTG-CRYPTO-2 and MSTG-CRYPTO-3)")</f>
         <v>Common Configuration Issues (MSTG-CRYPTO-1, MSTG-CRYPTO-2 and MSTG-CRYPTO-3)</v>
       </c>
-      <c r="I30" s="194" t="str">
+      <c r="I30" s="146" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05e-Testing-Cryptography.md#testing-the-configuration-of-cryptographic-standard-algorithms-mstg-crypto-2-mstg-crypto-3-and-mstg-crypto-4"),"Testing the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2, MSTG-CRYPTO-3 and MSTG-CRYPTO-4)")</f>
         <v>Testing the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2, MSTG-CRYPTO-3 and MSTG-CRYPTO-4)</v>
       </c>
-      <c r="J30" s="202"/>
+      <c r="J30" s="154"/>
       <c r="K30" s="111"/>
     </row>
     <row r="31" spans="2:11" ht="31" x14ac:dyDescent="0.35">
@@ -5845,15 +5846,15 @@
         <v>7</v>
       </c>
       <c r="G31" s="29"/>
-      <c r="H31" s="194" t="str">
+      <c r="H31" s="146" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05e-Testing-Cryptography.md#testing-the-configuration-of-cryptographic-standard-algorithms-mstg-crypto-2-mstg-crypto-3-and-mstg-crypto-4"),"Testing the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2, MSTG-CRYPTO-3 and MSTG-CRYPTO-4)")</f>
         <v>Testing the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2, MSTG-CRYPTO-3 and MSTG-CRYPTO-4)</v>
       </c>
-      <c r="I31" s="195" t="str">
+      <c r="I31" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04g-Testing-Cryptography.md#common-configuration-issues-mstg-crypto-1-mstg-crypto-2-and-mstg-crypto-3"),"Common Configuration Issues (MSTG-CRYPTO-1, MSTG-CRYPTO-2 and MSTG-CRYPTO-3)")</f>
         <v>Common Configuration Issues (MSTG-CRYPTO-1, MSTG-CRYPTO-2 and MSTG-CRYPTO-3)</v>
       </c>
-      <c r="J31" s="202"/>
+      <c r="J31" s="154"/>
       <c r="K31" s="111"/>
     </row>
     <row r="32" spans="2:11" ht="31" x14ac:dyDescent="0.35">
@@ -5873,15 +5874,15 @@
         <v>7</v>
       </c>
       <c r="G32" s="29"/>
-      <c r="H32" s="195" t="str">
+      <c r="H32" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04g-Testing-Cryptography.md#identifying-insecure-andor-deprecated-cryptographic-algorithms-mstg-crypto-4"),"Identifying Insecure and/or Deprecated Cryptographic Algorithms (MSTG-CRYPTO-4)")</f>
         <v>Identifying Insecure and/or Deprecated Cryptographic Algorithms (MSTG-CRYPTO-4)</v>
       </c>
-      <c r="I32" s="194" t="str">
+      <c r="I32" s="146" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05e-Testing-Cryptography.md#testing-the-configuration-of-cryptographic-standard-algorithms-mstg-crypto-2-mstg-crypto-3-and-mstg-crypto-4"),"Testing the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2, MSTG-CRYPTO-3 and MSTG-CRYPTO-4)")</f>
         <v>Testing the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2, MSTG-CRYPTO-3 and MSTG-CRYPTO-4)</v>
       </c>
-      <c r="J32" s="202"/>
+      <c r="J32" s="154"/>
       <c r="K32" s="111"/>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.35">
@@ -5901,12 +5902,12 @@
         <v>7</v>
       </c>
       <c r="G33" s="29"/>
-      <c r="H33" s="195" t="str">
+      <c r="H33" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05e-Testing-Cryptography.md#testing-key-management-mstg-storage-1-mstg-crypto-1-and-mstg-crypto-5"),"Testing Key Management (MSTG-STORAGE-1, MSTG-CRYPTO-1 and MSTG-CRYPTO-5)")</f>
         <v>Testing Key Management (MSTG-STORAGE-1, MSTG-CRYPTO-1 and MSTG-CRYPTO-5)</v>
       </c>
-      <c r="I33" s="202"/>
-      <c r="J33" s="202"/>
+      <c r="I33" s="154"/>
+      <c r="J33" s="154"/>
       <c r="K33" s="111"/>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.35">
@@ -5926,12 +5927,12 @@
         <v>7</v>
       </c>
       <c r="G34" s="29"/>
-      <c r="H34" s="195" t="str">
+      <c r="H34" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05e-Testing-Cryptography.md#testing-random-number-generation-mstg-crypto-6"),"Testing Random Number Generation (MSTG-CRYPTO-6)")</f>
         <v>Testing Random Number Generation (MSTG-CRYPTO-6)</v>
       </c>
-      <c r="I34" s="202"/>
-      <c r="J34" s="202"/>
+      <c r="I34" s="154"/>
+      <c r="J34" s="154"/>
       <c r="K34" s="111"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.35">
@@ -5945,9 +5946,9 @@
       <c r="E35" s="30"/>
       <c r="F35" s="36"/>
       <c r="G35" s="30"/>
-      <c r="H35" s="192"/>
-      <c r="I35" s="203"/>
-      <c r="J35" s="203"/>
+      <c r="H35" s="144"/>
+      <c r="I35" s="155"/>
+      <c r="J35" s="155"/>
       <c r="K35" s="110"/>
     </row>
     <row r="36" spans="2:13" ht="29" x14ac:dyDescent="0.35">
@@ -5967,15 +5968,15 @@
         <v>7</v>
       </c>
       <c r="G36" s="29"/>
-      <c r="H36" s="195" t="str">
+      <c r="H36" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05f-Testing-Local-Authentication.md#testing-confirm-credentials-mstg-auth-1-and-mstg-storage-11"),"Testing Confirm Credentials (MSTG-AUTH-1 and MSTG-STORAGE-11)")</f>
         <v>Testing Confirm Credentials (MSTG-AUTH-1 and MSTG-STORAGE-11)</v>
       </c>
-      <c r="I36" s="201" t="str">
+      <c r="I36" s="153" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#verifying-that-appropriate-authentication-is-in-place-mstg-arch-2-and-mstg-auth-1"),"Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)")</f>
         <v>Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)</v>
       </c>
-      <c r="J36" s="201" t="str">
+      <c r="J36" s="153" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-oauth-20-flows-mstg-auth-1-and-mstg-auth-3"),"Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)")</f>
         <v>Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)</v>
       </c>
@@ -5998,12 +5999,12 @@
         <v>7</v>
       </c>
       <c r="G37" s="29"/>
-      <c r="H37" s="195" t="str">
+      <c r="H37" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-stateful-session-management-mstg-auth-2"),"Testing Stateful Session Management (MSTG-AUTH-2)")</f>
         <v>Testing Stateful Session Management (MSTG-AUTH-2)</v>
       </c>
-      <c r="I37" s="202"/>
-      <c r="J37" s="202"/>
+      <c r="I37" s="154"/>
+      <c r="J37" s="154"/>
       <c r="K37" s="111"/>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.35">
@@ -6023,15 +6024,15 @@
         <v>7</v>
       </c>
       <c r="G38" s="29"/>
-      <c r="H38" s="194" t="str">
+      <c r="H38" s="146" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-stateless-token-based-authentication-mstg-auth-3"),"Testing Stateless (Token-Based) Authentication (MSTG-AUTH-3)")</f>
         <v>Testing Stateless (Token-Based) Authentication (MSTG-AUTH-3)</v>
       </c>
-      <c r="I38" s="201" t="str">
+      <c r="I38" s="153" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-oauth-20-flows-mstg-auth-1-and-mstg-auth-3"),"Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)")</f>
         <v>Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)</v>
       </c>
-      <c r="J38" s="202"/>
+      <c r="J38" s="154"/>
       <c r="K38" s="111"/>
       <c r="M38" s="38"/>
     </row>
@@ -6048,12 +6049,12 @@
       <c r="E39" s="25"/>
       <c r="F39" s="34"/>
       <c r="G39" s="29"/>
-      <c r="H39" s="195" t="str">
+      <c r="H39" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-user-logout-mstg-auth-4"),"Testing User Logout (MSTG-AUTH-4)")</f>
         <v>Testing User Logout (MSTG-AUTH-4)</v>
       </c>
-      <c r="I39" s="202"/>
-      <c r="J39" s="202"/>
+      <c r="I39" s="154"/>
+      <c r="J39" s="154"/>
       <c r="K39" s="111"/>
       <c r="M39" s="38"/>
     </row>
@@ -6074,12 +6075,12 @@
         <v>7</v>
       </c>
       <c r="G40" s="29"/>
-      <c r="H40" s="195" t="str">
+      <c r="H40" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-best-practices-for-passwords-mstg-auth-5-and-mstg-auth-6"),"Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)")</f>
         <v>Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)</v>
       </c>
-      <c r="I40" s="202"/>
-      <c r="J40" s="202"/>
+      <c r="I40" s="154"/>
+      <c r="J40" s="154"/>
       <c r="K40" s="111"/>
     </row>
     <row r="41" spans="2:13" ht="29" x14ac:dyDescent="0.35">
@@ -6099,15 +6100,15 @@
         <v>7</v>
       </c>
       <c r="G41" s="29"/>
-      <c r="H41" s="195" t="str">
+      <c r="H41" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-best-practices-for-passwords-mstg-auth-5-and-mstg-auth-6"),"Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)")</f>
         <v>Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)</v>
       </c>
-      <c r="I41" s="201" t="str">
+      <c r="I41" s="153" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#dynamic-testing-mstg-auth-6"),"Dynamic Testing (MSTG-AUTH-6)")</f>
         <v>Dynamic Testing (MSTG-AUTH-6)</v>
       </c>
-      <c r="J41" s="202"/>
+      <c r="J41" s="154"/>
       <c r="K41" s="111"/>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.35">
@@ -6127,12 +6128,12 @@
         <v>7</v>
       </c>
       <c r="G42" s="29"/>
-      <c r="H42" s="195" t="str">
+      <c r="H42" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-session-timeout-mstg-auth-7"),"Testing Session Timeout (MSTG-AUTH-7)")</f>
         <v>Testing Session Timeout (MSTG-AUTH-7)</v>
       </c>
-      <c r="I42" s="204"/>
-      <c r="J42" s="204"/>
+      <c r="I42" s="156"/>
+      <c r="J42" s="156"/>
       <c r="K42" s="113"/>
     </row>
     <row r="43" spans="2:13" ht="29" x14ac:dyDescent="0.35">
@@ -6152,12 +6153,12 @@
       <c r="G43" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H43" s="195" t="str">
+      <c r="H43" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05f-Testing-Local-Authentication.md#testing-biometric-authentication-mstg-auth-8"),"Testing Biometric Authentication (MSTG-AUTH-8)")</f>
         <v>Testing Biometric Authentication (MSTG-AUTH-8)</v>
       </c>
-      <c r="I43" s="202"/>
-      <c r="J43" s="202"/>
+      <c r="I43" s="154"/>
+      <c r="J43" s="154"/>
       <c r="K43" s="111"/>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.35">
@@ -6177,12 +6178,12 @@
       <c r="G44" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H44" s="195" t="str">
+      <c r="H44" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-two-factor-authentication-and-step-up-authentication-mstg-auth-9-and-mstg-auth-10"),"Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)")</f>
         <v>Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)</v>
       </c>
-      <c r="I44" s="202"/>
-      <c r="J44" s="202"/>
+      <c r="I44" s="154"/>
+      <c r="J44" s="154"/>
       <c r="K44" s="111"/>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.35">
@@ -6202,12 +6203,12 @@
       <c r="G45" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H45" s="195" t="str">
+      <c r="H45" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-two-factor-authentication-and-step-up-authentication-mstg-auth-9-and-mstg-auth-10"),"Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)")</f>
         <v>Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)</v>
       </c>
-      <c r="I45" s="202"/>
-      <c r="J45" s="202"/>
+      <c r="I45" s="154"/>
+      <c r="J45" s="154"/>
       <c r="K45" s="111"/>
     </row>
     <row r="46" spans="2:13" ht="29" x14ac:dyDescent="0.35">
@@ -6227,12 +6228,12 @@
       <c r="G46" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H46" s="197" t="str">
+      <c r="H46" s="149" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-login-activity-and-device-blocking-mstg-auth-11"),"Testing Login Activity and Device Blocking (MSTG-AUTH-11)")</f>
         <v>Testing Login Activity and Device Blocking (MSTG-AUTH-11)</v>
       </c>
-      <c r="I46" s="202"/>
-      <c r="J46" s="202"/>
+      <c r="I46" s="154"/>
+      <c r="J46" s="154"/>
       <c r="K46" s="111"/>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.35">
@@ -6246,9 +6247,9 @@
       <c r="E47" s="30"/>
       <c r="F47" s="36"/>
       <c r="G47" s="30"/>
-      <c r="H47" s="192"/>
-      <c r="I47" s="203"/>
-      <c r="J47" s="203"/>
+      <c r="H47" s="144"/>
+      <c r="I47" s="155"/>
+      <c r="J47" s="155"/>
       <c r="K47" s="110"/>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.35">
@@ -6268,12 +6269,12 @@
         <v>7</v>
       </c>
       <c r="G48" s="29"/>
-      <c r="H48" s="195" t="str">
+      <c r="H48" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#verifying-data-encryption-on-the-network-mstg-network-1-and-mstg-network-2"),"Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)")</f>
         <v>Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)</v>
       </c>
-      <c r="I48" s="202"/>
-      <c r="J48" s="202"/>
+      <c r="I48" s="154"/>
+      <c r="J48" s="154"/>
       <c r="K48" s="111"/>
     </row>
     <row r="49" spans="2:11" ht="29" x14ac:dyDescent="0.35">
@@ -6293,12 +6294,12 @@
         <v>7</v>
       </c>
       <c r="G49" s="29"/>
-      <c r="H49" s="195" t="str">
+      <c r="H49" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#verifying-data-encryption-on-the-network-mstg-network-1-and-mstg-network-2"),"Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)")</f>
         <v>Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)</v>
       </c>
-      <c r="I49" s="202"/>
-      <c r="J49" s="202"/>
+      <c r="I49" s="154"/>
+      <c r="J49" s="154"/>
       <c r="K49" s="111"/>
     </row>
     <row r="50" spans="2:11" ht="29" x14ac:dyDescent="0.35">
@@ -6318,12 +6319,12 @@
         <v>7</v>
       </c>
       <c r="G50" s="29"/>
-      <c r="H50" s="195" t="str">
+      <c r="H50" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05g-Testing-Network-Communication.md#testing-endpoint-identify-verification-mstg-network-3"),"Testing Endpoint Identify Verification (MSTG-NETWORK-3)")</f>
         <v>Testing Endpoint Identify Verification (MSTG-NETWORK-3)</v>
       </c>
-      <c r="I50" s="201"/>
-      <c r="J50" s="201"/>
+      <c r="I50" s="153"/>
+      <c r="J50" s="153"/>
       <c r="K50" s="116"/>
     </row>
     <row r="51" spans="2:11" ht="29" x14ac:dyDescent="0.35">
@@ -6343,15 +6344,15 @@
       <c r="G51" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H51" s="195" t="str">
+      <c r="H51" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05g-Testing-Network-Communication.md#testing-custom-certificate-stores-and-certificate-pinning-mstg-network-4"),"Testing Custom Certificate Stores and Certificate Pinning (MSTG-NETWORK-4)")</f>
         <v>Testing Custom Certificate Stores and Certificate Pinning (MSTG-NETWORK-4)</v>
       </c>
-      <c r="I51" s="195" t="str">
+      <c r="I51" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05g-Testing-Network-Communication.md#testing-the-network-security-configuration-settings-mstg-network-4"),"Testing the Network Security Configuration settings (MSTG-NETWORK-4)")</f>
         <v>Testing the Network Security Configuration settings (MSTG-NETWORK-4)</v>
       </c>
-      <c r="J51" s="202"/>
+      <c r="J51" s="154"/>
       <c r="K51" s="111"/>
     </row>
     <row r="52" spans="2:11" ht="29" x14ac:dyDescent="0.35">
@@ -6371,12 +6372,12 @@
       <c r="G52" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H52" s="195" t="str">
+      <c r="H52" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#making-sure-that-critical-operations-use-secure-communication-channels-mstg-network-5"),"Making Sure that Critical Operations Use Secure Communication Channels (MSTG-NETWORK-5)")</f>
         <v>Making Sure that Critical Operations Use Secure Communication Channels (MSTG-NETWORK-5)</v>
       </c>
-      <c r="I52" s="202"/>
-      <c r="J52" s="202"/>
+      <c r="I52" s="154"/>
+      <c r="J52" s="154"/>
       <c r="K52" s="111"/>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.35">
@@ -6396,12 +6397,12 @@
       <c r="G53" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H53" s="195" t="str">
+      <c r="H53" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05g-Testing-Network-Communication.md#testing-the-security-provider-mstg-network-6"),"Testing the Security Provider (MSTG-NETWORK-6)")</f>
         <v>Testing the Security Provider (MSTG-NETWORK-6)</v>
       </c>
-      <c r="I53" s="202"/>
-      <c r="J53" s="202"/>
+      <c r="I53" s="154"/>
+      <c r="J53" s="154"/>
       <c r="K53" s="111"/>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.35">
@@ -6415,9 +6416,9 @@
       <c r="E54" s="30"/>
       <c r="F54" s="36"/>
       <c r="G54" s="30"/>
-      <c r="H54" s="192"/>
-      <c r="I54" s="203"/>
-      <c r="J54" s="203"/>
+      <c r="H54" s="144"/>
+      <c r="I54" s="155"/>
+      <c r="J54" s="155"/>
       <c r="K54" s="110"/>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.35">
@@ -6437,12 +6438,12 @@
         <v>7</v>
       </c>
       <c r="G55" s="29"/>
-      <c r="H55" s="195" t="str">
+      <c r="H55" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#testing-app-permissions-mstg-platform-1"),"Testing App Permissions (MSTG-PLATFORM-1)")</f>
         <v>Testing App Permissions (MSTG-PLATFORM-1)</v>
       </c>
-      <c r="I55" s="202"/>
-      <c r="J55" s="202"/>
+      <c r="I55" s="154"/>
+      <c r="J55" s="154"/>
       <c r="K55" s="111"/>
     </row>
     <row r="56" spans="2:11" ht="29" x14ac:dyDescent="0.35">
@@ -6462,15 +6463,15 @@
         <v>7</v>
       </c>
       <c r="G56" s="29"/>
-      <c r="H56" s="195" t="str">
+      <c r="H56" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04h-Testing-Code-Quality.md#testing-for-injection-flaws-mstg-platform-2"),"Testing for Injection Flaws (MSTG-PLATFORM-2)")</f>
         <v>Testing for Injection Flaws (MSTG-PLATFORM-2)</v>
       </c>
-      <c r="I56" s="195" t="str">
+      <c r="I56" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04h-Testing-Code-Quality.md#testing-for-fragment-injection-mstg-platform-2"),"Testing for Fragment Injection (MSTG-PLATFORM-2)")</f>
         <v>Testing for Fragment Injection (MSTG-PLATFORM-2)</v>
       </c>
-      <c r="J56" s="202"/>
+      <c r="J56" s="154"/>
       <c r="K56" s="111"/>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.35">
@@ -6490,12 +6491,12 @@
         <v>7</v>
       </c>
       <c r="G57" s="29"/>
-      <c r="H57" s="195" t="str">
+      <c r="H57" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#testing-custom-url-schemes-mstg-platform-3"),"Testing Custom URL Schemes (MSTG-PLATFORM-3)")</f>
         <v>Testing Custom URL Schemes (MSTG-PLATFORM-3)</v>
       </c>
-      <c r="I57" s="202"/>
-      <c r="J57" s="202"/>
+      <c r="I57" s="154"/>
+      <c r="J57" s="154"/>
       <c r="K57" s="111"/>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.35">
@@ -6515,12 +6516,12 @@
         <v>7</v>
       </c>
       <c r="G58" s="29"/>
-      <c r="H58" s="195" t="str">
+      <c r="H58" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#testing-for-sensitive-functionality-exposure-through-ipc-mstg-platform-4"),"Testing for Sensitive Functionality Exposure Through IPC (MSTG-PLATFORM-4)")</f>
         <v>Testing for Sensitive Functionality Exposure Through IPC (MSTG-PLATFORM-4)</v>
       </c>
-      <c r="I58" s="202"/>
-      <c r="J58" s="202"/>
+      <c r="I58" s="154"/>
+      <c r="J58" s="154"/>
       <c r="K58" s="111"/>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.35">
@@ -6540,12 +6541,12 @@
         <v>7</v>
       </c>
       <c r="G59" s="29"/>
-      <c r="H59" s="195" t="str">
+      <c r="H59" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#testing-javascript-execution-in-webviews-mstg-platform-5"),"Testing JavaScript Execution in WebViews (MSTG-PLATFORM-5)")</f>
         <v>Testing JavaScript Execution in WebViews (MSTG-PLATFORM-5)</v>
       </c>
-      <c r="I59" s="202"/>
-      <c r="J59" s="202"/>
+      <c r="I59" s="154"/>
+      <c r="J59" s="154"/>
       <c r="K59" s="111"/>
     </row>
     <row r="60" spans="2:11" ht="29" x14ac:dyDescent="0.35">
@@ -6565,12 +6566,12 @@
         <v>7</v>
       </c>
       <c r="G60" s="29"/>
-      <c r="H60" s="195" t="str">
+      <c r="H60" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#testing-webview-protocol-handlers-mstg-platform-6"),"Testing WebView Protocol Handlers (MSTG-PLATFORM-6)")</f>
         <v>Testing WebView Protocol Handlers (MSTG-PLATFORM-6)</v>
       </c>
-      <c r="I60" s="202"/>
-      <c r="J60" s="202"/>
+      <c r="I60" s="154"/>
+      <c r="J60" s="154"/>
       <c r="K60" s="111"/>
     </row>
     <row r="61" spans="2:11" ht="29" x14ac:dyDescent="0.35">
@@ -6590,12 +6591,12 @@
         <v>7</v>
       </c>
       <c r="G61" s="29"/>
-      <c r="H61" s="195" t="str">
+      <c r="H61" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#determining-whether-java-objects-are-exposed-through-webviews-mstg-platform-7"),"Determining Whether Java Objects Are Exposed Through WebViews (MSTG-PLATFORM-7)")</f>
         <v>Determining Whether Java Objects Are Exposed Through WebViews (MSTG-PLATFORM-7)</v>
       </c>
-      <c r="I61" s="202"/>
-      <c r="J61" s="202"/>
+      <c r="I61" s="154"/>
+      <c r="J61" s="154"/>
       <c r="K61" s="111"/>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.35">
@@ -6615,12 +6616,12 @@
         <v>7</v>
       </c>
       <c r="G62" s="29"/>
-      <c r="H62" s="195" t="str">
+      <c r="H62" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#testing-object-persistence-mstg-platform-8"),"Testing Object Persistence (MSTG-PLATFORM-8)")</f>
         <v>Testing Object Persistence (MSTG-PLATFORM-8)</v>
       </c>
-      <c r="I62" s="202"/>
-      <c r="J62" s="202"/>
+      <c r="I62" s="154"/>
+      <c r="J62" s="154"/>
       <c r="K62" s="111"/>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.35">
@@ -6634,9 +6635,9 @@
       <c r="E63" s="30"/>
       <c r="F63" s="36"/>
       <c r="G63" s="30"/>
-      <c r="H63" s="192"/>
-      <c r="I63" s="203"/>
-      <c r="J63" s="203"/>
+      <c r="H63" s="144"/>
+      <c r="I63" s="155"/>
+      <c r="J63" s="155"/>
       <c r="K63" s="110"/>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.35">
@@ -6656,12 +6657,12 @@
         <v>7</v>
       </c>
       <c r="G64" s="29"/>
-      <c r="H64" s="195" t="str">
+      <c r="H64" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#making-sure-that-the-app-is-properly-signed-mstg-code-1"),"Making Sure That the App is Properly Signed (MSTG-CODE-1)")</f>
         <v>Making Sure That the App is Properly Signed (MSTG-CODE-1)</v>
       </c>
-      <c r="I64" s="202"/>
-      <c r="J64" s="202"/>
+      <c r="I64" s="154"/>
+      <c r="J64" s="154"/>
       <c r="K64" s="111"/>
     </row>
     <row r="65" spans="2:12" x14ac:dyDescent="0.35">
@@ -6681,12 +6682,12 @@
         <v>7</v>
       </c>
       <c r="G65" s="29"/>
-      <c r="H65" s="195" t="str">
+      <c r="H65" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#testing-whether-the-app-is-debuggable-mstg-code-2"),"Testing Whether the App is Debuggable (MSTG-CODE-2)")</f>
         <v>Testing Whether the App is Debuggable (MSTG-CODE-2)</v>
       </c>
-      <c r="I65" s="202"/>
-      <c r="J65" s="202"/>
+      <c r="I65" s="154"/>
+      <c r="J65" s="154"/>
       <c r="K65" s="111"/>
     </row>
     <row r="66" spans="2:12" x14ac:dyDescent="0.35">
@@ -6706,12 +6707,12 @@
         <v>7</v>
       </c>
       <c r="G66" s="29"/>
-      <c r="H66" s="195" t="str">
+      <c r="H66" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#testing-for-debugging-symbols-mstg-code-3"),"Testing for Debugging Symbols (MSTG-CODE-3)")</f>
         <v>Testing for Debugging Symbols (MSTG-CODE-3)</v>
       </c>
-      <c r="I66" s="202"/>
-      <c r="J66" s="202"/>
+      <c r="I66" s="154"/>
+      <c r="J66" s="154"/>
       <c r="K66" s="111"/>
     </row>
     <row r="67" spans="2:12" x14ac:dyDescent="0.35">
@@ -6731,12 +6732,12 @@
         <v>7</v>
       </c>
       <c r="G67" s="29"/>
-      <c r="H67" s="195" t="str">
+      <c r="H67" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#testing-for-debugging-code-and-verbose-error-logging-mstg-code-4"),"Testing for Debugging Code and Verbose Error Logging (MSTG-CODE-4)")</f>
         <v>Testing for Debugging Code and Verbose Error Logging (MSTG-CODE-4)</v>
       </c>
-      <c r="I67" s="202"/>
-      <c r="J67" s="202"/>
+      <c r="I67" s="154"/>
+      <c r="J67" s="154"/>
       <c r="K67" s="111"/>
     </row>
     <row r="68" spans="2:12" ht="29" x14ac:dyDescent="0.35">
@@ -6756,12 +6757,12 @@
         <v>7</v>
       </c>
       <c r="G68" s="29"/>
-      <c r="H68" s="197" t="str">
+      <c r="H68" s="149" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#checking-for-weaknesses-in-third-party-libraries-mstg-code-5"),"Checking for Weaknesses in Third Party Libraries (MSTG-CODE-5)")</f>
         <v>Checking for Weaknesses in Third Party Libraries (MSTG-CODE-5)</v>
       </c>
-      <c r="I68" s="202"/>
-      <c r="J68" s="202"/>
+      <c r="I68" s="154"/>
+      <c r="J68" s="154"/>
       <c r="K68" s="111"/>
     </row>
     <row r="69" spans="2:12" x14ac:dyDescent="0.35">
@@ -6781,12 +6782,12 @@
         <v>7</v>
       </c>
       <c r="G69" s="29"/>
-      <c r="H69" s="195" t="str">
+      <c r="H69" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#testing-exception-handling-mstg-code-6-and-mstg-code-7"),"Testing Exception Handling (MSTG-CODE-6 and MSTG-CODE-7)")</f>
         <v>Testing Exception Handling (MSTG-CODE-6 and MSTG-CODE-7)</v>
       </c>
-      <c r="I69" s="202"/>
-      <c r="J69" s="202"/>
+      <c r="I69" s="154"/>
+      <c r="J69" s="154"/>
       <c r="K69" s="111"/>
     </row>
     <row r="70" spans="2:12" x14ac:dyDescent="0.35">
@@ -6806,12 +6807,12 @@
         <v>7</v>
       </c>
       <c r="G70" s="29"/>
-      <c r="H70" s="195" t="str">
+      <c r="H70" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#testing-exception-handling-mstg-code-6-and-mstg-code-7"),"Testing Exception Handling (MSTG-CODE-6 and MSTG-CODE-7)")</f>
         <v>Testing Exception Handling (MSTG-CODE-6 and MSTG-CODE-7)</v>
       </c>
-      <c r="I70" s="202"/>
-      <c r="J70" s="202"/>
+      <c r="I70" s="154"/>
+      <c r="J70" s="154"/>
       <c r="K70" s="111"/>
     </row>
     <row r="71" spans="2:12" x14ac:dyDescent="0.35">
@@ -6831,12 +6832,12 @@
         <v>7</v>
       </c>
       <c r="G71" s="29"/>
-      <c r="H71" s="195" t="str">
+      <c r="H71" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04h-Testing-Code-Quality.md#memory-corruption-bugs-mstg-code-8"),"Memory Corruption Bugs (MSTG-CODE-8)")</f>
         <v>Memory Corruption Bugs (MSTG-CODE-8)</v>
       </c>
-      <c r="I71" s="202"/>
-      <c r="J71" s="202"/>
+      <c r="I71" s="154"/>
+      <c r="J71" s="154"/>
       <c r="K71" s="117"/>
       <c r="L71" s="75"/>
     </row>
@@ -6857,12 +6858,12 @@
         <v>7</v>
       </c>
       <c r="G72" s="29"/>
-      <c r="H72" s="195" t="str">
+      <c r="H72" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#make-sure-that-free-security-features-are-activated-mstg-code-9"),"Make Sure That Free Security Features Are Activated (MSTG-CODE-9)")</f>
         <v>Make Sure That Free Security Features Are Activated (MSTG-CODE-9)</v>
       </c>
-      <c r="I72" s="202"/>
-      <c r="J72" s="202"/>
+      <c r="I72" s="154"/>
+      <c r="J72" s="154"/>
       <c r="K72" s="111"/>
     </row>
     <row r="73" spans="2:12" x14ac:dyDescent="0.35">
@@ -6872,9 +6873,9 @@
       <c r="E73" s="31"/>
       <c r="F73" s="31"/>
       <c r="G73" s="31"/>
-      <c r="H73" s="198"/>
-      <c r="I73" s="205"/>
-      <c r="J73" s="205"/>
+      <c r="H73" s="150"/>
+      <c r="I73" s="157"/>
+      <c r="J73" s="157"/>
       <c r="K73" s="112"/>
     </row>
     <row r="74" spans="2:12" x14ac:dyDescent="0.35">
@@ -6884,9 +6885,9 @@
       <c r="E74" s="77"/>
       <c r="F74" s="77"/>
       <c r="G74" s="77"/>
-      <c r="H74" s="199"/>
-      <c r="I74" s="199"/>
-      <c r="J74" s="199"/>
+      <c r="H74" s="151"/>
+      <c r="I74" s="151"/>
+      <c r="J74" s="151"/>
       <c r="K74" s="95"/>
     </row>
     <row r="75" spans="2:12" x14ac:dyDescent="0.35">
@@ -6896,9 +6897,9 @@
       <c r="E75" s="77"/>
       <c r="F75" s="77"/>
       <c r="G75" s="77"/>
-      <c r="H75" s="199"/>
-      <c r="I75" s="199"/>
-      <c r="J75" s="199"/>
+      <c r="H75" s="151"/>
+      <c r="I75" s="151"/>
+      <c r="J75" s="151"/>
       <c r="K75" s="95"/>
     </row>
     <row r="76" spans="2:12" x14ac:dyDescent="0.35">
@@ -6908,9 +6909,9 @@
       <c r="E76" s="77"/>
       <c r="F76" s="77"/>
       <c r="G76" s="77"/>
-      <c r="H76" s="199"/>
-      <c r="I76" s="199"/>
-      <c r="J76" s="199"/>
+      <c r="H76" s="151"/>
+      <c r="I76" s="151"/>
+      <c r="J76" s="151"/>
       <c r="K76" s="95"/>
     </row>
     <row r="77" spans="2:12" x14ac:dyDescent="0.35">
@@ -6922,9 +6923,9 @@
       <c r="E77" s="77"/>
       <c r="F77" s="77"/>
       <c r="G77" s="77"/>
-      <c r="H77" s="199"/>
-      <c r="I77" s="199"/>
-      <c r="J77" s="199"/>
+      <c r="H77" s="151"/>
+      <c r="I77" s="151"/>
+      <c r="J77" s="151"/>
       <c r="K77" s="95"/>
     </row>
     <row r="78" spans="2:12" x14ac:dyDescent="0.35">
@@ -6938,9 +6939,9 @@
       <c r="E78" s="77"/>
       <c r="F78" s="77"/>
       <c r="G78" s="77"/>
-      <c r="H78" s="199"/>
-      <c r="I78" s="199"/>
-      <c r="J78" s="199"/>
+      <c r="H78" s="151"/>
+      <c r="I78" s="151"/>
+      <c r="J78" s="151"/>
       <c r="K78" s="95"/>
     </row>
     <row r="79" spans="2:12" x14ac:dyDescent="0.35">
@@ -6954,9 +6955,9 @@
       <c r="E79" s="77"/>
       <c r="F79" s="77"/>
       <c r="G79" s="77"/>
-      <c r="H79" s="199"/>
-      <c r="I79" s="199"/>
-      <c r="J79" s="199"/>
+      <c r="H79" s="151"/>
+      <c r="I79" s="151"/>
+      <c r="J79" s="151"/>
       <c r="K79" s="95"/>
     </row>
     <row r="80" spans="2:12" x14ac:dyDescent="0.35">
@@ -6970,9 +6971,9 @@
       <c r="E80" s="77"/>
       <c r="F80" s="77"/>
       <c r="G80" s="77"/>
-      <c r="H80" s="199"/>
-      <c r="I80" s="199"/>
-      <c r="J80" s="199"/>
+      <c r="H80" s="151"/>
+      <c r="I80" s="151"/>
+      <c r="J80" s="151"/>
       <c r="K80" s="95"/>
     </row>
     <row r="81" spans="2:11" x14ac:dyDescent="0.35">
@@ -6986,9 +6987,9 @@
       <c r="E81" s="77"/>
       <c r="F81" s="77"/>
       <c r="G81" s="77"/>
-      <c r="H81" s="199"/>
-      <c r="I81" s="199"/>
-      <c r="J81" s="199"/>
+      <c r="H81" s="151"/>
+      <c r="I81" s="151"/>
+      <c r="J81" s="151"/>
       <c r="K81" s="95"/>
     </row>
     <row r="82" spans="2:11" x14ac:dyDescent="0.35">
@@ -6998,9 +6999,9 @@
       <c r="E82" s="77"/>
       <c r="F82" s="77"/>
       <c r="G82" s="77"/>
-      <c r="H82" s="199"/>
-      <c r="I82" s="200"/>
-      <c r="J82" s="200"/>
+      <c r="H82" s="151"/>
+      <c r="I82" s="152"/>
+      <c r="J82" s="152"/>
       <c r="K82" s="102"/>
     </row>
     <row r="83" spans="2:11" x14ac:dyDescent="0.35">
@@ -7010,9 +7011,9 @@
       <c r="E83" s="77"/>
       <c r="F83" s="77"/>
       <c r="G83" s="77"/>
-      <c r="H83" s="199"/>
-      <c r="I83" s="200"/>
-      <c r="J83" s="200"/>
+      <c r="H83" s="151"/>
+      <c r="I83" s="152"/>
+      <c r="J83" s="152"/>
       <c r="K83" s="102"/>
     </row>
     <row r="84" spans="2:11" x14ac:dyDescent="0.35">
@@ -7022,9 +7023,9 @@
       <c r="E84" s="77"/>
       <c r="F84" s="77"/>
       <c r="G84" s="77"/>
-      <c r="H84" s="199"/>
-      <c r="I84" s="200"/>
-      <c r="J84" s="200"/>
+      <c r="H84" s="151"/>
+      <c r="I84" s="152"/>
+      <c r="J84" s="152"/>
       <c r="K84" s="102"/>
     </row>
     <row r="85" spans="2:11" x14ac:dyDescent="0.35">
@@ -7034,9 +7035,9 @@
       <c r="E85" s="79"/>
       <c r="F85" s="79"/>
       <c r="G85" s="79"/>
-      <c r="H85" s="200"/>
-      <c r="I85" s="200"/>
-      <c r="J85" s="200"/>
+      <c r="H85" s="152"/>
+      <c r="I85" s="152"/>
+      <c r="J85" s="152"/>
       <c r="K85" s="102"/>
     </row>
   </sheetData>
@@ -7087,7 +7088,7 @@
       <c r="D1" s="102"/>
       <c r="E1" s="79"/>
       <c r="F1" s="79"/>
-      <c r="G1" s="200"/>
+      <c r="G1" s="152"/>
       <c r="H1" s="102"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.35">
@@ -7096,7 +7097,7 @@
       <c r="D2" s="102"/>
       <c r="E2" s="79"/>
       <c r="F2" s="79"/>
-      <c r="G2" s="200"/>
+      <c r="G2" s="152"/>
       <c r="H2" s="102"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.35">
@@ -7115,7 +7116,7 @@
       <c r="F3" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="G3" s="206" t="s">
+      <c r="G3" s="158" t="s">
         <v>365</v>
       </c>
       <c r="H3" s="109" t="s">
@@ -7130,7 +7131,7 @@
       </c>
       <c r="E4" s="30"/>
       <c r="F4" s="30"/>
-      <c r="G4" s="207"/>
+      <c r="G4" s="159"/>
       <c r="H4" s="110"/>
     </row>
     <row r="5" spans="2:8" ht="29" x14ac:dyDescent="0.35">
@@ -7149,7 +7150,7 @@
       <c r="F5" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="208" t="str">
+      <c r="G5" s="160" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-root-detection-mstg-resilience-1"),"Testing Root Detection (MSTG-RESILIENCE-1)")</f>
         <v>Testing Root Detection (MSTG-RESILIENCE-1)</v>
       </c>
@@ -7171,7 +7172,7 @@
       <c r="F6" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G6" s="209" t="str">
+      <c r="G6" s="161" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-anti-debugging-detection-mstg-resilience-2"),"Testing Anti-Debugging Detection (MSTG-RESILIENCE-2)")</f>
         <v>Testing Anti-Debugging Detection (MSTG-RESILIENCE-2)</v>
       </c>
@@ -7193,7 +7194,7 @@
       <c r="F7" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G7" s="208" t="str">
+      <c r="G7" s="160" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-file-integrity-checks-mstg-resilience-3"),"Testing File Integrity Checks (MSTG-RESILIENCE-3)")</f>
         <v>Testing File Integrity Checks (MSTG-RESILIENCE-3)</v>
       </c>
@@ -7215,7 +7216,7 @@
       <c r="F8" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="195" t="str">
+      <c r="G8" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-reverse-engineering-tools-detection-mstg-resilience-4"),"Testing Reverse Engineering Tools Detection (MSTG-RESILIENCE-4)")</f>
         <v>Testing Reverse Engineering Tools Detection (MSTG-RESILIENCE-4)</v>
       </c>
@@ -7237,7 +7238,7 @@
       <c r="F9" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G9" s="208" t="str">
+      <c r="G9" s="160" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-emulator-detection-mstg-resilience-5"),"Testing Emulator Detection (MSTG-RESILIENCE-5)")</f>
         <v>Testing Emulator Detection (MSTG-RESILIENCE-5)</v>
       </c>
@@ -7259,7 +7260,7 @@
       <c r="F10" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G10" s="195" t="str">
+      <c r="G10" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-run-time-integrity-checks-mstg-resilience-6"),"Testing Run Time Integrity Checks (MSTG-RESILIENCE-6)")</f>
         <v>Testing Run Time Integrity Checks (MSTG-RESILIENCE-6)</v>
       </c>
@@ -7281,7 +7282,7 @@
       <c r="F11" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G11" s="210" t="s">
+      <c r="G11" s="162" t="s">
         <v>366</v>
       </c>
       <c r="H11" s="111"/>
@@ -7302,7 +7303,7 @@
       <c r="F12" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G12" s="211" t="s">
+      <c r="G12" s="163" t="s">
         <v>128</v>
       </c>
       <c r="H12" s="111"/>
@@ -7323,7 +7324,7 @@
       <c r="F13" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G13" s="195" t="str">
+      <c r="G13" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-obfuscation-mstg-resilience-9"),"Testing Obfuscation (MSTG-RESILIENCE-9)")</f>
         <v>Testing Obfuscation (MSTG-RESILIENCE-9)</v>
       </c>
@@ -7337,7 +7338,7 @@
       </c>
       <c r="E14" s="30"/>
       <c r="F14" s="30"/>
-      <c r="G14" s="207"/>
+      <c r="G14" s="159"/>
       <c r="H14" s="110"/>
     </row>
     <row r="15" spans="2:8" ht="29" x14ac:dyDescent="0.35">
@@ -7356,7 +7357,7 @@
       <c r="F15" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G15" s="195" t="str">
+      <c r="G15" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-device-binding-mstg-resilience-10"),"Testing Device Binding (MSTG-RESILIENCE-10)")</f>
         <v>Testing Device Binding (MSTG-RESILIENCE-10)</v>
       </c>
@@ -7370,7 +7371,7 @@
       </c>
       <c r="E16" s="30"/>
       <c r="F16" s="30"/>
-      <c r="G16" s="207"/>
+      <c r="G16" s="159"/>
       <c r="H16" s="110"/>
     </row>
     <row r="17" spans="2:8" ht="29" x14ac:dyDescent="0.35">
@@ -7389,7 +7390,7 @@
       <c r="F17" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G17" s="195" t="str">
+      <c r="G17" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-obfuscation-mstg-resilience-9"),"Testing Obfuscation (MSTG-RESILIENCE-9)")</f>
         <v>Testing Obfuscation (MSTG-RESILIENCE-9)</v>
       </c>
@@ -7411,7 +7412,7 @@
       <c r="F18" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G18" s="211" t="s">
+      <c r="G18" s="163" t="s">
         <v>366</v>
       </c>
       <c r="H18" s="111"/>
@@ -7422,7 +7423,7 @@
       <c r="D19" s="97"/>
       <c r="E19" s="31"/>
       <c r="F19" s="31"/>
-      <c r="G19" s="212"/>
+      <c r="G19" s="164"/>
       <c r="H19" s="112"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.35">
@@ -7431,7 +7432,7 @@
       <c r="D20" s="95"/>
       <c r="E20" s="77"/>
       <c r="F20" s="77"/>
-      <c r="G20" s="199"/>
+      <c r="G20" s="151"/>
       <c r="H20" s="95"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.35">
@@ -7440,7 +7441,7 @@
       <c r="D21" s="95"/>
       <c r="E21" s="77"/>
       <c r="F21" s="77"/>
-      <c r="G21" s="199"/>
+      <c r="G21" s="151"/>
       <c r="H21" s="95"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.35">
@@ -7451,7 +7452,7 @@
       <c r="D22" s="95"/>
       <c r="E22" s="77"/>
       <c r="F22" s="77"/>
-      <c r="G22" s="199"/>
+      <c r="G22" s="151"/>
       <c r="H22" s="95"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.35">
@@ -7464,7 +7465,7 @@
       </c>
       <c r="E23" s="77"/>
       <c r="F23" s="77"/>
-      <c r="G23" s="199"/>
+      <c r="G23" s="151"/>
       <c r="H23" s="95"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.35">
@@ -7477,7 +7478,7 @@
       </c>
       <c r="E24" s="77"/>
       <c r="F24" s="77"/>
-      <c r="G24" s="199"/>
+      <c r="G24" s="151"/>
       <c r="H24" s="95"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.35">
@@ -7490,7 +7491,7 @@
       </c>
       <c r="E25" s="77"/>
       <c r="F25" s="77"/>
-      <c r="G25" s="199"/>
+      <c r="G25" s="151"/>
       <c r="H25" s="95"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.35">
@@ -7503,7 +7504,7 @@
       </c>
       <c r="E26" s="77"/>
       <c r="F26" s="77"/>
-      <c r="G26" s="199"/>
+      <c r="G26" s="151"/>
       <c r="H26" s="95"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.35">
@@ -7512,7 +7513,7 @@
       <c r="D27" s="102"/>
       <c r="E27" s="79"/>
       <c r="F27" s="79"/>
-      <c r="G27" s="200"/>
+      <c r="G27" s="152"/>
       <c r="H27" s="102"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.35">
@@ -7521,7 +7522,7 @@
       <c r="D28" s="102"/>
       <c r="E28" s="79"/>
       <c r="F28" s="79"/>
-      <c r="G28" s="200"/>
+      <c r="G28" s="152"/>
       <c r="H28" s="102"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.35">
@@ -7530,7 +7531,7 @@
       <c r="D29" s="102"/>
       <c r="E29" s="79"/>
       <c r="F29" s="79"/>
-      <c r="G29" s="200"/>
+      <c r="G29" s="152"/>
       <c r="H29" s="102"/>
     </row>
   </sheetData>
@@ -7549,7 +7550,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B1:M85"/>
   <sheetViews>
-    <sheetView topLeftCell="F68" zoomScale="74" zoomScaleNormal="74" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="74" zoomScaleNormal="74" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -7588,9 +7589,9 @@
       <c r="E2" s="33"/>
       <c r="F2" s="33"/>
       <c r="G2" s="33"/>
-      <c r="H2" s="189"/>
-      <c r="I2" s="189"/>
-      <c r="J2" s="189"/>
+      <c r="H2" s="141"/>
+      <c r="I2" s="141"/>
+      <c r="J2" s="141"/>
       <c r="K2" s="93"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.35">
@@ -7612,11 +7613,11 @@
       <c r="G3" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="H3" s="186" t="s">
+      <c r="H3" s="214" t="s">
         <v>270</v>
       </c>
-      <c r="I3" s="186"/>
-      <c r="J3" s="187"/>
+      <c r="I3" s="214"/>
+      <c r="J3" s="215"/>
       <c r="K3" s="109" t="s">
         <v>108</v>
       </c>
@@ -7654,15 +7655,15 @@
         <v>7</v>
       </c>
       <c r="G5" s="29"/>
-      <c r="H5" s="190" t="str">
+      <c r="H5" s="142" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#architectural-information"),
 "Architectural Information")</f>
         <v>Architectural Information</v>
       </c>
-      <c r="I5" s="202"/>
-      <c r="J5" s="202"/>
+      <c r="I5" s="154"/>
+      <c r="J5" s="154"/>
       <c r="K5" s="111"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.35">
@@ -7682,24 +7683,18 @@
         <v>7</v>
       </c>
       <c r="G6" s="29"/>
-      <c r="H6" s="190" t="str">
+      <c r="H6" s="142" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04h-Testing-Code-Quality.md#injection-flaws-mstg-arch-2-and-mstg-platform-2"),
 "Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)")</f>
         <v>Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)</v>
       </c>
-      <c r="I6" s="201" t="str">
-        <f>HYPERLINK(CONCATENATE(
-BASE_URL,
-"0x04h-Testing-Code-Quality.md#cross-site-scripting-flaws-mstg-arch-2-and-mstg-platform-2"),
-"Cross-Site Scripting Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)")</f>
-        <v>Cross-Site Scripting Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)</v>
-      </c>
-      <c r="J6" s="195" t="str">
+      <c r="I6" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#verifying-that-appropriate-authentication-is-in-place-mstg-arch-2-and-mstg-auth-1"),"Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)")</f>
         <v>Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)</v>
       </c>
+      <c r="J6" s="147"/>
       <c r="K6" s="111"/>
     </row>
     <row r="7" spans="2:11" ht="29" x14ac:dyDescent="0.35">
@@ -7719,15 +7714,15 @@
         <v>7</v>
       </c>
       <c r="G7" s="29"/>
-      <c r="H7" s="190" t="str">
+      <c r="H7" s="142" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#architectural-information"),
 "Architectural Information")</f>
         <v>Architectural Information</v>
       </c>
-      <c r="I7" s="202"/>
-      <c r="J7" s="202"/>
+      <c r="I7" s="154"/>
+      <c r="J7" s="154"/>
       <c r="K7" s="111"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.35">
@@ -7747,15 +7742,15 @@
         <v>7</v>
       </c>
       <c r="G8" s="29"/>
-      <c r="H8" s="190" t="str">
+      <c r="H8" s="142" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#identifying-sensitive-data"),
 "Identifying Sensitive Data")</f>
         <v>Identifying Sensitive Data</v>
       </c>
-      <c r="I8" s="202"/>
-      <c r="J8" s="202"/>
+      <c r="I8" s="154"/>
+      <c r="J8" s="154"/>
       <c r="K8" s="111"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.35">
@@ -7775,15 +7770,15 @@
       <c r="G9" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H9" s="190" t="str">
+      <c r="H9" s="142" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#environmental-information"),
 "Environmental Information")</f>
         <v>Environmental Information</v>
       </c>
-      <c r="I9" s="202"/>
-      <c r="J9" s="202"/>
+      <c r="I9" s="154"/>
+      <c r="J9" s="154"/>
       <c r="K9" s="111"/>
     </row>
     <row r="10" spans="2:11" ht="29" x14ac:dyDescent="0.35">
@@ -7803,15 +7798,15 @@
       <c r="G10" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H10" s="190" t="str">
+      <c r="H10" s="142" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#mapping-the-application"),
 "Mapping the Application")</f>
         <v>Mapping the Application</v>
       </c>
-      <c r="I10" s="202"/>
-      <c r="J10" s="202"/>
+      <c r="I10" s="154"/>
+      <c r="J10" s="154"/>
       <c r="K10" s="111"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.35">
@@ -7831,21 +7826,21 @@
       <c r="G11" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H11" s="190" t="str">
+      <c r="H11" s="142" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#principles-of-testing"),
 "Principles of Testing")</f>
         <v>Principles of Testing</v>
       </c>
-      <c r="I11" s="201" t="str">
+      <c r="I11" s="153" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#penetration-testing-aka-pentesting"),
 "Penetration Testing (a.k.a. Pentesting)")</f>
         <v>Penetration Testing (a.k.a. Pentesting)</v>
       </c>
-      <c r="J11" s="201"/>
+      <c r="J11" s="153"/>
       <c r="K11" s="111"/>
     </row>
     <row r="12" spans="2:11" ht="29" x14ac:dyDescent="0.35">
@@ -7865,15 +7860,15 @@
       <c r="G12" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H12" s="190" t="str">
+      <c r="H12" s="142" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04g-Testing-Cryptography.md#cryptographic-policy"),
 "Cryptographic policy")</f>
         <v>Cryptographic policy</v>
       </c>
-      <c r="I12" s="202"/>
-      <c r="J12" s="202"/>
+      <c r="I12" s="154"/>
+      <c r="J12" s="154"/>
       <c r="K12" s="111"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.35">
@@ -7893,15 +7888,15 @@
       <c r="G13" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H13" s="190" t="str">
+      <c r="H13" s="142" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06h-Testing-Platform-Interaction.md#testing-enforced-updating-mstg-arch-9"),
 "Testing enforced updating (MSTG-ARCH-9)")</f>
         <v>Testing enforced updating (MSTG-ARCH-9)</v>
       </c>
-      <c r="I13" s="202"/>
-      <c r="J13" s="202"/>
+      <c r="I13" s="154"/>
+      <c r="J13" s="154"/>
       <c r="K13" s="111"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.35">
@@ -7921,15 +7916,15 @@
       <c r="G14" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H14" s="190" t="str">
+      <c r="H14" s="142" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04b-Mobile-App-Security-Testing.md#security-testing-and-the-sdlc"),
 "Security Testing and the SDLC")</f>
         <v>Security Testing and the SDLC</v>
       </c>
-      <c r="I14" s="202"/>
-      <c r="J14" s="202"/>
+      <c r="I14" s="154"/>
+      <c r="J14" s="154"/>
       <c r="K14" s="111"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.35">
@@ -7943,9 +7938,9 @@
       <c r="E15" s="30"/>
       <c r="F15" s="36"/>
       <c r="G15" s="30"/>
-      <c r="H15" s="192"/>
-      <c r="I15" s="203"/>
-      <c r="J15" s="203"/>
+      <c r="H15" s="144"/>
+      <c r="I15" s="155"/>
+      <c r="J15" s="155"/>
       <c r="K15" s="110"/>
     </row>
     <row r="16" spans="2:11" ht="29" x14ac:dyDescent="0.35">
@@ -7965,12 +7960,12 @@
         <v>7</v>
       </c>
       <c r="G16" s="29"/>
-      <c r="H16" s="195" t="str">
+      <c r="H16" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#testing-local-data-storage-mstg-storage-1-and-mstg-storage-2"),"Testing Local Data Storage (MSTG-STORAGE-1 and MSTG-STORAGE-2)")</f>
         <v>Testing Local Data Storage (MSTG-STORAGE-1 and MSTG-STORAGE-2)</v>
       </c>
-      <c r="I16" s="202"/>
-      <c r="J16" s="202"/>
+      <c r="I16" s="154"/>
+      <c r="J16" s="154"/>
       <c r="K16" s="111"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.35">
@@ -7986,12 +7981,12 @@
       <c r="E17" s="25"/>
       <c r="F17" s="34"/>
       <c r="G17" s="29"/>
-      <c r="H17" s="195" t="str">
+      <c r="H17" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#testing-local-data-storage-mstg-storage-1-and-mstg-storage-2"),"Testing Local Data Storage (MSTG-STORAGE-1 and MSTG-STORAGE-2)")</f>
         <v>Testing Local Data Storage (MSTG-STORAGE-1 and MSTG-STORAGE-2)</v>
       </c>
-      <c r="I17" s="202"/>
-      <c r="J17" s="202"/>
+      <c r="I17" s="154"/>
+      <c r="J17" s="154"/>
       <c r="K17" s="111"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.35">
@@ -8011,12 +8006,12 @@
         <v>7</v>
       </c>
       <c r="G18" s="29"/>
-      <c r="H18" s="195" t="str">
+      <c r="H18" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#checking-logs-for-sensitive-data-mstg-storage-3"),"Checking Logs for Sensitive Data (MSTG-STORAGE-3)")</f>
         <v>Checking Logs for Sensitive Data (MSTG-STORAGE-3)</v>
       </c>
-      <c r="I18" s="202"/>
-      <c r="J18" s="202"/>
+      <c r="I18" s="154"/>
+      <c r="J18" s="154"/>
       <c r="K18" s="111"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.35">
@@ -8036,12 +8031,12 @@
         <v>7</v>
       </c>
       <c r="G19" s="29"/>
-      <c r="H19" s="195" t="str">
+      <c r="H19" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#determining-whether-sensitive-data-is-sent-to-third-parties-mstg-storage-4"),"Determining Whether Sensitive Data Is Sent to Third Parties (MSTG-STORAGE-4)")</f>
         <v>Determining Whether Sensitive Data Is Sent to Third Parties (MSTG-STORAGE-4)</v>
       </c>
-      <c r="I19" s="202"/>
-      <c r="J19" s="202"/>
+      <c r="I19" s="154"/>
+      <c r="J19" s="154"/>
       <c r="K19" s="111"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.35">
@@ -8061,12 +8056,12 @@
         <v>7</v>
       </c>
       <c r="G20" s="29"/>
-      <c r="H20" s="195" t="str">
+      <c r="H20" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#finding-sensitive-data-in-the-keyboard-cache-mstg-storage-5"),"Finding Sensitive Data in the Keyboard Cache (MSTG-STORAGE-5)")</f>
         <v>Finding Sensitive Data in the Keyboard Cache (MSTG-STORAGE-5)</v>
       </c>
-      <c r="I20" s="202"/>
-      <c r="J20" s="202"/>
+      <c r="I20" s="154"/>
+      <c r="J20" s="154"/>
       <c r="K20" s="111"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.35">
@@ -8086,12 +8081,12 @@
         <v>7</v>
       </c>
       <c r="G21" s="29"/>
-      <c r="H21" s="194" t="str">
+      <c r="H21" s="146" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#determining-whether-sensitive-data-is-exposed-via-ipc-mechanisms-mstg-storage-6"),"Determining Whether Sensitive Data Is Exposed via IPC Mechanisms (MSTG-STORAGE-6)")</f>
         <v>Determining Whether Sensitive Data Is Exposed via IPC Mechanisms (MSTG-STORAGE-6)</v>
       </c>
-      <c r="I21" s="202"/>
-      <c r="J21" s="202"/>
+      <c r="I21" s="154"/>
+      <c r="J21" s="154"/>
       <c r="K21" s="111"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.35">
@@ -8111,12 +8106,12 @@
         <v>7</v>
       </c>
       <c r="G22" s="29"/>
-      <c r="H22" s="195" t="str">
+      <c r="H22" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#checking-for-sensitive-data-disclosed-through-the-user-interface-mstg-storage-7"),"Checking for Sensitive Data Disclosed Through the User Interface (MSTG-STORAGE-7)")</f>
         <v>Checking for Sensitive Data Disclosed Through the User Interface (MSTG-STORAGE-7)</v>
       </c>
-      <c r="I22" s="202"/>
-      <c r="J22" s="202"/>
+      <c r="I22" s="154"/>
+      <c r="J22" s="154"/>
       <c r="K22" s="111"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.35">
@@ -8136,12 +8131,12 @@
       <c r="G23" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H23" s="195" t="str">
+      <c r="H23" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#testing-backups-for-sensitive-data-mstg-storage-8"),"Testing Backups for Sensitive Data (MSTG-STORAGE-8)")</f>
         <v>Testing Backups for Sensitive Data (MSTG-STORAGE-8)</v>
       </c>
-      <c r="I23" s="202"/>
-      <c r="J23" s="202"/>
+      <c r="I23" s="154"/>
+      <c r="J23" s="154"/>
       <c r="K23" s="111"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.35">
@@ -8161,12 +8156,12 @@
       <c r="G24" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H24" s="195" t="str">
+      <c r="H24" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#testing-auto-generated-screenshots-for-sensitive-information-mstg-storage-9"),"Testing Auto-Generated Screenshots for Sensitive Information (MSTG-STORAGE-9)")</f>
         <v>Testing Auto-Generated Screenshots for Sensitive Information (MSTG-STORAGE-9)</v>
       </c>
-      <c r="I24" s="202"/>
-      <c r="J24" s="202"/>
+      <c r="I24" s="154"/>
+      <c r="J24" s="154"/>
       <c r="K24" s="111"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.35">
@@ -8186,12 +8181,12 @@
       <c r="G25" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H25" s="195" t="str">
+      <c r="H25" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#testing-memory-for-sensitive-data-mstg-storage-10"),"Testing Memory for Sensitive Data (MSTG-STORAGE-10)")</f>
         <v>Testing Memory for Sensitive Data (MSTG-STORAGE-10)</v>
       </c>
-      <c r="I25" s="202"/>
-      <c r="J25" s="202"/>
+      <c r="I25" s="154"/>
+      <c r="J25" s="154"/>
       <c r="K25" s="111"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.35">
@@ -8211,12 +8206,12 @@
       <c r="G26" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H26" s="195" t="str">
+      <c r="H26" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06f-Testing-Local-Authentication.md#testing-local-authentication-mstg-auth-8-and-mstg-storage-11"),"Testing Local Authentication (MSTG-AUTH-8 and MSTG-STORAGE-11)")</f>
         <v>Testing Local Authentication (MSTG-AUTH-8 and MSTG-STORAGE-11)</v>
       </c>
-      <c r="I26" s="202"/>
-      <c r="J26" s="202"/>
+      <c r="I26" s="154"/>
+      <c r="J26" s="154"/>
       <c r="K26" s="111"/>
       <c r="L26" s="85"/>
     </row>
@@ -8237,12 +8232,12 @@
       <c r="G27" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H27" s="197" t="str">
+      <c r="H27" s="149" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04i-Testing-user-interaction.md#testing-user-education-mstg-storage-12"),"Testing User Education (MSTG-STORAGE-12)")</f>
         <v>Testing User Education (MSTG-STORAGE-12)</v>
       </c>
-      <c r="I27" s="202"/>
-      <c r="J27" s="202"/>
+      <c r="I27" s="154"/>
+      <c r="J27" s="154"/>
       <c r="K27" s="111"/>
       <c r="L27" s="72"/>
     </row>
@@ -8257,9 +8252,9 @@
       <c r="E28" s="30"/>
       <c r="F28" s="36"/>
       <c r="G28" s="30"/>
-      <c r="H28" s="192"/>
-      <c r="I28" s="203"/>
-      <c r="J28" s="203"/>
+      <c r="H28" s="144"/>
+      <c r="I28" s="155"/>
+      <c r="J28" s="155"/>
       <c r="K28" s="110"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.35">
@@ -8279,12 +8274,12 @@
         <v>7</v>
       </c>
       <c r="G29" s="29"/>
-      <c r="H29" s="195" t="str">
+      <c r="H29" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#testing-key-management-mstg-crypto-1-and-mstg-crypto-5"),"Testing Key Management (MSTG-CRYPTO-1 and MSTG-CRYPTO-5)")</f>
         <v>Testing Key Management (MSTG-CRYPTO-1 and MSTG-CRYPTO-5)</v>
       </c>
-      <c r="I29" s="202"/>
-      <c r="J29" s="202"/>
+      <c r="I29" s="154"/>
+      <c r="J29" s="154"/>
       <c r="K29" s="111"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.35">
@@ -8304,12 +8299,12 @@
         <v>7</v>
       </c>
       <c r="G30" s="29"/>
-      <c r="H30" s="194" t="str">
+      <c r="H30" s="146" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#verifying-the-configuration-of-cryptographic-standard-algorithms-mstg-crypto-2-and-mstg-crypto-3"),"Verifying the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2 and MSTG-CRYPTO-3)")</f>
         <v>Verifying the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2 and MSTG-CRYPTO-3)</v>
       </c>
-      <c r="I30" s="202"/>
-      <c r="J30" s="202"/>
+      <c r="I30" s="154"/>
+      <c r="J30" s="154"/>
       <c r="K30" s="111"/>
     </row>
     <row r="31" spans="2:12" ht="29" x14ac:dyDescent="0.35">
@@ -8329,12 +8324,12 @@
         <v>7</v>
       </c>
       <c r="G31" s="29"/>
-      <c r="H31" s="194" t="str">
+      <c r="H31" s="146" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#verifying-the-configuration-of-cryptographic-standard-algorithms-mstg-crypto-2-and-mstg-crypto-3"),"Verifying the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2 and MSTG-CRYPTO-3)")</f>
         <v>Verifying the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2 and MSTG-CRYPTO-3)</v>
       </c>
-      <c r="I31" s="202"/>
-      <c r="J31" s="202"/>
+      <c r="I31" s="154"/>
+      <c r="J31" s="154"/>
       <c r="K31" s="111"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.35">
@@ -8354,12 +8349,12 @@
         <v>7</v>
       </c>
       <c r="G32" s="29"/>
-      <c r="H32" s="195" t="str">
+      <c r="H32" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04g-Testing-Cryptography.md#identifying-insecure-andor-deprecated-cryptographic-algorithms-mstg-crypto-4"),"Identifying Insecure and/or Deprecated Cryptographic Algorithms (MSTG-CRYPTO-4)")</f>
         <v>Identifying Insecure and/or Deprecated Cryptographic Algorithms (MSTG-CRYPTO-4)</v>
       </c>
-      <c r="I32" s="202"/>
-      <c r="J32" s="202"/>
+      <c r="I32" s="154"/>
+      <c r="J32" s="154"/>
       <c r="K32" s="111"/>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.35">
@@ -8379,12 +8374,12 @@
         <v>7</v>
       </c>
       <c r="G33" s="29"/>
-      <c r="H33" s="195" t="str">
+      <c r="H33" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#testing-key-management-mstg-crypto-1-and-mstg-crypto-5"),"Testing Key Management (MSTG-CRYPTO-1 and MSTG-CRYPTO-5)")</f>
         <v>Testing Key Management (MSTG-CRYPTO-1 and MSTG-CRYPTO-5)</v>
       </c>
-      <c r="I33" s="202"/>
-      <c r="J33" s="202"/>
+      <c r="I33" s="154"/>
+      <c r="J33" s="154"/>
       <c r="K33" s="111"/>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.35">
@@ -8404,12 +8399,12 @@
         <v>7</v>
       </c>
       <c r="G34" s="29"/>
-      <c r="H34" s="195" t="str">
+      <c r="H34" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#testing-random-number-generation-mstg-crypto-6")," Testing Random Number Generation (MSTG-CRYPTO-6)")</f>
         <v xml:space="preserve"> Testing Random Number Generation (MSTG-CRYPTO-6)</v>
       </c>
-      <c r="I34" s="202"/>
-      <c r="J34" s="202"/>
+      <c r="I34" s="154"/>
+      <c r="J34" s="154"/>
       <c r="K34" s="111"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.35">
@@ -8423,9 +8418,9 @@
       <c r="E35" s="30"/>
       <c r="F35" s="36"/>
       <c r="G35" s="30"/>
-      <c r="H35" s="192"/>
-      <c r="I35" s="203"/>
-      <c r="J35" s="203"/>
+      <c r="H35" s="144"/>
+      <c r="I35" s="155"/>
+      <c r="J35" s="155"/>
       <c r="K35" s="110"/>
     </row>
     <row r="36" spans="2:13" ht="29" x14ac:dyDescent="0.35">
@@ -8445,15 +8440,15 @@
         <v>7</v>
       </c>
       <c r="G36" s="29"/>
-      <c r="H36" s="195" t="str">
+      <c r="H36" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#verifying-that-appropriate-authentication-is-in-place-mstg-arch-2-and-mstg-auth-1"),"Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)")</f>
         <v>Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)</v>
       </c>
-      <c r="I36" s="195" t="str">
+      <c r="I36" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-oauth-20-flows-mstg-auth-1-and-mstg-auth-3"),"Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)")</f>
         <v>Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)</v>
       </c>
-      <c r="J36" s="195"/>
+      <c r="J36" s="147"/>
       <c r="K36" s="111"/>
     </row>
     <row r="37" spans="2:13" ht="29" x14ac:dyDescent="0.35">
@@ -8473,12 +8468,12 @@
         <v>7</v>
       </c>
       <c r="G37" s="29"/>
-      <c r="H37" s="195" t="str">
+      <c r="H37" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-stateful-session-management-mstg-auth-2"),"Testing Stateful Session Management (MSTG-AUTH-2)")</f>
         <v>Testing Stateful Session Management (MSTG-AUTH-2)</v>
       </c>
-      <c r="I37" s="202"/>
-      <c r="J37" s="202"/>
+      <c r="I37" s="154"/>
+      <c r="J37" s="154"/>
       <c r="K37" s="111"/>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.35">
@@ -8498,15 +8493,15 @@
         <v>7</v>
       </c>
       <c r="G38" s="29"/>
-      <c r="H38" s="195" t="str">
+      <c r="H38" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-stateless-token-based-authentication-mstg-auth-3"),"Testing Stateless (Token-Based) Authentication (MSTG-AUTH-3)")</f>
         <v>Testing Stateless (Token-Based) Authentication (MSTG-AUTH-3)</v>
       </c>
-      <c r="I38" s="195" t="str">
+      <c r="I38" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-oauth-20-flows-mstg-auth-1-and-mstg-auth-3"),"Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)")</f>
         <v>Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)</v>
       </c>
-      <c r="J38" s="195"/>
+      <c r="J38" s="147"/>
       <c r="K38" s="111"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.35">
@@ -8522,12 +8517,12 @@
       <c r="E39" s="25"/>
       <c r="F39" s="34"/>
       <c r="G39" s="29"/>
-      <c r="H39" s="195" t="str">
+      <c r="H39" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-user-logout-mstg-auth-4"),"Testing User Logout (MSTG-AUTH-4)")</f>
         <v>Testing User Logout (MSTG-AUTH-4)</v>
       </c>
-      <c r="I39" s="202"/>
-      <c r="J39" s="202"/>
+      <c r="I39" s="154"/>
+      <c r="J39" s="154"/>
       <c r="K39" s="111"/>
       <c r="M39" s="38"/>
     </row>
@@ -8548,12 +8543,12 @@
         <v>7</v>
       </c>
       <c r="G40" s="29"/>
-      <c r="H40" s="195" t="str">
+      <c r="H40" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-best-practices-for-passwords-mstg-auth-5-and-mstg-auth-6"),"Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)")</f>
         <v>Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)</v>
       </c>
-      <c r="I40" s="202"/>
-      <c r="J40" s="202"/>
+      <c r="I40" s="154"/>
+      <c r="J40" s="154"/>
       <c r="K40" s="111"/>
       <c r="M40" s="38"/>
     </row>
@@ -8574,15 +8569,15 @@
         <v>7</v>
       </c>
       <c r="G41" s="29"/>
-      <c r="H41" s="195" t="str">
+      <c r="H41" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-best-practices-for-passwords-mstg-auth-5-and-mstg-auth-6"),"Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)")</f>
         <v>Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)</v>
       </c>
-      <c r="I41" s="195" t="str">
+      <c r="I41" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#dynamic-testing-mstg-auth-6"),"Dynamic Testing (MSTG-AUTH-6)")</f>
         <v>Dynamic Testing (MSTG-AUTH-6)</v>
       </c>
-      <c r="J41" s="195"/>
+      <c r="J41" s="147"/>
       <c r="K41" s="111"/>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.35">
@@ -8602,12 +8597,12 @@
         <v>7</v>
       </c>
       <c r="G42" s="29"/>
-      <c r="H42" s="195" t="str">
+      <c r="H42" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-session-timeout-mstg-auth-7"),"Testing Session Timeout (MSTG-AUTH-7)")</f>
         <v>Testing Session Timeout (MSTG-AUTH-7)</v>
       </c>
-      <c r="I42" s="204"/>
-      <c r="J42" s="204"/>
+      <c r="I42" s="156"/>
+      <c r="J42" s="156"/>
       <c r="K42" s="113"/>
     </row>
     <row r="43" spans="2:13" ht="29" x14ac:dyDescent="0.35">
@@ -8627,12 +8622,12 @@
       <c r="G43" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H43" s="195" t="str">
+      <c r="H43" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06f-Testing-Local-Authentication.md#testing-local-authentication-mstg-auth-8-and-mstg-storage-11"),"Testing Local Authentication (MSTG-AUTH-8 and MSTG-STORAGE-11)")</f>
         <v>Testing Local Authentication (MSTG-AUTH-8 and MSTG-STORAGE-11)</v>
       </c>
-      <c r="I43" s="195"/>
-      <c r="J43" s="195"/>
+      <c r="I43" s="147"/>
+      <c r="J43" s="147"/>
       <c r="K43" s="111"/>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.35">
@@ -8652,12 +8647,12 @@
       <c r="G44" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H44" s="194" t="str">
+      <c r="H44" s="146" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-two-factor-authentication-and-step-up-authentication-mstg-auth-9-and-mstg-auth-10"),"Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)")</f>
         <v>Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)</v>
       </c>
-      <c r="I44" s="202"/>
-      <c r="J44" s="202"/>
+      <c r="I44" s="154"/>
+      <c r="J44" s="154"/>
       <c r="K44" s="111"/>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.35">
@@ -8677,12 +8672,12 @@
       <c r="G45" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H45" s="194" t="str">
+      <c r="H45" s="146" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-two-factor-authentication-and-step-up-authentication-mstg-auth-9-and-mstg-auth-10"),"Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)")</f>
         <v>Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)</v>
       </c>
-      <c r="I45" s="202"/>
-      <c r="J45" s="202"/>
+      <c r="I45" s="154"/>
+      <c r="J45" s="154"/>
       <c r="K45" s="111"/>
     </row>
     <row r="46" spans="2:13" ht="29" x14ac:dyDescent="0.35">
@@ -8702,15 +8697,15 @@
       <c r="G46" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H46" s="197" t="str">
+      <c r="H46" s="149" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04e-Testing-Authentication-and-Session-Management.md#testing-login-activity-and-device-blocking-mstg-auth-11"),
 "Testing Login Activity and Device Blocking (MSTG-AUTH-11)")</f>
         <v>Testing Login Activity and Device Blocking (MSTG-AUTH-11)</v>
       </c>
-      <c r="I46" s="202"/>
-      <c r="J46" s="202"/>
+      <c r="I46" s="154"/>
+      <c r="J46" s="154"/>
       <c r="K46" s="111"/>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.35">
@@ -8724,9 +8719,9 @@
       <c r="E47" s="30"/>
       <c r="F47" s="36"/>
       <c r="G47" s="30"/>
-      <c r="H47" s="192"/>
-      <c r="I47" s="203"/>
-      <c r="J47" s="203"/>
+      <c r="H47" s="144"/>
+      <c r="I47" s="155"/>
+      <c r="J47" s="155"/>
       <c r="K47" s="110"/>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.35">
@@ -8746,12 +8741,12 @@
         <v>7</v>
       </c>
       <c r="G48" s="29"/>
-      <c r="H48" s="194" t="str">
+      <c r="H48" s="146" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#verifying-data-encryption-on-the-network-mstg-network-1-and-mstg-network-2"),"Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)")</f>
         <v>Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)</v>
       </c>
-      <c r="I48" s="201"/>
-      <c r="J48" s="201"/>
+      <c r="I48" s="153"/>
+      <c r="J48" s="153"/>
       <c r="K48" s="116"/>
     </row>
     <row r="49" spans="2:11" ht="29" x14ac:dyDescent="0.35">
@@ -8771,15 +8766,15 @@
         <v>7</v>
       </c>
       <c r="G49" s="29"/>
-      <c r="H49" s="194" t="str">
+      <c r="H49" s="146" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#verifying-data-encryption-on-the-network-mstg-network-1-and-mstg-network-2"),"Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)")</f>
         <v>Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)</v>
       </c>
-      <c r="I49" s="201" t="str">
+      <c r="I49" s="153" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06g-Testing-Network-Communication.md#app-transport-security-mstg-network-2"),"App Transport Security (MSTG-NETWORK-2)")</f>
         <v>App Transport Security (MSTG-NETWORK-2)</v>
       </c>
-      <c r="J49" s="201"/>
+      <c r="J49" s="153"/>
       <c r="K49" s="116"/>
     </row>
     <row r="50" spans="2:11" ht="29" x14ac:dyDescent="0.35">
@@ -8799,12 +8794,12 @@
         <v>7</v>
       </c>
       <c r="G50" s="29"/>
-      <c r="H50" s="195" t="str">
+      <c r="H50" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06g-Testing-Network-Communication.md#testing-custom-certificate-stores-and-certificate-pinning-mstg-network-3-and-mstg-network-4"),"Testing Custom Certificate Stores and Certificate Pinning (MSTG-NETWORK-3 and MSTG-NETWORK-4)")</f>
         <v>Testing Custom Certificate Stores and Certificate Pinning (MSTG-NETWORK-3 and MSTG-NETWORK-4)</v>
       </c>
-      <c r="I50" s="202"/>
-      <c r="J50" s="202"/>
+      <c r="I50" s="154"/>
+      <c r="J50" s="154"/>
       <c r="K50" s="116"/>
     </row>
     <row r="51" spans="2:11" ht="29" x14ac:dyDescent="0.35">
@@ -8824,12 +8819,12 @@
       <c r="G51" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H51" s="195" t="str">
+      <c r="H51" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06g-Testing-Network-Communication.md#testing-custom-certificate-stores-and-certificate-pinning-mstg-network-3-and-mstg-network-4"),"Testing Custom Certificate Stores and Certificate Pinning (MSTG-NETWORK-3 and MSTG-NETWORK-4)")</f>
         <v>Testing Custom Certificate Stores and Certificate Pinning (MSTG-NETWORK-3 and MSTG-NETWORK-4)</v>
       </c>
-      <c r="I51" s="202"/>
-      <c r="J51" s="202"/>
+      <c r="I51" s="154"/>
+      <c r="J51" s="154"/>
       <c r="K51" s="111"/>
     </row>
     <row r="52" spans="2:11" ht="29" x14ac:dyDescent="0.35">
@@ -8849,12 +8844,12 @@
       <c r="G52" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H52" s="194" t="str">
+      <c r="H52" s="146" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#making-sure-that-critical-operations-use-secure-communication-channels-mstg-network-5"),"Making Sure that Critical Operations Use Secure Communication Channels (MSTG-NETWORK-5)")</f>
         <v>Making Sure that Critical Operations Use Secure Communication Channels (MSTG-NETWORK-5)</v>
       </c>
-      <c r="I52" s="202"/>
-      <c r="J52" s="202"/>
+      <c r="I52" s="154"/>
+      <c r="J52" s="154"/>
       <c r="K52" s="111"/>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.35">
@@ -8874,15 +8869,15 @@
       <c r="G53" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="H53" s="195" t="str">
+      <c r="H53" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06i-Testing-Code-Quality-and-Build-Settings.md#checking-for-weaknesses-in-third-party-libraries-mstg-code-5"),
 "Checking for Weaknesses in Third Party Libraries (MSTG-CODE-5)")</f>
         <v>Checking for Weaknesses in Third Party Libraries (MSTG-CODE-5)</v>
       </c>
-      <c r="I53" s="202"/>
-      <c r="J53" s="202"/>
+      <c r="I53" s="154"/>
+      <c r="J53" s="154"/>
       <c r="K53" s="111"/>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.35">
@@ -8896,9 +8891,9 @@
       <c r="E54" s="30"/>
       <c r="F54" s="36"/>
       <c r="G54" s="30"/>
-      <c r="H54" s="192"/>
-      <c r="I54" s="203"/>
-      <c r="J54" s="203"/>
+      <c r="H54" s="144"/>
+      <c r="I54" s="155"/>
+      <c r="J54" s="155"/>
       <c r="K54" s="110"/>
     </row>
     <row r="55" spans="2:11" ht="29" x14ac:dyDescent="0.35">
@@ -8918,12 +8913,12 @@
         <v>7</v>
       </c>
       <c r="G55" s="29"/>
-      <c r="H55" s="195" t="str">
+      <c r="H55" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-app-permissions-mstg-platform-1"),"Testing App Permissions (MSTG-PLATFORM-1)")</f>
         <v>Testing App Permissions (MSTG-PLATFORM-1)</v>
       </c>
-      <c r="I55" s="202"/>
-      <c r="J55" s="202"/>
+      <c r="I55" s="154"/>
+      <c r="J55" s="154"/>
       <c r="K55" s="111"/>
     </row>
     <row r="56" spans="2:11" ht="29" x14ac:dyDescent="0.35">
@@ -8943,12 +8938,12 @@
         <v>7</v>
       </c>
       <c r="G56" s="29"/>
-      <c r="H56" s="195" t="str">
+      <c r="H56" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04h-Testing-Code-Quality.md#injection-flaws-mstg-arch-2-and-mstg-platform-2"),"Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)")</f>
         <v>Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)</v>
       </c>
-      <c r="I56" s="202"/>
-      <c r="J56" s="202"/>
+      <c r="I56" s="154"/>
+      <c r="J56" s="154"/>
       <c r="K56" s="111"/>
     </row>
     <row r="57" spans="2:11" ht="29" x14ac:dyDescent="0.35">
@@ -8968,12 +8963,12 @@
         <v>7</v>
       </c>
       <c r="G57" s="29"/>
-      <c r="H57" s="195" t="str">
+      <c r="H57" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-custom-url-schemes-mstg-platform-3"),"Testing Custom URL Schemes (MSTG-PLATFORM-3)")</f>
         <v>Testing Custom URL Schemes (MSTG-PLATFORM-3)</v>
       </c>
-      <c r="I57" s="202"/>
-      <c r="J57" s="202"/>
+      <c r="I57" s="154"/>
+      <c r="J57" s="154"/>
       <c r="K57" s="111"/>
     </row>
     <row r="58" spans="2:11" ht="29" x14ac:dyDescent="0.35">
@@ -8993,15 +8988,15 @@
         <v>7</v>
       </c>
       <c r="G58" s="29"/>
-      <c r="H58" s="190" t="str">
+      <c r="H58" s="142" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06h-Testing-Platform-Interaction.md#testing-for-sensitive-functionality-exposure-through-ipc-mstg-platform-4"),
 "Testing for Sensitive Functionality Exposure Through IPC (MSTG-PLATFORM-4)")</f>
         <v>Testing for Sensitive Functionality Exposure Through IPC (MSTG-PLATFORM-4)</v>
       </c>
-      <c r="I58" s="202"/>
-      <c r="J58" s="202"/>
+      <c r="I58" s="154"/>
+      <c r="J58" s="154"/>
       <c r="K58" s="111"/>
     </row>
     <row r="59" spans="2:11" ht="29" x14ac:dyDescent="0.35">
@@ -9021,12 +9016,12 @@
         <v>7</v>
       </c>
       <c r="G59" s="29"/>
-      <c r="H59" s="195" t="str">
+      <c r="H59" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-ios-webviews-mstg-platform-5"),"Testing iOS WebViews (MSTG-PLATFORM-5)")</f>
         <v>Testing iOS WebViews (MSTG-PLATFORM-5)</v>
       </c>
-      <c r="I59" s="202"/>
-      <c r="J59" s="202"/>
+      <c r="I59" s="154"/>
+      <c r="J59" s="154"/>
       <c r="K59" s="111"/>
     </row>
     <row r="60" spans="2:11" ht="29" x14ac:dyDescent="0.35">
@@ -9046,12 +9041,12 @@
         <v>7</v>
       </c>
       <c r="G60" s="29"/>
-      <c r="H60" s="195" t="str">
+      <c r="H60" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-webview-protocol-handlers-mstg-platform-6"),"Testing WebView Protocol Handlers (MSTG-PLATFORM-6)")</f>
         <v>Testing WebView Protocol Handlers (MSTG-PLATFORM-6)</v>
       </c>
-      <c r="I60" s="202"/>
-      <c r="J60" s="202"/>
+      <c r="I60" s="154"/>
+      <c r="J60" s="154"/>
       <c r="K60" s="111"/>
     </row>
     <row r="61" spans="2:11" ht="29" x14ac:dyDescent="0.35">
@@ -9071,12 +9066,12 @@
         <v>7</v>
       </c>
       <c r="G61" s="29"/>
-      <c r="H61" s="195" t="str">
+      <c r="H61" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#determining-whether-native-methods-are-exposed-through-webviews-mstg-platform-7"),"Determining Whether Native Methods Are Exposed Through WebViews (MSTG-PLATFORM-7)")</f>
         <v>Determining Whether Native Methods Are Exposed Through WebViews (MSTG-PLATFORM-7)</v>
       </c>
-      <c r="I61" s="202"/>
-      <c r="J61" s="202"/>
+      <c r="I61" s="154"/>
+      <c r="J61" s="154"/>
       <c r="K61" s="111"/>
     </row>
     <row r="62" spans="2:11" ht="29" x14ac:dyDescent="0.35">
@@ -9096,12 +9091,12 @@
         <v>7</v>
       </c>
       <c r="G62" s="29"/>
-      <c r="H62" s="195" t="str">
+      <c r="H62" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-object-persistence-mstg-platform-8"),"Testing Object Persistence (MSTG-PLATFORM-8)")</f>
         <v>Testing Object Persistence (MSTG-PLATFORM-8)</v>
       </c>
-      <c r="I62" s="202"/>
-      <c r="J62" s="202"/>
+      <c r="I62" s="154"/>
+      <c r="J62" s="154"/>
       <c r="K62" s="111"/>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.35">
@@ -9115,9 +9110,9 @@
       <c r="E63" s="30"/>
       <c r="F63" s="36"/>
       <c r="G63" s="30"/>
-      <c r="H63" s="192"/>
-      <c r="I63" s="203"/>
-      <c r="J63" s="203"/>
+      <c r="H63" s="144"/>
+      <c r="I63" s="155"/>
+      <c r="J63" s="155"/>
       <c r="K63" s="110"/>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.35">
@@ -9137,12 +9132,12 @@
         <v>7</v>
       </c>
       <c r="G64" s="29"/>
-      <c r="H64" s="195" t="str">
+      <c r="H64" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#making-sure-that-the-app-is-properly-signed-mstg-code-1"),"Making Sure that the App Is Properly Signed (MSTG-CODE-1)")</f>
         <v>Making Sure that the App Is Properly Signed (MSTG-CODE-1)</v>
       </c>
-      <c r="I64" s="202"/>
-      <c r="J64" s="202"/>
+      <c r="I64" s="154"/>
+      <c r="J64" s="154"/>
       <c r="K64" s="111"/>
     </row>
     <row r="65" spans="2:11" x14ac:dyDescent="0.35">
@@ -9162,12 +9157,12 @@
         <v>7</v>
       </c>
       <c r="G65" s="29"/>
-      <c r="H65" s="195" t="str">
+      <c r="H65" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#determining-whether-the-app-is-debuggable-mstg-code-2"),"Determining Whether the App is Debuggable (MSTG-CODE-2)")</f>
         <v>Determining Whether the App is Debuggable (MSTG-CODE-2)</v>
       </c>
-      <c r="I65" s="202"/>
-      <c r="J65" s="202"/>
+      <c r="I65" s="154"/>
+      <c r="J65" s="154"/>
       <c r="K65" s="111"/>
     </row>
     <row r="66" spans="2:11" x14ac:dyDescent="0.35">
@@ -9187,12 +9182,12 @@
         <v>7</v>
       </c>
       <c r="G66" s="29"/>
-      <c r="H66" s="195" t="str">
+      <c r="H66" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#finding-debugging-symbols-mstg-code-3"),"Finding Debugging Symbols (MSTG-CODE-3)")</f>
         <v>Finding Debugging Symbols (MSTG-CODE-3)</v>
       </c>
-      <c r="I66" s="202"/>
-      <c r="J66" s="202"/>
+      <c r="I66" s="154"/>
+      <c r="J66" s="154"/>
       <c r="K66" s="111"/>
     </row>
     <row r="67" spans="2:11" x14ac:dyDescent="0.35">
@@ -9212,12 +9207,12 @@
         <v>7</v>
       </c>
       <c r="G67" s="29"/>
-      <c r="H67" s="195" t="str">
+      <c r="H67" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#finding-debugging-code-and-verbose-error-logging-mstg-code-4"),"Finding Debugging Code and Verbose Error Logging (MSTG-CODE-4)")</f>
         <v>Finding Debugging Code and Verbose Error Logging (MSTG-CODE-4)</v>
       </c>
-      <c r="I67" s="202"/>
-      <c r="J67" s="202"/>
+      <c r="I67" s="154"/>
+      <c r="J67" s="154"/>
       <c r="K67" s="111"/>
     </row>
     <row r="68" spans="2:11" ht="29" x14ac:dyDescent="0.35">
@@ -9237,12 +9232,12 @@
         <v>7</v>
       </c>
       <c r="G68" s="29"/>
-      <c r="H68" s="197" t="str">
+      <c r="H68" s="149" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#checking-for-weaknesses-in-third-party-libraries-mstg-code-5"),"Checking for Weaknesses in Third Party Libraries (MSTG-CODE-5)")</f>
         <v>Checking for Weaknesses in Third Party Libraries (MSTG-CODE-5)</v>
       </c>
-      <c r="I68" s="202"/>
-      <c r="J68" s="202"/>
+      <c r="I68" s="154"/>
+      <c r="J68" s="154"/>
       <c r="K68" s="111"/>
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.35">
@@ -9262,12 +9257,12 @@
         <v>7</v>
       </c>
       <c r="G69" s="29"/>
-      <c r="H69" s="195" t="str">
+      <c r="H69" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#testing-exception-handling-mstg-code-6"),"Testing Exception Handling (MSTG-CODE-6)")</f>
         <v>Testing Exception Handling (MSTG-CODE-6)</v>
       </c>
-      <c r="I69" s="202"/>
-      <c r="J69" s="202"/>
+      <c r="I69" s="154"/>
+      <c r="J69" s="154"/>
       <c r="K69" s="111"/>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.35">
@@ -9287,12 +9282,12 @@
         <v>7</v>
       </c>
       <c r="G70" s="29"/>
-      <c r="H70" s="195" t="str">
+      <c r="H70" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#testing-exception-handling-mstg-code-6"),"Testing Exception Handling (MSTG-CODE-6)")</f>
         <v>Testing Exception Handling (MSTG-CODE-6)</v>
       </c>
-      <c r="I70" s="202"/>
-      <c r="J70" s="202"/>
+      <c r="I70" s="154"/>
+      <c r="J70" s="154"/>
       <c r="K70" s="111"/>
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.35">
@@ -9312,12 +9307,12 @@
         <v>7</v>
       </c>
       <c r="G71" s="29"/>
-      <c r="H71" s="195" t="str">
+      <c r="H71" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#memory-corruption-bugs-mstg-code-8"),"Memory Corruption Bugs (MSTG-CODE-8)")</f>
         <v>Memory Corruption Bugs (MSTG-CODE-8)</v>
       </c>
-      <c r="I71" s="202"/>
-      <c r="J71" s="202"/>
+      <c r="I71" s="154"/>
+      <c r="J71" s="154"/>
       <c r="K71" s="111"/>
     </row>
     <row r="72" spans="2:11" ht="29" x14ac:dyDescent="0.35">
@@ -9337,12 +9332,12 @@
         <v>7</v>
       </c>
       <c r="G72" s="29"/>
-      <c r="H72" s="195" t="str">
+      <c r="H72" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#make-sure-that-free-security-features-are-activated-mstg-code-9"),"Make Sure That Free Security Features Are Activated (MSTG-CODE-9)")</f>
         <v>Make Sure That Free Security Features Are Activated (MSTG-CODE-9)</v>
       </c>
-      <c r="I72" s="202"/>
-      <c r="J72" s="202"/>
+      <c r="I72" s="154"/>
+      <c r="J72" s="154"/>
       <c r="K72" s="111"/>
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.35">
@@ -9352,9 +9347,9 @@
       <c r="E73" s="31"/>
       <c r="F73" s="31"/>
       <c r="G73" s="31"/>
-      <c r="H73" s="198"/>
-      <c r="I73" s="205"/>
-      <c r="J73" s="213"/>
+      <c r="H73" s="150"/>
+      <c r="I73" s="157"/>
+      <c r="J73" s="165"/>
       <c r="K73" s="118"/>
     </row>
     <row r="74" spans="2:11" x14ac:dyDescent="0.35">
@@ -9364,9 +9359,9 @@
       <c r="E74" s="32"/>
       <c r="F74" s="32"/>
       <c r="G74" s="32"/>
-      <c r="H74" s="199"/>
-      <c r="I74" s="199"/>
-      <c r="J74" s="199"/>
+      <c r="H74" s="151"/>
+      <c r="I74" s="151"/>
+      <c r="J74" s="151"/>
       <c r="K74" s="98"/>
     </row>
     <row r="75" spans="2:11" x14ac:dyDescent="0.35">
@@ -9376,9 +9371,9 @@
       <c r="E75" s="32"/>
       <c r="F75" s="32"/>
       <c r="G75" s="32"/>
-      <c r="H75" s="199"/>
-      <c r="I75" s="199"/>
-      <c r="J75" s="199"/>
+      <c r="H75" s="151"/>
+      <c r="I75" s="151"/>
+      <c r="J75" s="151"/>
       <c r="K75" s="98"/>
     </row>
     <row r="76" spans="2:11" x14ac:dyDescent="0.35">
@@ -9388,9 +9383,9 @@
       <c r="E76" s="32"/>
       <c r="F76" s="32"/>
       <c r="G76" s="32"/>
-      <c r="H76" s="199"/>
-      <c r="I76" s="199"/>
-      <c r="J76" s="199"/>
+      <c r="H76" s="151"/>
+      <c r="I76" s="151"/>
+      <c r="J76" s="151"/>
       <c r="K76" s="98"/>
     </row>
     <row r="77" spans="2:11" x14ac:dyDescent="0.35">
@@ -9402,9 +9397,9 @@
       <c r="E77" s="32"/>
       <c r="F77" s="32"/>
       <c r="G77" s="32"/>
-      <c r="H77" s="199"/>
-      <c r="I77" s="199"/>
-      <c r="J77" s="199"/>
+      <c r="H77" s="151"/>
+      <c r="I77" s="151"/>
+      <c r="J77" s="151"/>
       <c r="K77" s="98"/>
     </row>
     <row r="78" spans="2:11" x14ac:dyDescent="0.35">
@@ -9418,9 +9413,9 @@
       <c r="E78" s="32"/>
       <c r="F78" s="32"/>
       <c r="G78" s="32"/>
-      <c r="H78" s="199"/>
-      <c r="I78" s="199"/>
-      <c r="J78" s="199"/>
+      <c r="H78" s="151"/>
+      <c r="I78" s="151"/>
+      <c r="J78" s="151"/>
       <c r="K78" s="98"/>
     </row>
     <row r="79" spans="2:11" x14ac:dyDescent="0.35">
@@ -9434,9 +9429,9 @@
       <c r="E79" s="32"/>
       <c r="F79" s="32"/>
       <c r="G79" s="32"/>
-      <c r="H79" s="199"/>
-      <c r="I79" s="199"/>
-      <c r="J79" s="199"/>
+      <c r="H79" s="151"/>
+      <c r="I79" s="151"/>
+      <c r="J79" s="151"/>
       <c r="K79" s="98"/>
     </row>
     <row r="80" spans="2:11" x14ac:dyDescent="0.35">
@@ -9450,9 +9445,9 @@
       <c r="E80" s="32"/>
       <c r="F80" s="32"/>
       <c r="G80" s="32"/>
-      <c r="H80" s="199"/>
-      <c r="I80" s="199"/>
-      <c r="J80" s="199"/>
+      <c r="H80" s="151"/>
+      <c r="I80" s="151"/>
+      <c r="J80" s="151"/>
       <c r="K80" s="98"/>
     </row>
     <row r="81" spans="2:11" x14ac:dyDescent="0.35">
@@ -9466,9 +9461,9 @@
       <c r="E81" s="32"/>
       <c r="F81" s="32"/>
       <c r="G81" s="32"/>
-      <c r="H81" s="199"/>
-      <c r="I81" s="199"/>
-      <c r="J81" s="199"/>
+      <c r="H81" s="151"/>
+      <c r="I81" s="151"/>
+      <c r="J81" s="151"/>
       <c r="K81" s="98"/>
     </row>
     <row r="82" spans="2:11" x14ac:dyDescent="0.35">
@@ -9478,9 +9473,9 @@
       <c r="E82" s="23"/>
       <c r="F82" s="23"/>
       <c r="G82" s="23"/>
-      <c r="H82" s="199"/>
-      <c r="I82" s="200"/>
-      <c r="J82" s="200"/>
+      <c r="H82" s="151"/>
+      <c r="I82" s="152"/>
+      <c r="J82" s="152"/>
       <c r="K82" s="99"/>
     </row>
     <row r="83" spans="2:11" x14ac:dyDescent="0.35">
@@ -9490,9 +9485,9 @@
       <c r="E83" s="23"/>
       <c r="F83" s="23"/>
       <c r="G83" s="23"/>
-      <c r="H83" s="199"/>
-      <c r="I83" s="200"/>
-      <c r="J83" s="200"/>
+      <c r="H83" s="151"/>
+      <c r="I83" s="152"/>
+      <c r="J83" s="152"/>
       <c r="K83" s="99"/>
     </row>
     <row r="84" spans="2:11" x14ac:dyDescent="0.35">
@@ -9502,9 +9497,9 @@
       <c r="E84" s="23"/>
       <c r="F84" s="23"/>
       <c r="G84" s="23"/>
-      <c r="H84" s="199"/>
-      <c r="I84" s="200"/>
-      <c r="J84" s="200"/>
+      <c r="H84" s="151"/>
+      <c r="I84" s="152"/>
+      <c r="J84" s="152"/>
       <c r="K84" s="99"/>
     </row>
     <row r="85" spans="2:11" x14ac:dyDescent="0.35">
@@ -9514,9 +9509,9 @@
       <c r="E85" s="23"/>
       <c r="F85" s="23"/>
       <c r="G85" s="23"/>
-      <c r="H85" s="200"/>
-      <c r="I85" s="200"/>
-      <c r="J85" s="200"/>
+      <c r="H85" s="152"/>
+      <c r="I85" s="152"/>
+      <c r="J85" s="152"/>
       <c r="K85" s="99"/>
     </row>
   </sheetData>
@@ -9524,18 +9519,23 @@
     <mergeCell ref="H3:J3"/>
   </mergeCells>
   <conditionalFormatting sqref="M1:M1048576">
-    <cfRule type="containsText" dxfId="10" priority="3" operator="containsText" text="0x05">
+    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="0x05">
       <formula>NOT(ISERROR(SEARCH("0x05",M1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H26 H28:H1048576">
-    <cfRule type="containsText" dxfId="9" priority="2" operator="containsText" text="0x05">
+    <cfRule type="containsText" dxfId="10" priority="3" operator="containsText" text="0x05">
       <formula>NOT(ISERROR(SEARCH("0x05",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6">
+    <cfRule type="containsText" dxfId="9" priority="2" operator="containsText" text="0x05">
+      <formula>NOT(ISERROR(SEARCH("0x05",J6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="0x05">
-      <formula>NOT(ISERROR(SEARCH("0x05",J6)))</formula>
+      <formula>NOT(ISERROR(SEARCH("0x05",I6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="2">
@@ -9577,11 +9577,11 @@
         <v>130</v>
       </c>
       <c r="C1" s="53"/>
-      <c r="G1" s="200"/>
+      <c r="G1" s="152"/>
       <c r="H1" s="99"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="G2" s="200"/>
+      <c r="G2" s="152"/>
       <c r="H2" s="99"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.35">
@@ -9600,7 +9600,7 @@
       <c r="F3" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="G3" s="206" t="s">
+      <c r="G3" s="158" t="s">
         <v>365</v>
       </c>
       <c r="H3" s="109" t="s">
@@ -9615,7 +9615,7 @@
       </c>
       <c r="E4" s="30"/>
       <c r="F4" s="30"/>
-      <c r="G4" s="207"/>
+      <c r="G4" s="159"/>
       <c r="H4" s="110"/>
     </row>
     <row r="5" spans="2:8" ht="29" x14ac:dyDescent="0.35">
@@ -9634,7 +9634,7 @@
       <c r="F5" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="195" t="str">
+      <c r="G5" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#jailbreak-detection-mstg-resilience-1"),"Jailbreak Detection (MSTG-RESILIENCE-1)")</f>
         <v>Jailbreak Detection (MSTG-RESILIENCE-1)</v>
       </c>
@@ -9656,7 +9656,7 @@
       <c r="F6" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G6" s="208" t="str">
+      <c r="G6" s="160" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#anti-debugging-checks-mstg-resilience-2"),"Anti-Debugging Checks (MSTG-RESILIENCE-2)")</f>
         <v>Anti-Debugging Checks (MSTG-RESILIENCE-2)</v>
       </c>
@@ -9678,7 +9678,7 @@
       <c r="F7" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G7" s="208" t="str">
+      <c r="G7" s="160" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#file-integrity-checks-mstg-resilience-3-and-mstg-resilience-11"),"File Integrity Checks (MSTG-RESILIENCE-3 and MSTG-RESILIENCE-11)")</f>
         <v>File Integrity Checks (MSTG-RESILIENCE-3 and MSTG-RESILIENCE-11)</v>
       </c>
@@ -9700,7 +9700,7 @@
       <c r="F8" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="214" t="s">
+      <c r="G8" s="166" t="s">
         <v>128</v>
       </c>
       <c r="H8" s="111"/>
@@ -9721,7 +9721,7 @@
       <c r="F9" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G9" s="215" t="s">
+      <c r="G9" s="167" t="s">
         <v>128</v>
       </c>
       <c r="H9" s="111"/>
@@ -9742,7 +9742,7 @@
       <c r="F10" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G10" s="214" t="s">
+      <c r="G10" s="166" t="s">
         <v>128</v>
       </c>
       <c r="H10" s="111"/>
@@ -9763,7 +9763,7 @@
       <c r="F11" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G11" s="211" t="s">
+      <c r="G11" s="163" t="s">
         <v>128</v>
       </c>
       <c r="H11" s="111"/>
@@ -9784,7 +9784,7 @@
       <c r="F12" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G12" s="211" t="s">
+      <c r="G12" s="163" t="s">
         <v>128</v>
       </c>
       <c r="H12" s="111"/>
@@ -9805,7 +9805,7 @@
       <c r="F13" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G13" s="215" t="s">
+      <c r="G13" s="167" t="s">
         <v>128</v>
       </c>
       <c r="H13" s="111"/>
@@ -9818,7 +9818,7 @@
       </c>
       <c r="E14" s="30"/>
       <c r="F14" s="30"/>
-      <c r="G14" s="207"/>
+      <c r="G14" s="159"/>
       <c r="H14" s="110"/>
     </row>
     <row r="15" spans="2:8" ht="29" x14ac:dyDescent="0.35">
@@ -9837,7 +9837,7 @@
       <c r="F15" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G15" s="195" t="str">
+      <c r="G15" s="147" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#device-binding-mstg-resilience-10"),"Device Binding (MSTG-RESILIENCE-10)")</f>
         <v>Device Binding (MSTG-RESILIENCE-10)</v>
       </c>
@@ -9851,7 +9851,7 @@
       </c>
       <c r="E16" s="30"/>
       <c r="F16" s="30"/>
-      <c r="G16" s="207"/>
+      <c r="G16" s="159"/>
       <c r="H16" s="110"/>
     </row>
     <row r="17" spans="2:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -9870,7 +9870,7 @@
       <c r="F17" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G17" s="216" t="str">
+      <c r="G17" s="168" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#file-integrity-checks-mstg-resilience-3-and-mstg-resilience-11"),"File Integrity Checks (MSTG-RESILIENCE-3 and MSTG-RESILIENCE-11)")</f>
         <v>File Integrity Checks (MSTG-RESILIENCE-3 and MSTG-RESILIENCE-11)</v>
       </c>
@@ -9892,7 +9892,7 @@
       <c r="F18" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G18" s="211" t="s">
+      <c r="G18" s="163" t="s">
         <v>128</v>
       </c>
       <c r="H18" s="111"/>
@@ -9903,7 +9903,7 @@
       <c r="D19" s="97"/>
       <c r="E19" s="31"/>
       <c r="F19" s="31"/>
-      <c r="G19" s="212"/>
+      <c r="G19" s="164"/>
       <c r="H19" s="112"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.35">
@@ -9912,7 +9912,7 @@
       <c r="D20" s="98"/>
       <c r="E20" s="32"/>
       <c r="F20" s="32"/>
-      <c r="G20" s="199"/>
+      <c r="G20" s="151"/>
       <c r="H20" s="98"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.35">
@@ -9921,7 +9921,7 @@
       <c r="D21" s="98"/>
       <c r="E21" s="32"/>
       <c r="F21" s="32"/>
-      <c r="G21" s="199"/>
+      <c r="G21" s="151"/>
       <c r="H21" s="98"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.35">
@@ -9932,7 +9932,7 @@
       <c r="D22" s="98"/>
       <c r="E22" s="32"/>
       <c r="F22" s="32"/>
-      <c r="G22" s="199"/>
+      <c r="G22" s="151"/>
       <c r="H22" s="98"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.35">
@@ -9945,7 +9945,7 @@
       </c>
       <c r="E23" s="32"/>
       <c r="F23" s="32"/>
-      <c r="G23" s="199"/>
+      <c r="G23" s="151"/>
       <c r="H23" s="98"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.35">
@@ -9958,7 +9958,7 @@
       </c>
       <c r="E24" s="32"/>
       <c r="F24" s="32"/>
-      <c r="G24" s="199"/>
+      <c r="G24" s="151"/>
       <c r="H24" s="98"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.35">
@@ -9971,7 +9971,7 @@
       </c>
       <c r="E25" s="32"/>
       <c r="F25" s="32"/>
-      <c r="G25" s="199"/>
+      <c r="G25" s="151"/>
       <c r="H25" s="98"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.35">
@@ -9984,7 +9984,7 @@
       </c>
       <c r="E26" s="32"/>
       <c r="F26" s="32"/>
-      <c r="G26" s="199"/>
+      <c r="G26" s="151"/>
       <c r="H26" s="98"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.35">
@@ -9993,7 +9993,7 @@
       <c r="D27" s="98"/>
       <c r="E27" s="32"/>
       <c r="F27" s="32"/>
-      <c r="G27" s="200"/>
+      <c r="G27" s="152"/>
       <c r="H27" s="99"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.35">
@@ -10002,7 +10002,7 @@
       <c r="D28" s="98"/>
       <c r="E28" s="32"/>
       <c r="F28" s="32"/>
-      <c r="G28" s="200"/>
+      <c r="G28" s="152"/>
       <c r="H28" s="99"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.35">
@@ -10011,7 +10011,7 @@
       <c r="D29" s="98"/>
       <c r="E29" s="32"/>
       <c r="F29" s="32"/>
-      <c r="G29" s="200"/>
+      <c r="G29" s="152"/>
       <c r="H29" s="99"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.35">
@@ -10091,7 +10091,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -10103,10 +10103,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="188" t="s">
+      <c r="A1" s="216" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="188"/>
+      <c r="B1" s="216"/>
       <c r="C1" s="51"/>
       <c r="D1" s="33"/>
       <c r="E1" s="33"/>

</xml_diff>

<commit_message>
Fixed title link in Checklists
</commit_message>
<xml_diff>
--- a/Checklists/Mobile_App_Security_Checklist-English_1.1.2.xlsx
+++ b/Checklists/Mobile_App_Security_Checklist-English_1.1.2.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21901"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abderrahmane.LAPTOP-NBPOQCF6\Personal\R&amp;D\OWASP\MSTG\owasp-mstg\Checklists\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pec1be7\git\owasp-mstg\Checklists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3788FDF-1673-4488-8C43-1D76F6C726B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" tabRatio="500" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="6" r:id="rId1"/>
@@ -27,10 +26,10 @@
     <definedName name="MASVS_VERSION">Dashboard!$D$11</definedName>
     <definedName name="MSTG_VERSION">Dashboard!$D$13</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -839,6 +838,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 - Rewriting the "Detailed Verification Requirement" columns to match the wording of the MASVS
@@ -865,6 +865,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">n and shifting to github.com instead of gitbook.io
 - Reflecting MASVS/MSTG version in the "Dashboard" worksheet in cell D11 (named range "MASVS_VERSION")
@@ -1301,11 +1302,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
   </numFmts>
-  <fonts count="43" x14ac:knownFonts="1">
+  <fonts count="42" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1430,51 +1431,60 @@
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1501,6 +1511,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1515,13 +1526,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -2282,12 +2286,12 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="35" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="34" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="20" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2324,10 +2328,10 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="35" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="34" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="35" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="34" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -2348,13 +2352,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="34" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="37" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="33" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="36" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2425,7 +2429,7 @@
     <xf numFmtId="0" fontId="19" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="9" applyBorder="1" applyAlignment="1">
@@ -2458,7 +2462,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="18" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2470,7 +2474,7 @@
     <xf numFmtId="49" fontId="18" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="35" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="34" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="18" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2482,16 +2486,16 @@
     <xf numFmtId="49" fontId="18" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="35" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="34" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="18" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="35" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="34" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="37" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="37" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="24" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -2501,14 +2505,14 @@
     <xf numFmtId="0" fontId="18" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="9" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="9" quotePrefix="1" applyAlignment="1">
@@ -2524,10 +2528,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="9" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2535,35 +2539,35 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="9" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="11" borderId="37" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="11" borderId="37" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="37" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="37" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2576,85 +2580,113 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2665,33 +2697,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2704,7 +2709,6 @@
     <xf numFmtId="0" fontId="13" fillId="12" borderId="22" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2719,69 +2723,69 @@
     </xf>
   </cellXfs>
   <cellStyles count="63">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8"/>
-    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="15" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="17" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="19" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="21" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="23" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="25" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="27" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="29" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="31" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="33" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="35" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="37" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="39" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="41" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="43" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="45" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="47" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="49" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="51" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="53" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="55" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="57" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="59" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="62" xr:uid="{34BD3A51-AA52-F643-9E6A-B40E3FA0D56F}"/>
+    <cellStyle name="Normal 3" xfId="62"/>
   </cellStyles>
   <dxfs count="14">
     <dxf>
@@ -2901,7 +2905,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3103,7 +3107,7 @@
                 <a:cs typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="918959216"/>
@@ -3156,7 +3160,7 @@
                 <a:cs typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="918956896"/>
@@ -3203,7 +3207,7 @@
               <a:cs typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3233,7 +3237,7 @@
           <a:cs typeface="Arial"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3247,7 +3251,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3443,7 +3447,7 @@
                 <a:cs typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="920829984"/>
@@ -3496,7 +3500,7 @@
                 <a:cs typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="920827664"/>
@@ -3543,7 +3547,7 @@
               <a:cs typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3573,7 +3577,7 @@
           <a:cs typeface="Arial"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4041,7 +4045,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:D50"/>
   <sheetViews>
@@ -4049,79 +4053,79 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" customWidth="1"/>
+    <col min="1" max="1" width="2.296875" customWidth="1"/>
+    <col min="3" max="3" width="17.19921875" customWidth="1"/>
     <col min="4" max="4" width="92.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="8" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B2" s="180" t="s">
+    <row r="1" spans="2:4" ht="7.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="173" t="s">
         <v>218</v>
       </c>
-      <c r="C2" s="181"/>
-      <c r="D2" s="182"/>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B3" s="183"/>
-      <c r="C3" s="184"/>
-      <c r="D3" s="185"/>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B4" s="183"/>
-      <c r="C4" s="184"/>
-      <c r="D4" s="185"/>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B5" s="183"/>
-      <c r="C5" s="184"/>
-      <c r="D5" s="185"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B6" s="183"/>
-      <c r="C6" s="184"/>
-      <c r="D6" s="185"/>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B7" s="183"/>
-      <c r="C7" s="184"/>
-      <c r="D7" s="185"/>
-    </row>
-    <row r="8" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="186"/>
-      <c r="C8" s="187"/>
-      <c r="D8" s="188"/>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B9" s="189" t="s">
+      <c r="C2" s="174"/>
+      <c r="D2" s="175"/>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="176"/>
+      <c r="C3" s="177"/>
+      <c r="D3" s="178"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="176"/>
+      <c r="C4" s="177"/>
+      <c r="D4" s="178"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="176"/>
+      <c r="C5" s="177"/>
+      <c r="D5" s="178"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="176"/>
+      <c r="C6" s="177"/>
+      <c r="D6" s="178"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="176"/>
+      <c r="C7" s="177"/>
+      <c r="D7" s="178"/>
+    </row>
+    <row r="8" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="179"/>
+      <c r="C8" s="180"/>
+      <c r="D8" s="181"/>
+    </row>
+    <row r="9" spans="2:4" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="B9" s="182" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="176"/>
-      <c r="D9" s="177"/>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C9" s="183"/>
+      <c r="D9" s="184"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B10" s="120" t="s">
         <v>84</v>
       </c>
       <c r="C10" s="121"/>
       <c r="D10" s="122"/>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B11" s="195" t="s">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="190" t="s">
         <v>277</v>
       </c>
-      <c r="C11" s="195"/>
+      <c r="C11" s="190"/>
       <c r="D11" s="123" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B12" s="169" t="s">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="171" t="s">
         <v>279</v>
       </c>
-      <c r="C12" s="179"/>
+      <c r="C12" s="172"/>
       <c r="D12" s="124" t="str">
         <f>HYPERLINK(CONCATENATE(
 "https://github.com/OWASP/owasp-masvs/blob/",
@@ -4130,20 +4134,20 @@
         <v>https://github.com/OWASP/owasp-masvs/blob/1.1.4/Document/</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B13" s="190" t="s">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="185" t="s">
         <v>276</v>
       </c>
-      <c r="C13" s="191"/>
+      <c r="C13" s="186"/>
       <c r="D13" s="12" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B14" s="169" t="s">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="171" t="s">
         <v>220</v>
       </c>
-      <c r="C14" s="179"/>
+      <c r="C14" s="172"/>
       <c r="D14" s="119" t="str">
         <f>HYPERLINK(CONCATENATE(
 "https://github.com/OWASP/owasp-mstg/blob/",
@@ -4152,267 +4156,264 @@
         <v>https://github.com/OWASP/owasp-mstg/blob/1.1.3/Document/</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="192" t="s">
+    <row r="15" spans="2:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="187" t="s">
         <v>262</v>
       </c>
-      <c r="C15" s="193"/>
-      <c r="D15" s="194"/>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B16" s="174" t="s">
+      <c r="C15" s="188"/>
+      <c r="D15" s="189"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="169" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="175"/>
+      <c r="C16" s="170"/>
       <c r="D16" s="12"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B17" s="169" t="s">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="171" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="179"/>
+      <c r="C17" s="172"/>
       <c r="D17" s="12"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B18" s="174" t="s">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="169" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="175"/>
+      <c r="C18" s="170"/>
       <c r="D18" s="12"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B19" s="174" t="s">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="169" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="175"/>
+      <c r="C19" s="170"/>
       <c r="D19" s="12"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B20" s="174" t="s">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="169" t="s">
         <v>134</v>
       </c>
-      <c r="C20" s="175"/>
+      <c r="C20" s="170"/>
       <c r="D20" s="12"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B21" s="174" t="s">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="169" t="s">
         <v>104</v>
       </c>
-      <c r="C21" s="175"/>
+      <c r="C21" s="170"/>
       <c r="D21" s="12" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="174" t="s">
+    <row r="22" spans="2:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="169" t="s">
         <v>106</v>
       </c>
-      <c r="C22" s="175"/>
+      <c r="C22" s="170"/>
       <c r="D22" s="12" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B23" s="176"/>
-      <c r="C23" s="176"/>
-      <c r="D23" s="177"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:4" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="B23" s="183"/>
+      <c r="C23" s="183"/>
+      <c r="D23" s="184"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>97</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" s="4" t="s">
         <v>88</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="12"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B26" s="174" t="s">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B26" s="169" t="s">
         <v>98</v>
       </c>
-      <c r="C26" s="175"/>
+      <c r="C26" s="170"/>
       <c r="D26" s="12"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B27" s="174" t="s">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B27" s="169" t="s">
         <v>99</v>
       </c>
-      <c r="C27" s="175"/>
+      <c r="C27" s="170"/>
       <c r="D27" s="12"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B28" s="174" t="s">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B28" s="169" t="s">
         <v>100</v>
       </c>
-      <c r="C28" s="175"/>
+      <c r="C28" s="170"/>
       <c r="D28" s="12"/>
     </row>
-    <row r="29" spans="2:4" ht="66" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="178" t="s">
+    <row r="29" spans="2:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="195" t="s">
         <v>256</v>
       </c>
-      <c r="C29" s="175"/>
+      <c r="C29" s="170"/>
       <c r="D29" s="12"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B30" s="176"/>
-      <c r="C30" s="176"/>
-      <c r="D30" s="177"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:4" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="B30" s="183"/>
+      <c r="C30" s="183"/>
+      <c r="D30" s="184"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
         <v>101</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" s="48" t="s">
         <v>88</v>
       </c>
       <c r="C32" s="49"/>
       <c r="D32" s="12"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B33" s="174" t="s">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B33" s="169" t="s">
         <v>89</v>
       </c>
-      <c r="C33" s="175"/>
+      <c r="C33" s="170"/>
       <c r="D33" s="12"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B34" s="174" t="s">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B34" s="169" t="s">
         <v>99</v>
       </c>
-      <c r="C34" s="175"/>
+      <c r="C34" s="170"/>
       <c r="D34" s="12"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B35" s="174" t="s">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B35" s="169" t="s">
         <v>100</v>
       </c>
-      <c r="C35" s="175"/>
+      <c r="C35" s="170"/>
       <c r="D35" s="12"/>
     </row>
-    <row r="36" spans="2:4" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="178" t="s">
+    <row r="36" spans="2:4" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="195" t="s">
         <v>257</v>
       </c>
-      <c r="C36" s="175"/>
+      <c r="C36" s="170"/>
       <c r="D36" s="12"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B37" s="176"/>
-      <c r="C37" s="176"/>
-      <c r="D37" s="177"/>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:4" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="B37" s="183"/>
+      <c r="C37" s="183"/>
+      <c r="D37" s="184"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="3"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B39" s="171"/>
-      <c r="C39" s="172"/>
-      <c r="D39" s="173"/>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B40" s="169" t="s">
+    <row r="39" spans="2:4" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="B39" s="191"/>
+      <c r="C39" s="192"/>
+      <c r="D39" s="193"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B40" s="171" t="s">
         <v>91</v>
       </c>
-      <c r="C40" s="170"/>
+      <c r="C40" s="194"/>
       <c r="D40" s="39"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B41" s="169" t="s">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B41" s="171" t="s">
         <v>92</v>
       </c>
-      <c r="C41" s="170"/>
+      <c r="C41" s="194"/>
       <c r="D41" s="39"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B42" s="169" t="s">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B42" s="171" t="s">
         <v>93</v>
       </c>
-      <c r="C42" s="170"/>
+      <c r="C42" s="194"/>
       <c r="D42" s="39"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B43" s="169" t="s">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B43" s="171" t="s">
         <v>94</v>
       </c>
-      <c r="C43" s="170"/>
+      <c r="C43" s="194"/>
       <c r="D43" s="40"/>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B44" s="169" t="s">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B44" s="171" t="s">
         <v>95</v>
       </c>
-      <c r="C44" s="170"/>
+      <c r="C44" s="194"/>
       <c r="D44" s="39"/>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B45" s="171"/>
-      <c r="C45" s="172"/>
-      <c r="D45" s="173"/>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B46" s="169" t="s">
+    <row r="45" spans="2:4" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="B45" s="191"/>
+      <c r="C45" s="192"/>
+      <c r="D45" s="193"/>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B46" s="171" t="s">
         <v>91</v>
       </c>
-      <c r="C46" s="170"/>
+      <c r="C46" s="194"/>
       <c r="D46" s="39"/>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B47" s="169" t="s">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B47" s="171" t="s">
         <v>92</v>
       </c>
-      <c r="C47" s="170"/>
+      <c r="C47" s="194"/>
       <c r="D47" s="39"/>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B48" s="169" t="s">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B48" s="171" t="s">
         <v>93</v>
       </c>
-      <c r="C48" s="170"/>
+      <c r="C48" s="194"/>
       <c r="D48" s="39"/>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B49" s="169" t="s">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B49" s="171" t="s">
         <v>94</v>
       </c>
-      <c r="C49" s="170"/>
+      <c r="C49" s="194"/>
       <c r="D49" s="40"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B50" s="169" t="s">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B50" s="171" t="s">
         <v>95</v>
       </c>
-      <c r="C50" s="170"/>
+      <c r="C50" s="194"/>
       <c r="D50" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B2:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B46:C46"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B39:D39"/>
@@ -4427,16 +4428,19 @@
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B2:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -4445,7 +4449,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:X50"/>
   <sheetViews>
@@ -4453,20 +4457,20 @@
       <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.83203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="1.796875" style="6" customWidth="1"/>
     <col min="2" max="2" width="9.5" style="6" customWidth="1"/>
-    <col min="3" max="3" width="54.83203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="54.796875" style="6" customWidth="1"/>
     <col min="4" max="4" width="6" style="6" customWidth="1"/>
-    <col min="5" max="5" width="4.6640625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="5.83203125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="10.1640625" style="6" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="6"/>
+    <col min="5" max="5" width="4.69921875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="5.796875" style="6" customWidth="1"/>
+    <col min="7" max="7" width="10.19921875" style="6" customWidth="1"/>
+    <col min="8" max="16384" width="8.796875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:24" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:24" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:24" ht="15.6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="7"/>
       <c r="C2" s="22" t="s">
         <v>103</v>
@@ -4475,82 +4479,82 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="2:24" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:24" ht="15" x14ac:dyDescent="0.35">
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="2:24" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="212"/>
-      <c r="C4" s="212"/>
-      <c r="D4" s="212"/>
-      <c r="E4" s="212"/>
-      <c r="F4" s="212"/>
-    </row>
-    <row r="5" spans="2:24" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:24" ht="15" x14ac:dyDescent="0.35">
+      <c r="B4" s="196"/>
+      <c r="C4" s="196"/>
+      <c r="D4" s="196"/>
+      <c r="E4" s="196"/>
+      <c r="F4" s="196"/>
+    </row>
+    <row r="5" spans="2:24" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="20"/>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
       <c r="E5" s="20"/>
       <c r="F5" s="20"/>
     </row>
-    <row r="6" spans="2:24" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:24" ht="19.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
       <c r="F6" s="21"/>
-      <c r="G6" s="196" t="s">
+      <c r="G6" s="206" t="s">
         <v>117</v>
       </c>
-      <c r="H6" s="197"/>
-      <c r="I6" s="198"/>
-      <c r="V6" s="196" t="s">
+      <c r="H6" s="207"/>
+      <c r="I6" s="208"/>
+      <c r="V6" s="206" t="s">
         <v>117</v>
       </c>
-      <c r="W6" s="197"/>
-      <c r="X6" s="198"/>
-    </row>
-    <row r="7" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="W6" s="207"/>
+      <c r="X6" s="208"/>
+    </row>
+    <row r="7" spans="2:24" ht="15.6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
     </row>
-    <row r="8" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:24" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="20"/>
       <c r="C8" s="20"/>
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
-      <c r="G8" s="199">
+      <c r="G8" s="197">
         <f>AVERAGE(G43:G50)*5</f>
         <v>0</v>
       </c>
-      <c r="H8" s="200"/>
-      <c r="I8" s="201"/>
-      <c r="V8" s="199">
+      <c r="H8" s="198"/>
+      <c r="I8" s="199"/>
+      <c r="V8" s="197">
         <f>AVERAGE(K43:K50)*5</f>
         <v>0</v>
       </c>
-      <c r="W8" s="200"/>
-      <c r="X8" s="201"/>
-    </row>
-    <row r="9" spans="2:24" ht="91" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="W8" s="198"/>
+      <c r="X8" s="199"/>
+    </row>
+    <row r="9" spans="2:24" ht="91.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
-      <c r="G9" s="202"/>
-      <c r="H9" s="203"/>
-      <c r="I9" s="204"/>
-      <c r="V9" s="202"/>
-      <c r="W9" s="203"/>
-      <c r="X9" s="204"/>
+      <c r="G9" s="200"/>
+      <c r="H9" s="201"/>
+      <c r="I9" s="202"/>
+      <c r="V9" s="200"/>
+      <c r="W9" s="201"/>
+      <c r="X9" s="202"/>
     </row>
     <row r="10" spans="2:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="13"/>
@@ -4558,12 +4562,12 @@
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="202"/>
-      <c r="H10" s="203"/>
-      <c r="I10" s="204"/>
-      <c r="V10" s="202"/>
-      <c r="W10" s="203"/>
-      <c r="X10" s="204"/>
+      <c r="G10" s="200"/>
+      <c r="H10" s="201"/>
+      <c r="I10" s="202"/>
+      <c r="V10" s="200"/>
+      <c r="W10" s="201"/>
+      <c r="X10" s="202"/>
     </row>
     <row r="11" spans="2:24" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="13"/>
@@ -4571,113 +4575,113 @@
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="205"/>
-      <c r="H11" s="206"/>
-      <c r="I11" s="207"/>
-      <c r="V11" s="205"/>
-      <c r="W11" s="206"/>
-      <c r="X11" s="207"/>
-    </row>
-    <row r="12" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="208"/>
-      <c r="C12" s="208"/>
-      <c r="D12" s="208"/>
-      <c r="E12" s="208"/>
-      <c r="F12" s="208"/>
-    </row>
-    <row r="13" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="G11" s="203"/>
+      <c r="H11" s="204"/>
+      <c r="I11" s="205"/>
+      <c r="V11" s="203"/>
+      <c r="W11" s="204"/>
+      <c r="X11" s="205"/>
+    </row>
+    <row r="12" spans="2:24" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="209"/>
+      <c r="C12" s="209"/>
+      <c r="D12" s="209"/>
+      <c r="E12" s="209"/>
+      <c r="F12" s="209"/>
+    </row>
+    <row r="13" spans="2:24" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
     </row>
-    <row r="14" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:24" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
       <c r="F14" s="16"/>
     </row>
-    <row r="15" spans="2:24" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:24" ht="15" x14ac:dyDescent="0.35">
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
     </row>
-    <row r="16" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="208"/>
-      <c r="C16" s="208"/>
-      <c r="D16" s="208"/>
-      <c r="E16" s="208"/>
-      <c r="F16" s="208"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:24" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="209"/>
+      <c r="C16" s="209"/>
+      <c r="D16" s="209"/>
+      <c r="E16" s="209"/>
+      <c r="F16" s="209"/>
+    </row>
+    <row r="17" spans="2:6" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
       <c r="F18" s="16"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C23" s="18"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C24" s="18"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C25" s="18"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C26" s="18"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C27" s="18"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C28" s="18"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C29" s="18"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C30" s="18"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C31" s="18"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C32" s="18"/>
     </row>
-    <row r="35" spans="3:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="3:11" ht="14.5" x14ac:dyDescent="0.3">
-      <c r="D41" s="209" t="s">
+    <row r="35" spans="3:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="3:11" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="D41" s="210" t="s">
         <v>115</v>
       </c>
-      <c r="E41" s="210"/>
-      <c r="F41" s="210"/>
-      <c r="G41" s="211"/>
-      <c r="H41" s="209" t="s">
+      <c r="E41" s="211"/>
+      <c r="F41" s="211"/>
+      <c r="G41" s="212"/>
+      <c r="H41" s="210" t="s">
         <v>116</v>
       </c>
-      <c r="I41" s="210"/>
-      <c r="J41" s="210"/>
-      <c r="K41" s="211"/>
-    </row>
-    <row r="42" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="I41" s="211"/>
+      <c r="J41" s="211"/>
+      <c r="K41" s="212"/>
+    </row>
+    <row r="42" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D42" s="17" t="s">
         <v>111</v>
       </c>
@@ -4703,7 +4707,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="43" spans="3:11" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:11" ht="14.4" x14ac:dyDescent="0.25">
       <c r="C43" s="11" t="s">
         <v>121</v>
       </c>
@@ -4740,7 +4744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="3:11" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:11" ht="14.4" x14ac:dyDescent="0.25">
       <c r="C44" s="11" t="s">
         <v>122</v>
       </c>
@@ -4777,7 +4781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="3:11" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:11" ht="14.4" x14ac:dyDescent="0.25">
       <c r="C45" s="11" t="s">
         <v>123</v>
       </c>
@@ -4814,7 +4818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="3:11" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:11" ht="14.4" x14ac:dyDescent="0.25">
       <c r="C46" s="11" t="s">
         <v>124</v>
       </c>
@@ -4851,7 +4855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="3:11" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:11" ht="14.4" x14ac:dyDescent="0.25">
       <c r="C47" s="11" t="s">
         <v>125</v>
       </c>
@@ -4888,7 +4892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="3:11" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:11" ht="14.4" x14ac:dyDescent="0.25">
       <c r="C48" s="11" t="s">
         <v>148</v>
       </c>
@@ -4925,7 +4929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="3:11" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:11" ht="14.4" x14ac:dyDescent="0.25">
       <c r="C49" s="11" t="s">
         <v>126</v>
       </c>
@@ -4962,7 +4966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="3:11" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:11" ht="14.4" x14ac:dyDescent="0.25">
       <c r="C50" s="11" t="s">
         <v>127</v>
       </c>
@@ -5001,15 +5005,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="D41:G41"/>
+    <mergeCell ref="H41:K41"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="G8:I11"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="V6:X6"/>
     <mergeCell ref="V8:X11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="D41:G41"/>
-    <mergeCell ref="H41:K41"/>
   </mergeCells>
   <conditionalFormatting sqref="F14">
     <cfRule type="iconSet" priority="3">
@@ -5046,32 +5050,32 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:M85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="62" zoomScaleNormal="62" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="E19" zoomScale="62" zoomScaleNormal="62" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.83203125" style="72" customWidth="1"/>
+    <col min="1" max="1" width="1.796875" style="72" customWidth="1"/>
     <col min="2" max="2" width="8" style="81" customWidth="1"/>
-    <col min="3" max="3" width="17.9140625" style="81" customWidth="1"/>
-    <col min="4" max="4" width="97.33203125" style="103" customWidth="1"/>
-    <col min="5" max="6" width="6.6640625" style="72" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.83203125" style="72" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="101.58203125" customWidth="1"/>
-    <col min="9" max="9" width="83.58203125" customWidth="1"/>
-    <col min="10" max="10" width="73.4140625" customWidth="1"/>
-    <col min="11" max="11" width="30.83203125" style="103" customWidth="1"/>
+    <col min="3" max="3" width="17.8984375" style="81" customWidth="1"/>
+    <col min="4" max="4" width="97.296875" style="103" customWidth="1"/>
+    <col min="5" max="6" width="6.69921875" style="72" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.796875" style="72" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="101.59765625" customWidth="1"/>
+    <col min="9" max="9" width="83.59765625" customWidth="1"/>
+    <col min="10" max="10" width="73.3984375" customWidth="1"/>
+    <col min="11" max="11" width="30.796875" style="103" customWidth="1"/>
     <col min="12" max="12" width="11" style="72"/>
-    <col min="13" max="14" width="10.83203125" style="72" customWidth="1"/>
+    <col min="13" max="14" width="10.796875" style="72" customWidth="1"/>
     <col min="15" max="16384" width="11" style="72"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:11" ht="18" x14ac:dyDescent="0.3">
       <c r="B1" s="213" t="s">
         <v>118</v>
       </c>
@@ -5085,7 +5089,7 @@
       <c r="J1" s="213"/>
       <c r="K1" s="213"/>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B2" s="73"/>
       <c r="C2" s="73"/>
       <c r="D2" s="101"/>
@@ -5097,7 +5101,7 @@
       <c r="J2" s="141"/>
       <c r="K2" s="101"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" s="66" t="s">
         <v>0</v>
       </c>
@@ -5125,7 +5129,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="67" t="s">
         <v>4</v>
       </c>
@@ -5141,7 +5145,7 @@
       <c r="J4" s="94"/>
       <c r="K4" s="114"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" s="57" t="s">
         <v>6</v>
       </c>
@@ -5175,7 +5179,7 @@
       <c r="J5" s="154"/>
       <c r="K5" s="111"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="70" t="s">
         <v>232</v>
       </c>
@@ -5206,7 +5210,7 @@
       <c r="J6" s="153"/>
       <c r="K6" s="111"/>
     </row>
-    <row r="7" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="70" t="s">
         <v>231</v>
       </c>
@@ -5234,7 +5238,7 @@
       <c r="J7" s="154"/>
       <c r="K7" s="111"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="70" t="s">
         <v>230</v>
       </c>
@@ -5262,7 +5266,7 @@
       <c r="J8" s="154"/>
       <c r="K8" s="111"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="70" t="s">
         <v>229</v>
       </c>
@@ -5290,7 +5294,7 @@
       <c r="J9" s="154"/>
       <c r="K9" s="111"/>
     </row>
-    <row r="10" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="70" t="s">
         <v>228</v>
       </c>
@@ -5318,7 +5322,7 @@
       <c r="J10" s="154"/>
       <c r="K10" s="111"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" s="57" t="s">
         <v>8</v>
       </c>
@@ -5355,7 +5359,7 @@
       </c>
       <c r="K11" s="111"/>
     </row>
-    <row r="12" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="70" t="s">
         <v>227</v>
       </c>
@@ -5383,7 +5387,7 @@
       <c r="J12" s="154"/>
       <c r="K12" s="111"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" s="70" t="s">
         <v>226</v>
       </c>
@@ -5411,7 +5415,7 @@
       <c r="J13" s="154"/>
       <c r="K13" s="111"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" s="58" t="s">
         <v>9</v>
       </c>
@@ -5439,7 +5443,7 @@
       <c r="J14" s="154"/>
       <c r="K14" s="111"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15" s="56" t="s">
         <v>10</v>
       </c>
@@ -5455,7 +5459,7 @@
       <c r="J15" s="155"/>
       <c r="K15" s="110"/>
     </row>
-    <row r="16" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="68" t="s">
         <v>11</v>
       </c>
@@ -5483,7 +5487,7 @@
       <c r="J16" s="154"/>
       <c r="K16" s="111"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" s="68" t="s">
         <v>48</v>
       </c>
@@ -5504,7 +5508,7 @@
       <c r="J17" s="154"/>
       <c r="K17" s="115"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" s="68" t="s">
         <v>49</v>
       </c>
@@ -5529,7 +5533,7 @@
       <c r="J18" s="154"/>
       <c r="K18" s="111"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" s="68" t="s">
         <v>12</v>
       </c>
@@ -5554,7 +5558,7 @@
       <c r="J19" s="154"/>
       <c r="K19" s="111"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" s="68" t="s">
         <v>50</v>
       </c>
@@ -5579,7 +5583,7 @@
       <c r="J20" s="154"/>
       <c r="K20" s="111"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" s="68" t="s">
         <v>13</v>
       </c>
@@ -5604,7 +5608,7 @@
       <c r="J21" s="154"/>
       <c r="K21" s="111"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" s="68" t="s">
         <v>14</v>
       </c>
@@ -5629,7 +5633,7 @@
       <c r="J22" s="154"/>
       <c r="K22" s="111"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" s="68" t="s">
         <v>15</v>
       </c>
@@ -5654,7 +5658,7 @@
       <c r="J23" s="154"/>
       <c r="K23" s="111"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B24" s="68" t="s">
         <v>16</v>
       </c>
@@ -5679,7 +5683,7 @@
       <c r="J24" s="154"/>
       <c r="K24" s="111"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B25" s="68" t="s">
         <v>51</v>
       </c>
@@ -5704,7 +5708,7 @@
       <c r="J25" s="154"/>
       <c r="K25" s="111"/>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B26" s="68" t="s">
         <v>52</v>
       </c>
@@ -5732,7 +5736,7 @@
       <c r="J26" s="154"/>
       <c r="K26" s="111"/>
     </row>
-    <row r="27" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B27" s="68" t="s">
         <v>17</v>
       </c>
@@ -5757,7 +5761,7 @@
       <c r="J27" s="154"/>
       <c r="K27" s="111"/>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B28" s="56" t="s">
         <v>18</v>
       </c>
@@ -5773,7 +5777,7 @@
       <c r="J28" s="155"/>
       <c r="K28" s="110"/>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B29" s="68" t="s">
         <v>19</v>
       </c>
@@ -5801,7 +5805,7 @@
       <c r="J29" s="154"/>
       <c r="K29" s="111"/>
     </row>
-    <row r="30" spans="2:11" ht="31" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B30" s="68" t="s">
         <v>20</v>
       </c>
@@ -5829,7 +5833,7 @@
       <c r="J30" s="154"/>
       <c r="K30" s="111"/>
     </row>
-    <row r="31" spans="2:11" ht="31" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B31" s="68" t="s">
         <v>21</v>
       </c>
@@ -5857,7 +5861,7 @@
       <c r="J31" s="154"/>
       <c r="K31" s="111"/>
     </row>
-    <row r="32" spans="2:11" ht="31" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B32" s="68" t="s">
         <v>22</v>
       </c>
@@ -5885,7 +5889,7 @@
       <c r="J32" s="154"/>
       <c r="K32" s="111"/>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B33" s="68" t="s">
         <v>23</v>
       </c>
@@ -5910,7 +5914,7 @@
       <c r="J33" s="154"/>
       <c r="K33" s="111"/>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B34" s="68" t="s">
         <v>24</v>
       </c>
@@ -5935,7 +5939,7 @@
       <c r="J34" s="154"/>
       <c r="K34" s="111"/>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B35" s="56" t="s">
         <v>25</v>
       </c>
@@ -5951,7 +5955,7 @@
       <c r="J35" s="155"/>
       <c r="K35" s="110"/>
     </row>
-    <row r="36" spans="2:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B36" s="68" t="s">
         <v>26</v>
       </c>
@@ -5982,7 +5986,7 @@
       </c>
       <c r="K36" s="111"/>
     </row>
-    <row r="37" spans="2:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B37" s="68" t="s">
         <v>55</v>
       </c>
@@ -6007,7 +6011,7 @@
       <c r="J37" s="154"/>
       <c r="K37" s="111"/>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B38" s="68" t="s">
         <v>56</v>
       </c>
@@ -6036,7 +6040,7 @@
       <c r="K38" s="111"/>
       <c r="M38" s="38"/>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B39" s="68" t="s">
         <v>27</v>
       </c>
@@ -6058,7 +6062,7 @@
       <c r="K39" s="111"/>
       <c r="M39" s="38"/>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B40" s="68" t="s">
         <v>28</v>
       </c>
@@ -6083,7 +6087,7 @@
       <c r="J40" s="154"/>
       <c r="K40" s="111"/>
     </row>
-    <row r="41" spans="2:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B41" s="68" t="s">
         <v>57</v>
       </c>
@@ -6111,7 +6115,7 @@
       <c r="J41" s="154"/>
       <c r="K41" s="111"/>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B42" s="68" t="s">
         <v>58</v>
       </c>
@@ -6136,7 +6140,7 @@
       <c r="J42" s="156"/>
       <c r="K42" s="113"/>
     </row>
-    <row r="43" spans="2:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B43" s="68" t="s">
         <v>29</v>
       </c>
@@ -6161,7 +6165,7 @@
       <c r="J43" s="154"/>
       <c r="K43" s="111"/>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B44" s="68" t="s">
         <v>30</v>
       </c>
@@ -6186,7 +6190,7 @@
       <c r="J44" s="154"/>
       <c r="K44" s="111"/>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B45" s="68" t="s">
         <v>31</v>
       </c>
@@ -6211,7 +6215,7 @@
       <c r="J45" s="154"/>
       <c r="K45" s="111"/>
     </row>
-    <row r="46" spans="2:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B46" s="68" t="s">
         <v>150</v>
       </c>
@@ -6236,7 +6240,7 @@
       <c r="J46" s="154"/>
       <c r="K46" s="111"/>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B47" s="56" t="s">
         <v>32</v>
       </c>
@@ -6252,7 +6256,7 @@
       <c r="J47" s="155"/>
       <c r="K47" s="110"/>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B48" s="68" t="s">
         <v>33</v>
       </c>
@@ -6277,7 +6281,7 @@
       <c r="J48" s="154"/>
       <c r="K48" s="111"/>
     </row>
-    <row r="49" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B49" s="68" t="s">
         <v>60</v>
       </c>
@@ -6302,7 +6306,7 @@
       <c r="J49" s="154"/>
       <c r="K49" s="111"/>
     </row>
-    <row r="50" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B50" s="68" t="s">
         <v>34</v>
       </c>
@@ -6327,7 +6331,7 @@
       <c r="J50" s="153"/>
       <c r="K50" s="116"/>
     </row>
-    <row r="51" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B51" s="68" t="s">
         <v>61</v>
       </c>
@@ -6349,13 +6353,13 @@
         <v>Testing Custom Certificate Stores and Certificate Pinning (MSTG-NETWORK-4)</v>
       </c>
       <c r="I51" s="147" t="str">
-        <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05g-Testing-Network-Communication.md#testing-the-network-security-configuration-settings-mstg-network-4"),"Testing the Network Security Configuration settings (MSTG-NETWORK-4)")</f>
-        <v>Testing the Network Security Configuration settings (MSTG-NETWORK-4)</v>
+        <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05g-Testing-Network-Communication.md#testing-the-network-security-configuration-settings-mstg-network-4"),"Testing the Network Security Configuration Settings (MSTG-NETWORK-4)")</f>
+        <v>Testing the Network Security Configuration Settings (MSTG-NETWORK-4)</v>
       </c>
       <c r="J51" s="154"/>
       <c r="K51" s="111"/>
     </row>
-    <row r="52" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B52" s="68" t="s">
         <v>35</v>
       </c>
@@ -6380,7 +6384,7 @@
       <c r="J52" s="154"/>
       <c r="K52" s="111"/>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B53" s="71" t="s">
         <v>225</v>
       </c>
@@ -6405,7 +6409,7 @@
       <c r="J53" s="154"/>
       <c r="K53" s="111"/>
     </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B54" s="56" t="s">
         <v>36</v>
       </c>
@@ -6421,7 +6425,7 @@
       <c r="J54" s="155"/>
       <c r="K54" s="110"/>
     </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B55" s="68" t="s">
         <v>62</v>
       </c>
@@ -6446,7 +6450,7 @@
       <c r="J55" s="154"/>
       <c r="K55" s="111"/>
     </row>
-    <row r="56" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B56" s="68" t="s">
         <v>63</v>
       </c>
@@ -6474,7 +6478,7 @@
       <c r="J56" s="154"/>
       <c r="K56" s="111"/>
     </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B57" s="68" t="s">
         <v>64</v>
       </c>
@@ -6499,7 +6503,7 @@
       <c r="J57" s="154"/>
       <c r="K57" s="111"/>
     </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B58" s="68" t="s">
         <v>65</v>
       </c>
@@ -6524,7 +6528,7 @@
       <c r="J58" s="154"/>
       <c r="K58" s="111"/>
     </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B59" s="68" t="s">
         <v>66</v>
       </c>
@@ -6549,7 +6553,7 @@
       <c r="J59" s="154"/>
       <c r="K59" s="111"/>
     </row>
-    <row r="60" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B60" s="68" t="s">
         <v>67</v>
       </c>
@@ -6574,7 +6578,7 @@
       <c r="J60" s="154"/>
       <c r="K60" s="111"/>
     </row>
-    <row r="61" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B61" s="71" t="s">
         <v>224</v>
       </c>
@@ -6599,7 +6603,7 @@
       <c r="J61" s="154"/>
       <c r="K61" s="111"/>
     </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B62" s="71" t="s">
         <v>223</v>
       </c>
@@ -6624,7 +6628,7 @@
       <c r="J62" s="154"/>
       <c r="K62" s="111"/>
     </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B63" s="56" t="s">
         <v>37</v>
       </c>
@@ -6640,7 +6644,7 @@
       <c r="J63" s="155"/>
       <c r="K63" s="110"/>
     </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B64" s="68" t="s">
         <v>68</v>
       </c>
@@ -6665,7 +6669,7 @@
       <c r="J64" s="154"/>
       <c r="K64" s="111"/>
     </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B65" s="68" t="s">
         <v>38</v>
       </c>
@@ -6690,7 +6694,7 @@
       <c r="J65" s="154"/>
       <c r="K65" s="111"/>
     </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B66" s="68" t="s">
         <v>69</v>
       </c>
@@ -6715,7 +6719,7 @@
       <c r="J66" s="154"/>
       <c r="K66" s="111"/>
     </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B67" s="68" t="s">
         <v>70</v>
       </c>
@@ -6740,7 +6744,7 @@
       <c r="J67" s="154"/>
       <c r="K67" s="111"/>
     </row>
-    <row r="68" spans="2:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B68" s="68" t="s">
         <v>71</v>
       </c>
@@ -6765,7 +6769,7 @@
       <c r="J68" s="154"/>
       <c r="K68" s="111"/>
     </row>
-    <row r="69" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B69" s="68" t="s">
         <v>39</v>
       </c>
@@ -6790,7 +6794,7 @@
       <c r="J69" s="154"/>
       <c r="K69" s="111"/>
     </row>
-    <row r="70" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B70" s="68" t="s">
         <v>40</v>
       </c>
@@ -6815,7 +6819,7 @@
       <c r="J70" s="154"/>
       <c r="K70" s="111"/>
     </row>
-    <row r="71" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B71" s="68" t="s">
         <v>41</v>
       </c>
@@ -6841,7 +6845,7 @@
       <c r="K71" s="117"/>
       <c r="L71" s="75"/>
     </row>
-    <row r="72" spans="2:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B72" s="68" t="s">
         <v>152</v>
       </c>
@@ -6866,7 +6870,7 @@
       <c r="J72" s="154"/>
       <c r="K72" s="111"/>
     </row>
-    <row r="73" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B73" s="59"/>
       <c r="C73" s="135"/>
       <c r="D73" s="97"/>
@@ -6878,7 +6882,7 @@
       <c r="J73" s="157"/>
       <c r="K73" s="112"/>
     </row>
-    <row r="74" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B74" s="76"/>
       <c r="C74" s="76"/>
       <c r="D74" s="95"/>
@@ -6890,7 +6894,7 @@
       <c r="J74" s="151"/>
       <c r="K74" s="95"/>
     </row>
-    <row r="75" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B75" s="76"/>
       <c r="C75" s="76"/>
       <c r="D75" s="106"/>
@@ -6902,7 +6906,7 @@
       <c r="J75" s="151"/>
       <c r="K75" s="95"/>
     </row>
-    <row r="76" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B76" s="76"/>
       <c r="C76" s="76"/>
       <c r="D76" s="95"/>
@@ -6914,7 +6918,7 @@
       <c r="J76" s="151"/>
       <c r="K76" s="95"/>
     </row>
-    <row r="77" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B77" s="78" t="s">
         <v>77</v>
       </c>
@@ -6928,7 +6932,7 @@
       <c r="J77" s="151"/>
       <c r="K77" s="95"/>
     </row>
-    <row r="78" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B78" s="62" t="s">
         <v>78</v>
       </c>
@@ -6944,7 +6948,7 @@
       <c r="J78" s="151"/>
       <c r="K78" s="95"/>
     </row>
-    <row r="79" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B79" s="63" t="s">
         <v>109</v>
       </c>
@@ -6960,7 +6964,7 @@
       <c r="J79" s="151"/>
       <c r="K79" s="95"/>
     </row>
-    <row r="80" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B80" s="63" t="s">
         <v>110</v>
       </c>
@@ -6976,7 +6980,7 @@
       <c r="J80" s="151"/>
       <c r="K80" s="95"/>
     </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B81" s="63" t="s">
         <v>81</v>
       </c>
@@ -6992,7 +6996,7 @@
       <c r="J81" s="151"/>
       <c r="K81" s="95"/>
     </row>
-    <row r="82" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B82" s="76"/>
       <c r="C82" s="76"/>
       <c r="D82" s="95"/>
@@ -7004,7 +7008,7 @@
       <c r="J82" s="152"/>
       <c r="K82" s="102"/>
     </row>
-    <row r="83" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B83" s="76"/>
       <c r="C83" s="76"/>
       <c r="D83" s="95"/>
@@ -7016,7 +7020,7 @@
       <c r="J83" s="152"/>
       <c r="K83" s="102"/>
     </row>
-    <row r="84" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B84" s="76"/>
       <c r="C84" s="76"/>
       <c r="D84" s="95"/>
@@ -7028,7 +7032,7 @@
       <c r="J84" s="152"/>
       <c r="K84" s="102"/>
     </row>
-    <row r="85" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B85" s="80"/>
       <c r="C85" s="80"/>
       <c r="D85" s="102"/>
@@ -7046,10 +7050,10 @@
     <mergeCell ref="H3:I3"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G74:G1048576 I74:K1048576" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G74:G1048576 I74:K1048576">
       <formula1>"Yes,No,N/A"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G29:G34 G36:G46 G64:G72 G5:G14 G55:G62 G16:G27 G48:G53" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G29:G34 G36:G46 G64:G72 G5:G14 G55:G62 G16:G27 G48:G53">
       <formula1>"Pass,Fail,N/A"</formula1>
     </dataValidation>
   </dataValidations>
@@ -7059,7 +7063,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="B1:H29"/>
   <sheetViews>
@@ -7067,20 +7071,20 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.83203125" style="72" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" style="81" customWidth="1"/>
-    <col min="3" max="3" width="16.9140625" style="81" customWidth="1"/>
-    <col min="4" max="4" width="97.33203125" style="103" customWidth="1"/>
+    <col min="1" max="1" width="1.796875" style="72" customWidth="1"/>
+    <col min="2" max="2" width="7.296875" style="81" customWidth="1"/>
+    <col min="3" max="3" width="16.8984375" style="81" customWidth="1"/>
+    <col min="4" max="4" width="97.296875" style="103" customWidth="1"/>
     <col min="5" max="5" width="3" style="72" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.83203125" style="72" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="69.25" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" style="103" customWidth="1"/>
+    <col min="6" max="6" width="5.796875" style="72" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="69.19921875" customWidth="1"/>
+    <col min="8" max="8" width="30.69921875" style="103" customWidth="1"/>
     <col min="9" max="16384" width="11" style="72"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="82" t="s">
         <v>131</v>
       </c>
@@ -7091,7 +7095,7 @@
       <c r="G1" s="152"/>
       <c r="H1" s="102"/>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="80"/>
       <c r="C2" s="80"/>
       <c r="D2" s="102"/>
@@ -7100,7 +7104,7 @@
       <c r="G2" s="152"/>
       <c r="H2" s="102"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="55" t="s">
         <v>0</v>
       </c>
@@ -7123,7 +7127,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="56"/>
       <c r="C4" s="132"/>
       <c r="D4" s="96" t="s">
@@ -7134,7 +7138,7 @@
       <c r="G4" s="159"/>
       <c r="H4" s="110"/>
     </row>
-    <row r="5" spans="2:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="70" t="s">
         <v>233</v>
       </c>
@@ -7156,7 +7160,7 @@
       </c>
       <c r="H5" s="111"/>
     </row>
-    <row r="6" spans="2:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B6" s="70" t="s">
         <v>234</v>
       </c>
@@ -7178,7 +7182,7 @@
       </c>
       <c r="H6" s="111"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="70" t="s">
         <v>235</v>
       </c>
@@ -7200,7 +7204,7 @@
       </c>
       <c r="H7" s="111"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="70" t="s">
         <v>236</v>
       </c>
@@ -7222,7 +7226,7 @@
       </c>
       <c r="H8" s="111"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="70" t="s">
         <v>237</v>
       </c>
@@ -7244,7 +7248,7 @@
       </c>
       <c r="H9" s="111"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="70" t="s">
         <v>238</v>
       </c>
@@ -7266,7 +7270,7 @@
       </c>
       <c r="H10" s="111"/>
     </row>
-    <row r="11" spans="2:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="70" t="s">
         <v>239</v>
       </c>
@@ -7287,7 +7291,7 @@
       </c>
       <c r="H11" s="111"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="70" t="s">
         <v>240</v>
       </c>
@@ -7308,7 +7312,7 @@
       </c>
       <c r="H12" s="111"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="70" t="s">
         <v>154</v>
       </c>
@@ -7330,7 +7334,7 @@
       </c>
       <c r="H13" s="111"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="56"/>
       <c r="C14" s="132"/>
       <c r="D14" s="96" t="s">
@@ -7341,7 +7345,7 @@
       <c r="G14" s="159"/>
       <c r="H14" s="110"/>
     </row>
-    <row r="15" spans="2:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="58" t="s">
         <v>73</v>
       </c>
@@ -7363,7 +7367,7 @@
       </c>
       <c r="H15" s="111"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="56"/>
       <c r="C16" s="132"/>
       <c r="D16" s="96" t="s">
@@ -7374,7 +7378,7 @@
       <c r="G16" s="159"/>
       <c r="H16" s="110"/>
     </row>
-    <row r="17" spans="2:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B17" s="70" t="s">
         <v>241</v>
       </c>
@@ -7396,7 +7400,7 @@
       </c>
       <c r="H17" s="111"/>
     </row>
-    <row r="18" spans="2:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B18" s="70" t="s">
         <v>242</v>
       </c>
@@ -7417,7 +7421,7 @@
       </c>
       <c r="H18" s="111"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="59"/>
       <c r="C19" s="135"/>
       <c r="D19" s="97"/>
@@ -7426,7 +7430,7 @@
       <c r="G19" s="164"/>
       <c r="H19" s="112"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="76"/>
       <c r="C20" s="76"/>
       <c r="D20" s="95"/>
@@ -7435,7 +7439,7 @@
       <c r="G20" s="151"/>
       <c r="H20" s="95"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="76"/>
       <c r="C21" s="76"/>
       <c r="D21" s="95"/>
@@ -7444,7 +7448,7 @@
       <c r="G21" s="151"/>
       <c r="H21" s="95"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="78" t="s">
         <v>77</v>
       </c>
@@ -7455,7 +7459,7 @@
       <c r="G22" s="151"/>
       <c r="H22" s="95"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="62" t="s">
         <v>78</v>
       </c>
@@ -7468,7 +7472,7 @@
       <c r="G23" s="151"/>
       <c r="H23" s="95"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="63" t="s">
         <v>109</v>
       </c>
@@ -7481,7 +7485,7 @@
       <c r="G24" s="151"/>
       <c r="H24" s="95"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" s="63" t="s">
         <v>110</v>
       </c>
@@ -7494,7 +7498,7 @@
       <c r="G25" s="151"/>
       <c r="H25" s="95"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" s="63" t="s">
         <v>81</v>
       </c>
@@ -7507,7 +7511,7 @@
       <c r="G26" s="151"/>
       <c r="H26" s="95"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B27" s="80"/>
       <c r="C27" s="80"/>
       <c r="D27" s="102"/>
@@ -7516,7 +7520,7 @@
       <c r="G27" s="152"/>
       <c r="H27" s="102"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B28" s="80"/>
       <c r="C28" s="80"/>
       <c r="D28" s="102"/>
@@ -7525,7 +7529,7 @@
       <c r="G28" s="152"/>
       <c r="H28" s="102"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B29" s="80"/>
       <c r="C29" s="80"/>
       <c r="D29" s="102"/>
@@ -7536,7 +7540,7 @@
     </row>
   </sheetData>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F17:F18 F15 F5:F13" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F17:F18 F15 F5:F13">
       <formula1>"Pass,Fail,N/A"</formula1>
     </dataValidation>
   </dataValidations>
@@ -7546,7 +7550,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B1:M85"/>
   <sheetViews>
@@ -7554,21 +7558,21 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.83203125" customWidth="1"/>
+    <col min="1" max="1" width="1.796875" customWidth="1"/>
     <col min="2" max="2" width="8" style="54" customWidth="1"/>
-    <col min="3" max="3" width="15.58203125" style="54" customWidth="1"/>
-    <col min="4" max="4" width="97.33203125" style="100" customWidth="1"/>
-    <col min="5" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="91.58203125" customWidth="1"/>
-    <col min="9" max="10" width="75.4140625" customWidth="1"/>
-    <col min="11" max="11" width="30.83203125" style="100" customWidth="1"/>
-    <col min="13" max="14" width="10.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.59765625" style="54" customWidth="1"/>
+    <col min="4" max="4" width="97.296875" style="100" customWidth="1"/>
+    <col min="5" max="6" width="6.69921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="91.59765625" customWidth="1"/>
+    <col min="9" max="10" width="75.3984375" customWidth="1"/>
+    <col min="11" max="11" width="30.796875" style="100" customWidth="1"/>
+    <col min="13" max="14" width="10.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="64" t="s">
         <v>132</v>
       </c>
@@ -7582,7 +7586,7 @@
       <c r="J1" s="101"/>
       <c r="K1" s="93"/>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B2" s="65"/>
       <c r="C2" s="65"/>
       <c r="D2" s="93"/>
@@ -7594,7 +7598,7 @@
       <c r="J2" s="141"/>
       <c r="K2" s="93"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" s="66" t="s">
         <v>0</v>
       </c>
@@ -7622,7 +7626,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="67" t="s">
         <v>4</v>
       </c>
@@ -7638,7 +7642,7 @@
       <c r="J4" s="94"/>
       <c r="K4" s="114"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" s="57" t="s">
         <v>6</v>
       </c>
@@ -7666,7 +7670,7 @@
       <c r="J5" s="154"/>
       <c r="K5" s="111"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="57" t="s">
         <v>232</v>
       </c>
@@ -7697,7 +7701,7 @@
       <c r="J6" s="147"/>
       <c r="K6" s="111"/>
     </row>
-    <row r="7" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="57" t="s">
         <v>231</v>
       </c>
@@ -7725,7 +7729,7 @@
       <c r="J7" s="154"/>
       <c r="K7" s="111"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="57" t="s">
         <v>230</v>
       </c>
@@ -7753,7 +7757,7 @@
       <c r="J8" s="154"/>
       <c r="K8" s="111"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="57" t="s">
         <v>229</v>
       </c>
@@ -7781,7 +7785,7 @@
       <c r="J9" s="154"/>
       <c r="K9" s="111"/>
     </row>
-    <row r="10" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="57" t="s">
         <v>228</v>
       </c>
@@ -7809,7 +7813,7 @@
       <c r="J10" s="154"/>
       <c r="K10" s="111"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" s="57" t="s">
         <v>8</v>
       </c>
@@ -7843,7 +7847,7 @@
       <c r="J11" s="153"/>
       <c r="K11" s="111"/>
     </row>
-    <row r="12" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="57" t="s">
         <v>227</v>
       </c>
@@ -7871,7 +7875,7 @@
       <c r="J12" s="154"/>
       <c r="K12" s="111"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" s="57" t="s">
         <v>226</v>
       </c>
@@ -7899,7 +7903,7 @@
       <c r="J13" s="154"/>
       <c r="K13" s="111"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" s="57" t="s">
         <v>9</v>
       </c>
@@ -7927,7 +7931,7 @@
       <c r="J14" s="154"/>
       <c r="K14" s="111"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15" s="56" t="s">
         <v>10</v>
       </c>
@@ -7943,7 +7947,7 @@
       <c r="J15" s="155"/>
       <c r="K15" s="110"/>
     </row>
-    <row r="16" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="68" t="s">
         <v>11</v>
       </c>
@@ -7968,7 +7972,7 @@
       <c r="J16" s="154"/>
       <c r="K16" s="111"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="68" t="s">
         <v>48</v>
       </c>
@@ -7989,7 +7993,7 @@
       <c r="J17" s="154"/>
       <c r="K17" s="111"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="68" t="s">
         <v>49</v>
       </c>
@@ -8014,7 +8018,7 @@
       <c r="J18" s="154"/>
       <c r="K18" s="111"/>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" s="68" t="s">
         <v>12</v>
       </c>
@@ -8039,7 +8043,7 @@
       <c r="J19" s="154"/>
       <c r="K19" s="111"/>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" s="68" t="s">
         <v>50</v>
       </c>
@@ -8064,7 +8068,7 @@
       <c r="J20" s="154"/>
       <c r="K20" s="111"/>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21" s="68" t="s">
         <v>13</v>
       </c>
@@ -8089,7 +8093,7 @@
       <c r="J21" s="154"/>
       <c r="K21" s="111"/>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B22" s="68" t="s">
         <v>14</v>
       </c>
@@ -8114,7 +8118,7 @@
       <c r="J22" s="154"/>
       <c r="K22" s="111"/>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B23" s="68" t="s">
         <v>15</v>
       </c>
@@ -8139,7 +8143,7 @@
       <c r="J23" s="154"/>
       <c r="K23" s="111"/>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B24" s="68" t="s">
         <v>16</v>
       </c>
@@ -8164,7 +8168,7 @@
       <c r="J24" s="154"/>
       <c r="K24" s="111"/>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25" s="68" t="s">
         <v>51</v>
       </c>
@@ -8189,7 +8193,7 @@
       <c r="J25" s="154"/>
       <c r="K25" s="111"/>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B26" s="68" t="s">
         <v>52</v>
       </c>
@@ -8215,7 +8219,7 @@
       <c r="K26" s="111"/>
       <c r="L26" s="85"/>
     </row>
-    <row r="27" spans="2:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B27" s="68" t="s">
         <v>17</v>
       </c>
@@ -8241,7 +8245,7 @@
       <c r="K27" s="111"/>
       <c r="L27" s="72"/>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B28" s="56" t="s">
         <v>18</v>
       </c>
@@ -8257,7 +8261,7 @@
       <c r="J28" s="155"/>
       <c r="K28" s="110"/>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B29" s="68" t="s">
         <v>19</v>
       </c>
@@ -8282,7 +8286,7 @@
       <c r="J29" s="154"/>
       <c r="K29" s="111"/>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B30" s="68" t="s">
         <v>20</v>
       </c>
@@ -8307,7 +8311,7 @@
       <c r="J30" s="154"/>
       <c r="K30" s="111"/>
     </row>
-    <row r="31" spans="2:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B31" s="68" t="s">
         <v>21</v>
       </c>
@@ -8332,7 +8336,7 @@
       <c r="J31" s="154"/>
       <c r="K31" s="111"/>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B32" s="68" t="s">
         <v>22</v>
       </c>
@@ -8357,7 +8361,7 @@
       <c r="J32" s="154"/>
       <c r="K32" s="111"/>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B33" s="68" t="s">
         <v>23</v>
       </c>
@@ -8382,7 +8386,7 @@
       <c r="J33" s="154"/>
       <c r="K33" s="111"/>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B34" s="68" t="s">
         <v>24</v>
       </c>
@@ -8407,7 +8411,7 @@
       <c r="J34" s="154"/>
       <c r="K34" s="111"/>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B35" s="56" t="s">
         <v>25</v>
       </c>
@@ -8423,7 +8427,7 @@
       <c r="J35" s="155"/>
       <c r="K35" s="110"/>
     </row>
-    <row r="36" spans="2:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B36" s="68" t="s">
         <v>26</v>
       </c>
@@ -8451,7 +8455,7 @@
       <c r="J36" s="147"/>
       <c r="K36" s="111"/>
     </row>
-    <row r="37" spans="2:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B37" s="68" t="s">
         <v>55</v>
       </c>
@@ -8476,7 +8480,7 @@
       <c r="J37" s="154"/>
       <c r="K37" s="111"/>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B38" s="68" t="s">
         <v>56</v>
       </c>
@@ -8504,7 +8508,7 @@
       <c r="J38" s="147"/>
       <c r="K38" s="111"/>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B39" s="68" t="s">
         <v>27</v>
       </c>
@@ -8526,7 +8530,7 @@
       <c r="K39" s="111"/>
       <c r="M39" s="38"/>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B40" s="68" t="s">
         <v>28</v>
       </c>
@@ -8552,7 +8556,7 @@
       <c r="K40" s="111"/>
       <c r="M40" s="38"/>
     </row>
-    <row r="41" spans="2:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B41" s="68" t="s">
         <v>57</v>
       </c>
@@ -8580,7 +8584,7 @@
       <c r="J41" s="147"/>
       <c r="K41" s="111"/>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B42" s="68" t="s">
         <v>58</v>
       </c>
@@ -8605,7 +8609,7 @@
       <c r="J42" s="156"/>
       <c r="K42" s="113"/>
     </row>
-    <row r="43" spans="2:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B43" s="68" t="s">
         <v>29</v>
       </c>
@@ -8630,7 +8634,7 @@
       <c r="J43" s="147"/>
       <c r="K43" s="111"/>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B44" s="68" t="s">
         <v>30</v>
       </c>
@@ -8655,7 +8659,7 @@
       <c r="J44" s="154"/>
       <c r="K44" s="111"/>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B45" s="68" t="s">
         <v>31</v>
       </c>
@@ -8680,7 +8684,7 @@
       <c r="J45" s="154"/>
       <c r="K45" s="111"/>
     </row>
-    <row r="46" spans="2:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B46" s="68" t="s">
         <v>150</v>
       </c>
@@ -8708,7 +8712,7 @@
       <c r="J46" s="154"/>
       <c r="K46" s="111"/>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B47" s="56" t="s">
         <v>32</v>
       </c>
@@ -8724,7 +8728,7 @@
       <c r="J47" s="155"/>
       <c r="K47" s="110"/>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B48" s="68" t="s">
         <v>33</v>
       </c>
@@ -8749,7 +8753,7 @@
       <c r="J48" s="153"/>
       <c r="K48" s="116"/>
     </row>
-    <row r="49" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B49" s="68" t="s">
         <v>60</v>
       </c>
@@ -8777,7 +8781,7 @@
       <c r="J49" s="153"/>
       <c r="K49" s="116"/>
     </row>
-    <row r="50" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B50" s="68" t="s">
         <v>34</v>
       </c>
@@ -8802,7 +8806,7 @@
       <c r="J50" s="154"/>
       <c r="K50" s="116"/>
     </row>
-    <row r="51" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B51" s="68" t="s">
         <v>61</v>
       </c>
@@ -8827,7 +8831,7 @@
       <c r="J51" s="154"/>
       <c r="K51" s="111"/>
     </row>
-    <row r="52" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B52" s="68" t="s">
         <v>35</v>
       </c>
@@ -8852,7 +8856,7 @@
       <c r="J52" s="154"/>
       <c r="K52" s="111"/>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B53" s="68" t="s">
         <v>225</v>
       </c>
@@ -8880,7 +8884,7 @@
       <c r="J53" s="154"/>
       <c r="K53" s="111"/>
     </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B54" s="56" t="s">
         <v>36</v>
       </c>
@@ -8896,7 +8900,7 @@
       <c r="J54" s="155"/>
       <c r="K54" s="110"/>
     </row>
-    <row r="55" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B55" s="68" t="s">
         <v>62</v>
       </c>
@@ -8921,7 +8925,7 @@
       <c r="J55" s="154"/>
       <c r="K55" s="111"/>
     </row>
-    <row r="56" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B56" s="68" t="s">
         <v>63</v>
       </c>
@@ -8946,7 +8950,7 @@
       <c r="J56" s="154"/>
       <c r="K56" s="111"/>
     </row>
-    <row r="57" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B57" s="68" t="s">
         <v>64</v>
       </c>
@@ -8971,7 +8975,7 @@
       <c r="J57" s="154"/>
       <c r="K57" s="111"/>
     </row>
-    <row r="58" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B58" s="68" t="s">
         <v>65</v>
       </c>
@@ -8999,7 +9003,7 @@
       <c r="J58" s="154"/>
       <c r="K58" s="111"/>
     </row>
-    <row r="59" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B59" s="68" t="s">
         <v>66</v>
       </c>
@@ -9024,7 +9028,7 @@
       <c r="J59" s="154"/>
       <c r="K59" s="111"/>
     </row>
-    <row r="60" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B60" s="68" t="s">
         <v>67</v>
       </c>
@@ -9049,7 +9053,7 @@
       <c r="J60" s="154"/>
       <c r="K60" s="111"/>
     </row>
-    <row r="61" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B61" s="68" t="s">
         <v>224</v>
       </c>
@@ -9074,7 +9078,7 @@
       <c r="J61" s="154"/>
       <c r="K61" s="111"/>
     </row>
-    <row r="62" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B62" s="68" t="s">
         <v>223</v>
       </c>
@@ -9099,7 +9103,7 @@
       <c r="J62" s="154"/>
       <c r="K62" s="111"/>
     </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B63" s="56" t="s">
         <v>37</v>
       </c>
@@ -9115,7 +9119,7 @@
       <c r="J63" s="155"/>
       <c r="K63" s="110"/>
     </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B64" s="68" t="s">
         <v>68</v>
       </c>
@@ -9140,7 +9144,7 @@
       <c r="J64" s="154"/>
       <c r="K64" s="111"/>
     </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B65" s="68" t="s">
         <v>38</v>
       </c>
@@ -9165,7 +9169,7 @@
       <c r="J65" s="154"/>
       <c r="K65" s="111"/>
     </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B66" s="68" t="s">
         <v>69</v>
       </c>
@@ -9190,7 +9194,7 @@
       <c r="J66" s="154"/>
       <c r="K66" s="111"/>
     </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B67" s="68" t="s">
         <v>70</v>
       </c>
@@ -9215,7 +9219,7 @@
       <c r="J67" s="154"/>
       <c r="K67" s="111"/>
     </row>
-    <row r="68" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B68" s="68" t="s">
         <v>71</v>
       </c>
@@ -9240,7 +9244,7 @@
       <c r="J68" s="154"/>
       <c r="K68" s="111"/>
     </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B69" s="68" t="s">
         <v>39</v>
       </c>
@@ -9265,7 +9269,7 @@
       <c r="J69" s="154"/>
       <c r="K69" s="111"/>
     </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B70" s="68" t="s">
         <v>40</v>
       </c>
@@ -9290,7 +9294,7 @@
       <c r="J70" s="154"/>
       <c r="K70" s="111"/>
     </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B71" s="68" t="s">
         <v>41</v>
       </c>
@@ -9315,7 +9319,7 @@
       <c r="J71" s="154"/>
       <c r="K71" s="111"/>
     </row>
-    <row r="72" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B72" s="68" t="s">
         <v>152</v>
       </c>
@@ -9340,7 +9344,7 @@
       <c r="J72" s="154"/>
       <c r="K72" s="111"/>
     </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B73" s="59"/>
       <c r="C73" s="135"/>
       <c r="D73" s="97"/>
@@ -9352,7 +9356,7 @@
       <c r="J73" s="165"/>
       <c r="K73" s="118"/>
     </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B74" s="60"/>
       <c r="C74" s="60"/>
       <c r="D74" s="98"/>
@@ -9364,7 +9368,7 @@
       <c r="J74" s="151"/>
       <c r="K74" s="98"/>
     </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B75" s="60"/>
       <c r="C75" s="60"/>
       <c r="D75" s="98"/>
@@ -9376,7 +9380,7 @@
       <c r="J75" s="151"/>
       <c r="K75" s="98"/>
     </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B76" s="60"/>
       <c r="C76" s="60"/>
       <c r="D76" s="98"/>
@@ -9388,7 +9392,7 @@
       <c r="J76" s="151"/>
       <c r="K76" s="98"/>
     </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B77" s="61" t="s">
         <v>77</v>
       </c>
@@ -9402,7 +9406,7 @@
       <c r="J77" s="151"/>
       <c r="K77" s="98"/>
     </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B78" s="62" t="s">
         <v>78</v>
       </c>
@@ -9418,7 +9422,7 @@
       <c r="J78" s="151"/>
       <c r="K78" s="98"/>
     </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B79" s="63" t="s">
         <v>109</v>
       </c>
@@ -9434,7 +9438,7 @@
       <c r="J79" s="151"/>
       <c r="K79" s="98"/>
     </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B80" s="63" t="s">
         <v>110</v>
       </c>
@@ -9450,7 +9454,7 @@
       <c r="J80" s="151"/>
       <c r="K80" s="98"/>
     </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B81" s="63" t="s">
         <v>81</v>
       </c>
@@ -9466,7 +9470,7 @@
       <c r="J81" s="151"/>
       <c r="K81" s="98"/>
     </row>
-    <row r="82" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B82" s="69"/>
       <c r="C82" s="69"/>
       <c r="D82" s="99"/>
@@ -9478,7 +9482,7 @@
       <c r="J82" s="152"/>
       <c r="K82" s="99"/>
     </row>
-    <row r="83" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B83" s="69"/>
       <c r="C83" s="69"/>
       <c r="D83" s="99"/>
@@ -9490,7 +9494,7 @@
       <c r="J83" s="152"/>
       <c r="K83" s="99"/>
     </row>
-    <row r="84" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B84" s="69"/>
       <c r="C84" s="69"/>
       <c r="D84" s="99"/>
@@ -9502,7 +9506,7 @@
       <c r="J84" s="152"/>
       <c r="K84" s="99"/>
     </row>
-    <row r="85" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B85" s="69"/>
       <c r="C85" s="69"/>
       <c r="D85" s="99"/>
@@ -9534,15 +9538,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="0x05">
+    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="0x05">
       <formula>NOT(ISERROR(SEARCH("0x05",I6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G74:G1048576 I74:K1048576" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G74:G1048576 I74:K1048576">
       <formula1>"Yes,No,N/A"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G29:G34 G36:G46 G48:G53 G64:G72 G5:G14 G55:G62 G16:G27" xr:uid="{00000000-0002-0000-0400-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G29:G34 G36:G46 G48:G53 G64:G72 G5:G14 G55:G62 G16:G27">
       <formula1>"Pass,Fail,N/A"</formula1>
     </dataValidation>
   </dataValidations>
@@ -9552,7 +9556,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="B1:H32"/>
   <sheetViews>
@@ -9560,19 +9564,19 @@
       <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.83203125" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" style="54" customWidth="1"/>
-    <col min="3" max="3" width="17.58203125" style="54" customWidth="1"/>
-    <col min="4" max="4" width="93.33203125" style="100" customWidth="1"/>
+    <col min="1" max="1" width="1.796875" customWidth="1"/>
+    <col min="2" max="2" width="7.296875" style="54" customWidth="1"/>
+    <col min="3" max="3" width="17.59765625" style="54" customWidth="1"/>
+    <col min="4" max="4" width="93.296875" style="100" customWidth="1"/>
     <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="61.83203125" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" style="100" customWidth="1"/>
+    <col min="6" max="6" width="5.796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="61.796875" customWidth="1"/>
+    <col min="8" max="8" width="30.69921875" style="100" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="53" t="s">
         <v>130</v>
       </c>
@@ -9580,11 +9584,11 @@
       <c r="G1" s="152"/>
       <c r="H1" s="99"/>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="G2" s="152"/>
       <c r="H2" s="99"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="55" t="s">
         <v>0</v>
       </c>
@@ -9607,7 +9611,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="56"/>
       <c r="C4" s="132"/>
       <c r="D4" s="96" t="s">
@@ -9618,7 +9622,7 @@
       <c r="G4" s="159"/>
       <c r="H4" s="110"/>
     </row>
-    <row r="5" spans="2:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="70" t="s">
         <v>233</v>
       </c>
@@ -9640,7 +9644,7 @@
       </c>
       <c r="H5" s="111"/>
     </row>
-    <row r="6" spans="2:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B6" s="70" t="s">
         <v>234</v>
       </c>
@@ -9662,7 +9666,7 @@
       </c>
       <c r="H6" s="111"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="70" t="s">
         <v>235</v>
       </c>
@@ -9684,7 +9688,7 @@
       </c>
       <c r="H7" s="111"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="70" t="s">
         <v>236</v>
       </c>
@@ -9705,7 +9709,7 @@
       </c>
       <c r="H8" s="111"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="70" t="s">
         <v>237</v>
       </c>
@@ -9726,7 +9730,7 @@
       </c>
       <c r="H9" s="111"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="70" t="s">
         <v>238</v>
       </c>
@@ -9747,7 +9751,7 @@
       </c>
       <c r="H10" s="111"/>
     </row>
-    <row r="11" spans="2:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="70" t="s">
         <v>239</v>
       </c>
@@ -9768,7 +9772,7 @@
       </c>
       <c r="H11" s="111"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="70" t="s">
         <v>240</v>
       </c>
@@ -9789,7 +9793,7 @@
       </c>
       <c r="H12" s="111"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="70" t="s">
         <v>154</v>
       </c>
@@ -9810,7 +9814,7 @@
       </c>
       <c r="H13" s="111"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="56"/>
       <c r="C14" s="132"/>
       <c r="D14" s="96" t="s">
@@ -9821,7 +9825,7 @@
       <c r="G14" s="159"/>
       <c r="H14" s="110"/>
     </row>
-    <row r="15" spans="2:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="58" t="s">
         <v>73</v>
       </c>
@@ -9843,7 +9847,7 @@
       </c>
       <c r="H15" s="111"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="56"/>
       <c r="C16" s="132"/>
       <c r="D16" s="96" t="s">
@@ -9854,7 +9858,7 @@
       <c r="G16" s="159"/>
       <c r="H16" s="110"/>
     </row>
-    <row r="17" spans="2:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B17" s="70" t="s">
         <v>241</v>
       </c>
@@ -9876,7 +9880,7 @@
       </c>
       <c r="H17" s="111"/>
     </row>
-    <row r="18" spans="2:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B18" s="70" t="s">
         <v>242</v>
       </c>
@@ -9897,7 +9901,7 @@
       </c>
       <c r="H18" s="111"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="59"/>
       <c r="C19" s="135"/>
       <c r="D19" s="97"/>
@@ -9906,7 +9910,7 @@
       <c r="G19" s="164"/>
       <c r="H19" s="112"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="60"/>
       <c r="C20" s="60"/>
       <c r="D20" s="98"/>
@@ -9915,7 +9919,7 @@
       <c r="G20" s="151"/>
       <c r="H20" s="98"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="60"/>
       <c r="C21" s="60"/>
       <c r="D21" s="98"/>
@@ -9924,7 +9928,7 @@
       <c r="G21" s="151"/>
       <c r="H21" s="98"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="61" t="s">
         <v>77</v>
       </c>
@@ -9935,7 +9939,7 @@
       <c r="G22" s="151"/>
       <c r="H22" s="98"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="62" t="s">
         <v>78</v>
       </c>
@@ -9948,7 +9952,7 @@
       <c r="G23" s="151"/>
       <c r="H23" s="98"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="63" t="s">
         <v>109</v>
       </c>
@@ -9961,7 +9965,7 @@
       <c r="G24" s="151"/>
       <c r="H24" s="98"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" s="63" t="s">
         <v>110</v>
       </c>
@@ -9974,7 +9978,7 @@
       <c r="G25" s="151"/>
       <c r="H25" s="98"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" s="63" t="s">
         <v>81</v>
       </c>
@@ -9987,7 +9991,7 @@
       <c r="G26" s="151"/>
       <c r="H26" s="98"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B27" s="60"/>
       <c r="C27" s="60"/>
       <c r="D27" s="98"/>
@@ -9996,7 +10000,7 @@
       <c r="G27" s="152"/>
       <c r="H27" s="99"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B28" s="60"/>
       <c r="C28" s="60"/>
       <c r="D28" s="98"/>
@@ -10005,7 +10009,7 @@
       <c r="G28" s="152"/>
       <c r="H28" s="99"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B29" s="60"/>
       <c r="C29" s="60"/>
       <c r="D29" s="98"/>
@@ -10014,21 +10018,21 @@
       <c r="G29" s="152"/>
       <c r="H29" s="99"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B30" s="60"/>
       <c r="C30" s="60"/>
       <c r="D30" s="98"/>
       <c r="E30" s="32"/>
       <c r="F30" s="32"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B31" s="60"/>
       <c r="C31" s="60"/>
       <c r="D31" s="98"/>
       <c r="E31" s="32"/>
       <c r="F31" s="32"/>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B32" s="60"/>
       <c r="C32" s="60"/>
       <c r="D32" s="98"/>
@@ -10037,47 +10041,47 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G8">
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="0x05">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="0x05">
       <formula>NOT(ISERROR(SEARCH("0x05",G8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="0x05">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="0x05">
       <formula>NOT(ISERROR(SEARCH("0x05",G9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="0x05">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="0x05">
       <formula>NOT(ISERROR(SEARCH("0x05",G10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="0x05">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="0x05">
       <formula>NOT(ISERROR(SEARCH("0x05",G11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12">
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="0x05">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="0x05">
       <formula>NOT(ISERROR(SEARCH("0x05",G12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G13">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="0x05">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="0x05">
       <formula>NOT(ISERROR(SEARCH("0x05",G13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G17">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="0x05">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="0x05">
       <formula>NOT(ISERROR(SEARCH("0x05",G17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="0x05">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="0x05">
       <formula>NOT(ISERROR(SEARCH("0x05",G18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F15 F17:F18 F5:F13" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F15 F17:F18 F5:F13">
       <formula1>"Pass,Fail,N/A"</formula1>
     </dataValidation>
   </dataValidations>
@@ -10087,7 +10091,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:E25"/>
   <sheetViews>
@@ -10095,14 +10099,14 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="119.6640625" customWidth="1"/>
+    <col min="1" max="1" width="33.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="119.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="216" t="s">
         <v>74</v>
       </c>
@@ -10111,7 +10115,7 @@
       <c r="D1" s="33"/>
       <c r="E1" s="33"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="44" t="s">
         <v>137</v>
       </c>
@@ -10128,7 +10132,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="42" t="s">
         <v>75</v>
       </c>
@@ -10143,7 +10147,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="41" t="s">
         <v>76</v>
       </c>
@@ -10158,7 +10162,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="41" t="s">
         <v>119</v>
       </c>
@@ -10173,7 +10177,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="41" t="s">
         <v>120</v>
       </c>
@@ -10188,7 +10192,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="41" t="s">
         <v>76</v>
       </c>
@@ -10203,7 +10207,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="41" t="s">
         <v>120</v>
       </c>
@@ -10218,7 +10222,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="41" t="s">
         <v>76</v>
       </c>
@@ -10233,7 +10237,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="41" t="s">
         <v>76</v>
       </c>
@@ -10248,7 +10252,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="41" t="s">
         <v>76</v>
       </c>
@@ -10263,7 +10267,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="41" t="s">
         <v>76</v>
       </c>
@@ -10278,7 +10282,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="86" t="s">
         <v>258</v>
       </c>
@@ -10293,7 +10297,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="86" t="s">
         <v>259</v>
       </c>
@@ -10308,7 +10312,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="409" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="409.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="52" t="s">
         <v>222</v>
       </c>
@@ -10325,7 +10329,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="86" t="s">
         <v>258</v>
       </c>
@@ -10342,7 +10346,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="78" x14ac:dyDescent="0.3">
       <c r="A17" s="52" t="s">
         <v>222</v>
       </c>
@@ -10359,7 +10363,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A18" s="52" t="s">
         <v>222</v>
       </c>
@@ -10376,7 +10380,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A19" s="52" t="s">
         <v>222</v>
       </c>
@@ -10393,7 +10397,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A20" s="52" t="s">
         <v>258</v>
       </c>
@@ -10410,7 +10414,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="52" t="s">
         <v>258</v>
       </c>
@@ -10427,7 +10431,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A22" s="52" t="s">
         <v>258</v>
       </c>
@@ -10444,7 +10448,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="52" t="s">
         <v>258</v>
       </c>
@@ -10461,7 +10465,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="52" t="s">
         <v>258</v>
       </c>
@@ -10478,7 +10482,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A25" s="52" t="s">
         <v>258</v>
       </c>

</xml_diff>